<commit_message>
Additional Unit Testing, refactoring
Added unit tests for LineSegments. Refactored some classes and changed a namespace name.
</commit_message>
<xml_diff>
--- a/docs/Geometry Tests.xlsx
+++ b/docs/Geometry Tests.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\personal\MPT.Net\MPT\Geometry\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E19E8B8-4DE3-4384-9983-3BB1370B32AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA2EC4C-4861-48A6-B0F0-02BE7EE38286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24330" yWindow="2475" windowWidth="21600" windowHeight="11325" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extents" sheetId="4" r:id="rId1"/>
+    <sheet name="LineSegment" sheetId="12" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>X</t>
   </si>
@@ -39,6 +40,27 @@
     <t>Y</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
     <t>Rotation(Radians)</t>
   </si>
   <si>
@@ -48,6 +70,9 @@
     <t>ResultY</t>
   </si>
   <si>
+    <t>s</t>
+  </si>
+  <si>
     <t>Rotate</t>
   </si>
   <si>
@@ -61,13 +86,94 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Intercepts</t>
+  </si>
+  <si>
+    <t>x-intercept</t>
+  </si>
+  <si>
+    <t>y-intercept</t>
+  </si>
+  <si>
+    <t>i coordinate at x-intercept</t>
+  </si>
+  <si>
+    <t>j coordinate at x-intercept</t>
+  </si>
+  <si>
+    <t>i coordinate at y-intercept</t>
+  </si>
+  <si>
+    <t>j coordinate at y-intercept</t>
+  </si>
+  <si>
+    <t>- intercept</t>
+  </si>
+  <si>
+    <t>+ intercept</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>Intersections</t>
+  </si>
+  <si>
+    <t>x-intersection</t>
+  </si>
+  <si>
+    <t>y-intersection</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>segment 1</t>
+  </si>
+  <si>
+    <t>segment 2</t>
+  </si>
+  <si>
+    <t>Perpendicular</t>
+  </si>
+  <si>
+    <t>Parallel</t>
+  </si>
+  <si>
+    <t>xo</t>
+  </si>
+  <si>
+    <t>yo</t>
+  </si>
+  <si>
+    <t>deltaX</t>
+  </si>
+  <si>
+    <t>deltaY</t>
+  </si>
+  <si>
+    <t>Length, Xo, Yo</t>
+  </si>
+  <si>
+    <t>X, Y, PointByPathPosition</t>
+  </si>
+  <si>
+    <t>Normal Vector</t>
+  </si>
+  <si>
+    <t>Tangent Vector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,12 +190,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +216,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,18 +231,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,10 +567,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980E11E1-220A-447B-A3F4-1C24A01EFBA2}">
-  <dimension ref="A1:G14"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,32 +583,32 @@
     <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -560,8 +724,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="3" t="s">
-        <v>8</v>
+      <c r="E7" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="F7">
         <f>MIN(F3:F6)</f>
@@ -573,8 +737,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="3" t="s">
-        <v>9</v>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="F8">
         <f>MAX(F3:F7)</f>
@@ -706,8 +870,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="3" t="s">
-        <v>8</v>
+      <c r="E13" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="F13">
         <f>MIN(F9:F12)</f>
@@ -719,8 +883,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="3" t="s">
-        <v>9</v>
+      <c r="E14" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="F14">
         <f>MAX(F9:F13)</f>
@@ -729,10 +893,1663 @@
       <c r="G14">
         <f>MAX(G9:G13)</f>
         <v>9.4138179999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <f>31/5</f>
+        <v>6.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E420A0-5044-4817-9532-D9946D0E8FC8}">
+  <dimension ref="A1:R42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="e">
+        <f>(D3-B3)/(C3-A3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F3" t="e">
+        <f>A3-B3/E3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" t="e">
+        <f>B3-A3*E3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E10" si="0">(D4-B4)/(C4-A4)</f>
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F10" si="1">A4-B4/E4</f>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G10" si="2">B4-A4*E4</f>
+        <v>-3</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="str">
+        <f>"[TestCase("&amp;A4&amp;", "&amp;B4&amp;", "&amp;C4&amp;", "&amp;D4&amp;", "&amp;ROUND(F4,6)&amp;")]    // "&amp;H4</f>
+        <v>[TestCase(1, 0, 2, 3, 1)]    // i coordinate at x-intercept</v>
+      </c>
+      <c r="K4" t="str">
+        <f>"[TestCase("&amp;A4&amp;", "&amp;B4&amp;", "&amp;C4&amp;", "&amp;D4&amp;", "&amp;ROUND(G4,6)&amp;")]    // "&amp;H4</f>
+        <v>[TestCase(1, 0, 2, 3, -3)]    // i coordinate at x-intercept</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>-4</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" ref="J5:J9" si="3">"[TestCase("&amp;A5&amp;", "&amp;B5&amp;", "&amp;C5&amp;", "&amp;D5&amp;", "&amp;ROUND(F5,6)&amp;")]    // "&amp;H5</f>
+        <v>[TestCase(1, 2, -4, 0, -4)]    // j coordinate at x-intercept</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" ref="K5:K9" si="4">"[TestCase("&amp;A5&amp;", "&amp;B5&amp;", "&amp;C5&amp;", "&amp;D5&amp;", "&amp;ROUND(G5,6)&amp;")]    // "&amp;H5</f>
+        <v>[TestCase(1, 2, -4, 0, 1.6)]    // j coordinate at x-intercept</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="3"/>
+        <v>[TestCase(0, 1, 2, 3, -1)]    // i coordinate at y-intercept</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>[TestCase(0, 1, 2, 3, 1)]    // i coordinate at y-intercept</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>-4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
+        <v>[TestCase(1, 2, 0, -4, 0.666667)]    // j coordinate at y-intercept</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>[TestCase(1, 2, 0, -4, -4)]    // j coordinate at y-intercept</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
+        <v>[TestCase(1, 2, 3, 4, -1)]    // + intercept</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>[TestCase(1, 2, 3, 4, 1)]    // + intercept</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>-1</v>
+      </c>
+      <c r="B9">
+        <v>-2</v>
+      </c>
+      <c r="C9">
+        <v>-3</v>
+      </c>
+      <c r="D9">
+        <v>-4</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
+        <v>[TestCase(-1, -2, -3, -4, 1)]    // - intercept</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>[TestCase(-1, -2, -3, -4, -1)]    // - intercept</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1.5</v>
+      </c>
+      <c r="B10">
+        <v>2.75</v>
+      </c>
+      <c r="C10">
+        <v>3.75</v>
+      </c>
+      <c r="D10">
+        <v>4.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>-2.0357142857142856</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>1.5833333333333333</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" ref="J10" si="5">"[TestCase("&amp;A10&amp;", "&amp;B10&amp;", "&amp;C10&amp;", "&amp;D10&amp;", "&amp;ROUND(F10,6)&amp;")]    // "&amp;H10</f>
+        <v>[TestCase(1.5, 2.75, 3.75, 4.5, -2.035714)]    // decimal</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" ref="K10" si="6">"[TestCase("&amp;A10&amp;", "&amp;B10&amp;", "&amp;C10&amp;", "&amp;D10&amp;", "&amp;ROUND(G10,6)&amp;")]    // "&amp;H10</f>
+        <v>[TestCase(1.5, 2.75, 3.75, 4.5, 1.583333)]    // decimal</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="16"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>0</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" t="e">
+        <f>(D15-B15)/(C15-A15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" t="e">
+        <f>A15-B15/E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" t="e">
+        <f>B15-A15*E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0</v>
+      </c>
+      <c r="I15" s="18">
+        <v>0</v>
+      </c>
+      <c r="J15" s="18">
+        <v>0</v>
+      </c>
+      <c r="K15" s="18">
+        <v>0</v>
+      </c>
+      <c r="L15" s="8" t="e">
+        <f>(K15-I15)/(J15-H15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="8" t="e">
+        <f>H15-I15/L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="10" t="e">
+        <f>I15-H15*L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" t="e">
+        <f>(G15-N15)/(L15-E15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" t="e">
+        <f>G15+E15*(G15-N15)/(L15-E15)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f>(D16-B16)/(C16-A16)</f>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F19" si="7">A16-B16/E16</f>
+        <v>-1</v>
+      </c>
+      <c r="G16">
+        <f>B16-A16*E16</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="17">
+        <v>1</v>
+      </c>
+      <c r="I16" s="18">
+        <v>3</v>
+      </c>
+      <c r="J16" s="18">
+        <v>3</v>
+      </c>
+      <c r="K16" s="18">
+        <v>5</v>
+      </c>
+      <c r="L16" s="8">
+        <f>(K16-I16)/(J16-H16)</f>
+        <v>1</v>
+      </c>
+      <c r="M16" s="8">
+        <f t="shared" ref="M16:M19" si="8">H16-I16/L16</f>
+        <v>-2</v>
+      </c>
+      <c r="N16" s="10">
+        <f>I16-H16*L16</f>
+        <v>2</v>
+      </c>
+      <c r="O16" t="e">
+        <f>(G16-N16)/(L16-E16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" t="e">
+        <f>G16+E16*(G16-N16)/(L16-E16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>-5</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <f>(D17-B17)/(C17-A17)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17">
+        <f>B17-A17*E17</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="I17" s="18">
+        <v>-2.4</v>
+      </c>
+      <c r="J17" s="18">
+        <v>3.3</v>
+      </c>
+      <c r="K17" s="18">
+        <v>6.6</v>
+      </c>
+      <c r="L17" s="8" t="e">
+        <f>(K17-I17)/(J17-H17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="18">
+        <v>3.3</v>
+      </c>
+      <c r="N17" s="10" t="e">
+        <f>I17-H17*L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="P17" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5">
+        <v>3</v>
+      </c>
+      <c r="D18" s="5">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <f>(D18-B18)/(C18-A18)</f>
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="G18">
+        <f>B18-A18*E18</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="I18" s="18">
+        <v>-2.4</v>
+      </c>
+      <c r="J18" s="18">
+        <v>-5.7</v>
+      </c>
+      <c r="K18" s="18">
+        <v>6.6</v>
+      </c>
+      <c r="L18" s="8">
+        <f>(K18-I18)/(J18-H18)</f>
+        <v>-1</v>
+      </c>
+      <c r="M18" s="8">
+        <f t="shared" si="8"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="N18" s="10">
+        <f>I18-H18*L18</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="O18">
+        <f>(G18-N18)/(L18-E18)</f>
+        <v>-5.0000000000000044E-2</v>
+      </c>
+      <c r="P18">
+        <f>G18+E18*(G18-N18)/(L18-E18)</f>
+        <v>0.95</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <f>(D19-B19)/(C19-A19)</f>
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="G19">
+        <f>B19-A19*E19</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="I19" s="18">
+        <v>-2.4</v>
+      </c>
+      <c r="J19" s="18">
+        <v>-1</v>
+      </c>
+      <c r="K19" s="18">
+        <v>6.6</v>
+      </c>
+      <c r="L19" s="8">
+        <f>(K19-I19)/(J19-H19)</f>
+        <v>-2.0930232558139537</v>
+      </c>
+      <c r="M19" s="8">
+        <f t="shared" si="8"/>
+        <v>2.1533333333333333</v>
+      </c>
+      <c r="N19" s="10">
+        <f>I19-H19*L19</f>
+        <v>4.506976744186046</v>
+      </c>
+      <c r="O19">
+        <f>(G19-N19)/(L19-E19)</f>
+        <v>1.1338345864661652</v>
+      </c>
+      <c r="P19">
+        <f>G19+E19*(G19-N19)/(L19-E19)</f>
+        <v>2.1338345864661652</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f>C24-A24</f>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f>D24-B24</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f>SQRT(E24^2+F24^2)</f>
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <f>0.5*(A24+C24)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I24">
+        <f>0.5*(B24+D24)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ref="E25:E28" si="9">C25-A25</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25:F28" si="10">D25-B25</f>
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25:G28" si="11">SQRT(E25^2+F25^2)</f>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H28" si="12">0.5*(A25+C25)</f>
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ref="I25:I28" si="13">0.5*(B25+D25)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5">
+        <v>2</v>
+      </c>
+      <c r="C26" s="5">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="11"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B27" s="5">
+        <v>-2</v>
+      </c>
+      <c r="C27" s="5">
+        <v>-3</v>
+      </c>
+      <c r="D27" s="5">
+        <v>-4</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="10"/>
+        <v>-2</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="11"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="12"/>
+        <v>-2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="13"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>-3</v>
+      </c>
+      <c r="D28" s="5">
+        <v>-4</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="10"/>
+        <v>-6</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="11"/>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="13"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O31" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="R31" s="12"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O32" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P32" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q32" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="R32" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f>(D33-B33)/(C33-A33)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" t="e">
+        <f>A33-B33/E33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G33">
+        <f>B33-A33*E33</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="11">
+        <f>A33+J33*(C33-A33)</f>
+        <v>1.25</v>
+      </c>
+      <c r="I33" s="11">
+        <f>B33+J33*(D33-B33)</f>
+        <v>1</v>
+      </c>
+      <c r="J33" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="K33" s="11">
+        <f>SQRT((H33-A33)^2+(I33-B33)^2)/SQRT((C33-A33)^2+(D33-B33)^2)</f>
+        <v>0.25</v>
+      </c>
+      <c r="L33">
+        <f>C33-A33</f>
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <f>D33-B33</f>
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <f>SQRT(L33^2+M33^2)</f>
+        <v>1</v>
+      </c>
+      <c r="O33" s="11">
+        <f>-M33/$N33</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="11">
+        <f>L33/$N33</f>
+        <v>1</v>
+      </c>
+      <c r="Q33" s="11">
+        <f>L33/$N33</f>
+        <v>1</v>
+      </c>
+      <c r="R33" s="11">
+        <f>M33/$N33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5">
+        <v>2</v>
+      </c>
+      <c r="E34" t="e">
+        <f t="shared" ref="E34:E41" si="14">(D34-B34)/(C34-A34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F34" t="e">
+        <f t="shared" ref="F34:F41" si="15">A34-B34/E34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G34" t="e">
+        <f t="shared" ref="G34:G41" si="16">B34-A34*E34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" s="11">
+        <f t="shared" ref="H34:H37" si="17">A34+J34*(C34-A34)</f>
+        <v>1</v>
+      </c>
+      <c r="I34" s="11">
+        <f t="shared" ref="I34:I37" si="18">B34+J34*(D34-B34)</f>
+        <v>1.25</v>
+      </c>
+      <c r="J34" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="K34" s="11">
+        <f>SQRT((H34-A34)^2+(I34-B34)^2)/SQRT((C34-A34)^2+(D34-B34)^2)</f>
+        <v>0.25</v>
+      </c>
+      <c r="L34">
+        <f t="shared" ref="L34:L41" si="19">C34-A34</f>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f t="shared" ref="M34:M41" si="20">D34-B34</f>
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ref="N34:N41" si="21">SQRT(L34^2+M34^2)</f>
+        <v>1</v>
+      </c>
+      <c r="O34" s="11">
+        <f t="shared" ref="O34:O41" si="22">-M34/$N34</f>
+        <v>-1</v>
+      </c>
+      <c r="P34" s="11">
+        <f t="shared" ref="P34:P41" si="23">L34/$N34</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="11">
+        <f t="shared" ref="Q34:Q41" si="24">L34/$N34</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="11">
+        <f t="shared" ref="R34:R41" si="25">M34/$N34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5">
+        <v>2</v>
+      </c>
+      <c r="C35" s="5">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="H35" s="11">
+        <f t="shared" si="17"/>
+        <v>1.5</v>
+      </c>
+      <c r="I35" s="11">
+        <f t="shared" si="18"/>
+        <v>2.5</v>
+      </c>
+      <c r="J35" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="K35" s="11">
+        <f>SQRT((H35-A35)^2+(I35-B35)^2)/SQRT((C35-A35)^2+(D35-B35)^2)</f>
+        <v>0.25</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="21"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="O35" s="20">
+        <f t="shared" si="22"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="P35" s="20">
+        <f t="shared" si="23"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="Q35" s="11">
+        <f t="shared" si="24"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="R35" s="11">
+        <f t="shared" si="25"/>
+        <v>0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B36" s="5">
+        <v>-2</v>
+      </c>
+      <c r="C36" s="5">
+        <v>-3</v>
+      </c>
+      <c r="D36" s="5">
+        <v>-4</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="H36" s="11">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
+      <c r="I36" s="11">
+        <f t="shared" si="18"/>
+        <v>-2.5</v>
+      </c>
+      <c r="J36" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="K36" s="11">
+        <f>SQRT((H36-A36)^2+(I36-B36)^2)/SQRT((C36-A36)^2+(D36-B36)^2)</f>
+        <v>0.25</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="19"/>
+        <v>-2</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="20"/>
+        <v>-2</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="21"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="O36" s="20">
+        <f t="shared" si="22"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="P36" s="20">
+        <f t="shared" si="23"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="Q36" s="20">
+        <f t="shared" si="24"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="R36" s="20">
+        <f t="shared" si="25"/>
+        <v>-0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>1</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2</v>
+      </c>
+      <c r="C37" s="5">
+        <v>-3</v>
+      </c>
+      <c r="D37" s="5">
+        <v>-4</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="14"/>
+        <v>1.5</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="15"/>
+        <v>-0.33333333333333326</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="H37" s="11">
+        <f t="shared" si="17"/>
+        <v>-0.19999999999999996</v>
+      </c>
+      <c r="I37" s="11">
+        <f t="shared" si="18"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="J37" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="K37" s="11">
+        <f>SQRT((H37-A37)^2+(I37-B37)^2)/SQRT((C37-A37)^2+(D37-B37)^2)</f>
+        <v>0.3</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="19"/>
+        <v>-4</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="20"/>
+        <v>-6</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="21"/>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="O37" s="20">
+        <f t="shared" si="22"/>
+        <v>0.83205029433784372</v>
+      </c>
+      <c r="P37" s="20">
+        <f t="shared" si="23"/>
+        <v>-0.55470019622522915</v>
+      </c>
+      <c r="Q37" s="20">
+        <f t="shared" si="24"/>
+        <v>-0.55470019622522915</v>
+      </c>
+      <c r="R37" s="20">
+        <f t="shared" si="25"/>
+        <v>-0.83205029433784372</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>3</v>
+      </c>
+      <c r="B38" s="5">
+        <v>4</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="H38" s="11">
+        <f t="shared" ref="H38:H41" si="26">A38+J38*(C38-A38)</f>
+        <v>2</v>
+      </c>
+      <c r="I38" s="11">
+        <f t="shared" ref="I38:I41" si="27">B38+J38*(D38-B38)</f>
+        <v>3</v>
+      </c>
+      <c r="J38" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="19"/>
+        <v>-2</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="20"/>
+        <v>-2</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="21"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="O38" s="20">
+        <f t="shared" si="22"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="P38" s="20">
+        <f t="shared" si="23"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="Q38" s="20">
+        <f t="shared" si="24"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="R38" s="20">
+        <f t="shared" si="25"/>
+        <v>-0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
+        <v>1</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5">
+        <v>3</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="F39" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="H39" s="11">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="I39" s="11">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="O39" s="20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="20">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q39" s="20">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="R39" s="20">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40" s="5">
+        <v>1</v>
+      </c>
+      <c r="B40" s="5">
+        <v>2</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1</v>
+      </c>
+      <c r="D40" s="5">
+        <v>4</v>
+      </c>
+      <c r="E40" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F40" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G40" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="11">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="I40" s="11">
+        <f t="shared" si="27"/>
+        <v>3</v>
+      </c>
+      <c r="J40" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="O40" s="20">
+        <f t="shared" si="22"/>
+        <v>-1</v>
+      </c>
+      <c r="P40" s="20">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="20">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="R40" s="20">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
+        <v>1</v>
+      </c>
+      <c r="B41" s="5">
+        <v>2</v>
+      </c>
+      <c r="C41" s="5">
+        <v>3</v>
+      </c>
+      <c r="D41" s="5">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="H41" s="11">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="I41" s="11">
+        <f>B41+J41*(D41-B41)</f>
+        <v>3</v>
+      </c>
+      <c r="J41" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="21"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="O41" s="20">
+        <f t="shared" si="22"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="P41" s="20">
+        <f t="shared" si="23"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="Q41" s="20">
+        <f t="shared" si="24"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="R41" s="20">
+        <f t="shared" si="25"/>
+        <v>0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="B42" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="C42" s="5">
+        <v>6.7</v>
+      </c>
+      <c r="D42" s="5">
+        <v>9.1</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ref="E42" si="28">(D42-B42)/(C42-A42)</f>
+        <v>1.0363636363636362</v>
+      </c>
+      <c r="F42">
+        <f t="shared" ref="F42" si="29">A42-B42/E42</f>
+        <v>-2.0807017543859656</v>
+      </c>
+      <c r="G42">
+        <f t="shared" ref="G42" si="30">B42-A42*E42</f>
+        <v>2.1563636363636363</v>
+      </c>
+      <c r="H42" s="11">
+        <f t="shared" ref="H42" si="31">A42+J42*(C42-A42)</f>
+        <v>2.8499999999999996</v>
+      </c>
+      <c r="I42" s="11">
+        <f t="shared" ref="I42" si="32">B42+J42*(D42-B42)</f>
+        <v>5.1099999999999994</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="L42">
+        <f t="shared" ref="L42" si="33">C42-A42</f>
+        <v>5.5</v>
+      </c>
+      <c r="M42">
+        <f t="shared" ref="M42" si="34">D42-B42</f>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="N42">
+        <f t="shared" ref="N42" si="35">SQRT(L42^2+M42^2)</f>
+        <v>7.9208585393251401</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H13:N13"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:R31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Basic Point Intersection Methods
Testing, refactoring, additional development for segments and determining whether a point lies on a point, on a path, or within a shape.
</commit_message>
<xml_diff>
--- a/docs/Geometry Tests.xlsx
+++ b/docs/Geometry Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\personal\MPT.Net\MPT\Geometry\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA2EC4C-4861-48A6-B0F0-02BE7EE38286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8565F5EE-CCAF-4F95-8369-FF46B2B36D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -254,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -266,6 +266,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,6 +288,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,7 +728,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F7">
@@ -737,7 +741,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F8">
@@ -870,7 +874,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F13">
@@ -883,7 +887,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F14">
@@ -909,10 +913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E420A0-5044-4817-9532-D9946D0E8FC8}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1249,24 +1253,24 @@
       </c>
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="14" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="16"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="18"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -1343,16 +1347,16 @@
         <f>B15-A15*E15</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="17">
-        <v>0</v>
-      </c>
-      <c r="I15" s="18">
-        <v>0</v>
-      </c>
-      <c r="J15" s="18">
-        <v>0</v>
-      </c>
-      <c r="K15" s="18">
+      <c r="H15" s="19">
+        <v>0</v>
+      </c>
+      <c r="I15" s="20">
+        <v>0</v>
+      </c>
+      <c r="J15" s="20">
+        <v>0</v>
+      </c>
+      <c r="K15" s="20">
         <v>0</v>
       </c>
       <c r="L15" s="8" t="e">
@@ -1394,23 +1398,23 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F19" si="7">A16-B16/E16</f>
+        <f t="shared" ref="F16:F23" si="7">A16-B16/E16</f>
         <v>-1</v>
       </c>
       <c r="G16">
         <f>B16-A16*E16</f>
         <v>1</v>
       </c>
-      <c r="H16" s="17">
-        <v>1</v>
-      </c>
-      <c r="I16" s="18">
+      <c r="H16" s="19">
+        <v>1</v>
+      </c>
+      <c r="I16" s="20">
         <v>3</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="20">
         <v>3</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="20">
         <v>5</v>
       </c>
       <c r="L16" s="8">
@@ -1418,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="8">
-        <f t="shared" ref="M16:M19" si="8">H16-I16/L16</f>
+        <f t="shared" ref="M16:M23" si="8">H16-I16/L16</f>
         <v>-2</v>
       </c>
       <c r="N16" s="10">
@@ -1437,7 +1441,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>-5</v>
       </c>
@@ -1462,23 +1466,23 @@
         <f>B17-A17*E17</f>
         <v>1</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="19">
         <v>3.3</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="20">
         <v>-2.4</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="20">
         <v>3.3</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="20">
         <v>6.6</v>
       </c>
       <c r="L17" s="8" t="e">
         <f>(K17-I17)/(J17-H17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M17" s="18">
+      <c r="M17" s="20">
         <v>3.3</v>
       </c>
       <c r="N17" s="10" t="e">
@@ -1495,7 +1499,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>1</v>
       </c>
@@ -1520,16 +1524,16 @@
         <f>B18-A18*E18</f>
         <v>1</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="19">
         <v>3.3</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="20">
         <v>-2.4</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="20">
         <v>-5.7</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="20">
         <v>6.6</v>
       </c>
       <c r="L18" s="8">
@@ -1556,7 +1560,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>1</v>
       </c>
@@ -1581,16 +1585,16 @@
         <f>B19-A19*E19</f>
         <v>1</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H19" s="19">
         <v>3.3</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="20">
         <v>-2.4</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="20">
         <v>-1</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="20">
         <v>6.6</v>
       </c>
       <c r="L19" s="8">
@@ -1614,689 +1618,550 @@
         <v>2.1338345864661652</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>-5</v>
+      </c>
+      <c r="B20" s="5">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5">
+        <v>-3</v>
+      </c>
+      <c r="D20" s="5">
+        <v>-2</v>
+      </c>
+      <c r="E20">
+        <f>(D20-B20)/(C20-A20)</f>
+        <v>-4</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>-3.5</v>
+      </c>
+      <c r="G20">
+        <f>B20-A20*E20</f>
+        <v>-14</v>
+      </c>
+      <c r="H20" s="23">
+        <v>1</v>
+      </c>
+      <c r="I20" s="24">
+        <v>5</v>
+      </c>
+      <c r="J20" s="24">
+        <v>-7</v>
+      </c>
+      <c r="K20" s="24">
+        <v>3</v>
+      </c>
+      <c r="L20" s="11">
+        <f>(K20-I20)/(J20-H20)</f>
+        <v>0.25</v>
+      </c>
+      <c r="M20" s="11">
+        <f t="shared" si="8"/>
+        <v>-19</v>
+      </c>
+      <c r="N20" s="12">
+        <f>I20-H20*L20</f>
+        <v>4.75</v>
+      </c>
+      <c r="O20">
+        <f>(G20-N20)/(L20-E20)</f>
+        <v>-4.4117647058823533</v>
+      </c>
+      <c r="P20">
+        <f>G20+E20*(G20-N20)/(L20-E20)</f>
+        <v>3.647058823529413</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>-5</v>
+      </c>
+      <c r="B21" s="5">
+        <v>2</v>
+      </c>
+      <c r="C21" s="5">
+        <v>-5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>8</v>
+      </c>
+      <c r="E21" t="e">
+        <f>(D21-B21)/(C21-A21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F21" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" t="e">
+        <f>B21-A21*E21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="24">
+        <v>-5</v>
+      </c>
+      <c r="I21" s="24">
+        <v>6</v>
+      </c>
+      <c r="J21" s="24">
+        <v>5</v>
+      </c>
+      <c r="K21" s="24">
+        <v>6</v>
+      </c>
+      <c r="L21" s="11">
+        <f>(K21-I21)/(J21-H21)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="11" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" s="12">
+        <f>I21-H21*L21</f>
+        <v>6</v>
+      </c>
+      <c r="O21" t="e">
+        <f>(G21-N21)/(L21-E21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" t="e">
+        <f>G21+E21*(G21-N21)/(L21-E21)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>-5</v>
+      </c>
+      <c r="B22" s="5">
+        <v>8</v>
+      </c>
+      <c r="C22" s="5">
+        <v>-5</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
+      </c>
+      <c r="E22" t="e">
+        <f>(D22-B22)/(C22-A22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" s="11" t="e">
+        <f>B22-A22*E22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="24">
+        <v>-5</v>
+      </c>
+      <c r="I22" s="24">
+        <v>6</v>
+      </c>
+      <c r="J22" s="24">
+        <v>5</v>
+      </c>
+      <c r="K22" s="24">
+        <v>6</v>
+      </c>
+      <c r="L22" s="11">
+        <f>(K22-I22)/(J22-H22)</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="11" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N22" s="12">
+        <f>I22-H22*L22</f>
+        <v>6</v>
+      </c>
+      <c r="O22" t="e">
+        <f>(G22-N22)/(L22-E22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P22" t="e">
+        <f>G22+E22*(G22-N22)/(L22-E22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>-5</v>
+      </c>
+      <c r="B23" s="5">
+        <v>6</v>
+      </c>
+      <c r="C23" s="5">
+        <v>-3</v>
+      </c>
+      <c r="D23" s="5">
+        <v>-2</v>
+      </c>
+      <c r="E23">
+        <f>(D23-B23)/(C23-A23)</f>
+        <v>-4</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="7"/>
+        <v>-3.5</v>
+      </c>
+      <c r="G23" s="11">
+        <f>B23-A23*E23</f>
+        <v>-14</v>
+      </c>
+      <c r="H23" s="24">
+        <v>5.2</v>
+      </c>
+      <c r="I23" s="24">
+        <v>6.1</v>
+      </c>
+      <c r="J23" s="24">
+        <v>7.7</v>
+      </c>
+      <c r="K23" s="24">
+        <v>-1.3</v>
+      </c>
+      <c r="L23" s="11">
+        <f>(K23-I23)/(J23-H23)</f>
+        <v>-2.96</v>
+      </c>
+      <c r="M23" s="11">
+        <f t="shared" si="8"/>
+        <v>7.2608108108108107</v>
+      </c>
+      <c r="N23" s="12">
+        <f>I23-H23*L23</f>
+        <v>21.491999999999997</v>
+      </c>
+      <c r="O23">
+        <f>(G23-N23)/(L23-E23)</f>
+        <v>-34.12692307692307</v>
+      </c>
+      <c r="P23">
+        <f>G23+E23*(G23-N23)/(L23-E23)</f>
+        <v>122.50769230769228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="28" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I29" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>1</v>
-      </c>
-      <c r="B24" s="5">
-        <v>1</v>
-      </c>
-      <c r="C24" s="5">
-        <v>2</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <f>C24-A24</f>
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <f>D24-B24</f>
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <f>SQRT(E24^2+F24^2)</f>
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <f>0.5*(A24+C24)</f>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f>C30-A30</f>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f>D30-B30</f>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f>SQRT(E30^2+F30^2)</f>
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <f>0.5*(A30+C30)</f>
         <v>1.5</v>
       </c>
-      <c r="I24">
-        <f>0.5*(B24+D24)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>1</v>
-      </c>
-      <c r="B25" s="5">
-        <v>1</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1</v>
-      </c>
-      <c r="D25" s="5">
-        <v>2</v>
-      </c>
-      <c r="E25">
-        <f t="shared" ref="E25:E28" si="9">C25-A25</f>
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <f t="shared" ref="F25:F28" si="10">D25-B25</f>
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <f t="shared" ref="G25:G28" si="11">SQRT(E25^2+F25^2)</f>
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <f t="shared" ref="H25:H28" si="12">0.5*(A25+C25)</f>
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <f t="shared" ref="I25:I28" si="13">0.5*(B25+D25)</f>
+      <c r="I30">
+        <f>0.5*(B30+D30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ref="E31:E34" si="9">C31-A31</f>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" ref="F31:F34" si="10">D31-B31</f>
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ref="G31:G34" si="11">SQRT(E31^2+F31^2)</f>
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ref="H31:H34" si="12">0.5*(A31+C31)</f>
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <f t="shared" ref="I31:I34" si="13">0.5*(B31+D31)</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>1</v>
-      </c>
-      <c r="B26" s="5">
-        <v>2</v>
-      </c>
-      <c r="C26" s="5">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5">
         <v>3</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D32" s="5">
         <v>4</v>
       </c>
-      <c r="E26">
+      <c r="E32">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="F26">
+      <c r="F32">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="G26">
+      <c r="G32">
         <f t="shared" si="11"/>
         <v>2.8284271247461903</v>
       </c>
-      <c r="H26">
+      <c r="H32">
         <f t="shared" si="12"/>
         <v>2</v>
       </c>
-      <c r="I26">
+      <c r="I32">
         <f t="shared" si="13"/>
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
         <v>-1</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B33" s="5">
         <v>-2</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C33" s="5">
         <v>-3</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D33" s="5">
         <v>-4</v>
       </c>
-      <c r="E27">
+      <c r="E33">
         <f t="shared" si="9"/>
         <v>-2</v>
       </c>
-      <c r="F27">
+      <c r="F33">
         <f t="shared" si="10"/>
         <v>-2</v>
       </c>
-      <c r="G27">
+      <c r="G33">
         <f t="shared" si="11"/>
         <v>2.8284271247461903</v>
       </c>
-      <c r="H27">
+      <c r="H33">
         <f t="shared" si="12"/>
         <v>-2</v>
       </c>
-      <c r="I27">
+      <c r="I33">
         <f t="shared" si="13"/>
         <v>-3</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <v>1</v>
-      </c>
-      <c r="B28" s="5">
-        <v>2</v>
-      </c>
-      <c r="C28" s="5">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="B34" s="5">
+        <v>2</v>
+      </c>
+      <c r="C34" s="5">
         <v>-3</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D34" s="5">
         <v>-4</v>
       </c>
-      <c r="E28">
+      <c r="E34">
         <f t="shared" si="9"/>
         <v>-4</v>
       </c>
-      <c r="F28">
+      <c r="F34">
         <f t="shared" si="10"/>
         <v>-6</v>
       </c>
-      <c r="G28">
+      <c r="G34">
         <f t="shared" si="11"/>
         <v>7.2111025509279782</v>
       </c>
-      <c r="H28">
+      <c r="H34">
         <f t="shared" si="12"/>
         <v>-1</v>
       </c>
-      <c r="I28">
+      <c r="I34">
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+    <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O31" s="12" t="s">
+    <row r="37" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O37" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12" t="s">
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="R31" s="12"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="R37" s="14"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F38" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="I32" s="19" t="s">
+      <c r="H38" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K38" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="L38" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M32" s="4" t="s">
+      <c r="M38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N32" s="4" t="s">
+      <c r="N38" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O32" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="P32" s="19" t="s">
+      <c r="O38" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="P38" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="Q32" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="R32" s="19" t="s">
+      <c r="Q38" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="R38" s="21" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
-        <v>1</v>
-      </c>
-      <c r="B33" s="5">
-        <v>1</v>
-      </c>
-      <c r="C33" s="5">
-        <v>2</v>
-      </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <f>(D33-B33)/(C33-A33)</f>
-        <v>0</v>
-      </c>
-      <c r="F33" t="e">
-        <f>A33-B33/E33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G33">
-        <f>B33-A33*E33</f>
-        <v>1</v>
-      </c>
-      <c r="H33" s="11">
-        <f>A33+J33*(C33-A33)</f>
-        <v>1.25</v>
-      </c>
-      <c r="I33" s="11">
-        <f>B33+J33*(D33-B33)</f>
-        <v>1</v>
-      </c>
-      <c r="J33" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="K33" s="11">
-        <f>SQRT((H33-A33)^2+(I33-B33)^2)/SQRT((C33-A33)^2+(D33-B33)^2)</f>
-        <v>0.25</v>
-      </c>
-      <c r="L33">
-        <f>C33-A33</f>
-        <v>1</v>
-      </c>
-      <c r="M33">
-        <f>D33-B33</f>
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <f>SQRT(L33^2+M33^2)</f>
-        <v>1</v>
-      </c>
-      <c r="O33" s="11">
-        <f>-M33/$N33</f>
-        <v>0</v>
-      </c>
-      <c r="P33" s="11">
-        <f>L33/$N33</f>
-        <v>1</v>
-      </c>
-      <c r="Q33" s="11">
-        <f>L33/$N33</f>
-        <v>1</v>
-      </c>
-      <c r="R33" s="11">
-        <f>M33/$N33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
-        <v>1</v>
-      </c>
-      <c r="B34" s="5">
-        <v>1</v>
-      </c>
-      <c r="C34" s="5">
-        <v>1</v>
-      </c>
-      <c r="D34" s="5">
-        <v>2</v>
-      </c>
-      <c r="E34" t="e">
-        <f t="shared" ref="E34:E41" si="14">(D34-B34)/(C34-A34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F34" t="e">
-        <f t="shared" ref="F34:F41" si="15">A34-B34/E34</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G34" t="e">
-        <f t="shared" ref="G34:G41" si="16">B34-A34*E34</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H34" s="11">
-        <f t="shared" ref="H34:H37" si="17">A34+J34*(C34-A34)</f>
-        <v>1</v>
-      </c>
-      <c r="I34" s="11">
-        <f t="shared" ref="I34:I37" si="18">B34+J34*(D34-B34)</f>
-        <v>1.25</v>
-      </c>
-      <c r="J34" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="K34" s="11">
-        <f>SQRT((H34-A34)^2+(I34-B34)^2)/SQRT((C34-A34)^2+(D34-B34)^2)</f>
-        <v>0.25</v>
-      </c>
-      <c r="L34">
-        <f t="shared" ref="L34:L41" si="19">C34-A34</f>
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <f t="shared" ref="M34:M41" si="20">D34-B34</f>
-        <v>1</v>
-      </c>
-      <c r="N34">
-        <f t="shared" ref="N34:N41" si="21">SQRT(L34^2+M34^2)</f>
-        <v>1</v>
-      </c>
-      <c r="O34" s="11">
-        <f t="shared" ref="O34:O41" si="22">-M34/$N34</f>
-        <v>-1</v>
-      </c>
-      <c r="P34" s="11">
-        <f t="shared" ref="P34:P41" si="23">L34/$N34</f>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="11">
-        <f t="shared" ref="Q34:Q41" si="24">L34/$N34</f>
-        <v>0</v>
-      </c>
-      <c r="R34" s="11">
-        <f t="shared" ref="R34:R41" si="25">M34/$N34</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
-        <v>1</v>
-      </c>
-      <c r="B35" s="5">
-        <v>2</v>
-      </c>
-      <c r="C35" s="5">
-        <v>3</v>
-      </c>
-      <c r="D35" s="5">
-        <v>4</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="15"/>
-        <v>-1</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="H35" s="11">
-        <f t="shared" si="17"/>
-        <v>1.5</v>
-      </c>
-      <c r="I35" s="11">
-        <f t="shared" si="18"/>
-        <v>2.5</v>
-      </c>
-      <c r="J35" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="K35" s="11">
-        <f>SQRT((H35-A35)^2+(I35-B35)^2)/SQRT((C35-A35)^2+(D35-B35)^2)</f>
-        <v>0.25</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="19"/>
-        <v>2</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="20"/>
-        <v>2</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="21"/>
-        <v>2.8284271247461903</v>
-      </c>
-      <c r="O35" s="20">
-        <f t="shared" si="22"/>
-        <v>-0.70710678118654746</v>
-      </c>
-      <c r="P35" s="20">
-        <f t="shared" si="23"/>
-        <v>0.70710678118654746</v>
-      </c>
-      <c r="Q35" s="11">
-        <f t="shared" si="24"/>
-        <v>0.70710678118654746</v>
-      </c>
-      <c r="R35" s="11">
-        <f t="shared" si="25"/>
-        <v>0.70710678118654746</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
-        <v>-1</v>
-      </c>
-      <c r="B36" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C36" s="5">
-        <v>-3</v>
-      </c>
-      <c r="D36" s="5">
-        <v>-4</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="16"/>
-        <v>-1</v>
-      </c>
-      <c r="H36" s="11">
-        <f t="shared" si="17"/>
-        <v>-1.5</v>
-      </c>
-      <c r="I36" s="11">
-        <f t="shared" si="18"/>
-        <v>-2.5</v>
-      </c>
-      <c r="J36" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="K36" s="11">
-        <f>SQRT((H36-A36)^2+(I36-B36)^2)/SQRT((C36-A36)^2+(D36-B36)^2)</f>
-        <v>0.25</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="19"/>
-        <v>-2</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="20"/>
-        <v>-2</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="21"/>
-        <v>2.8284271247461903</v>
-      </c>
-      <c r="O36" s="20">
-        <f t="shared" si="22"/>
-        <v>0.70710678118654746</v>
-      </c>
-      <c r="P36" s="20">
-        <f t="shared" si="23"/>
-        <v>-0.70710678118654746</v>
-      </c>
-      <c r="Q36" s="20">
-        <f t="shared" si="24"/>
-        <v>-0.70710678118654746</v>
-      </c>
-      <c r="R36" s="20">
-        <f t="shared" si="25"/>
-        <v>-0.70710678118654746</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
-        <v>1</v>
-      </c>
-      <c r="B37" s="5">
-        <v>2</v>
-      </c>
-      <c r="C37" s="5">
-        <v>-3</v>
-      </c>
-      <c r="D37" s="5">
-        <v>-4</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="14"/>
-        <v>1.5</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="15"/>
-        <v>-0.33333333333333326</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="16"/>
-        <v>0.5</v>
-      </c>
-      <c r="H37" s="11">
-        <f t="shared" si="17"/>
-        <v>-0.19999999999999996</v>
-      </c>
-      <c r="I37" s="11">
-        <f t="shared" si="18"/>
-        <v>0.20000000000000018</v>
-      </c>
-      <c r="J37" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="K37" s="11">
-        <f>SQRT((H37-A37)^2+(I37-B37)^2)/SQRT((C37-A37)^2+(D37-B37)^2)</f>
-        <v>0.3</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="19"/>
-        <v>-4</v>
-      </c>
-      <c r="M37">
-        <f t="shared" si="20"/>
-        <v>-6</v>
-      </c>
-      <c r="N37">
-        <f t="shared" si="21"/>
-        <v>7.2111025509279782</v>
-      </c>
-      <c r="O37" s="20">
-        <f t="shared" si="22"/>
-        <v>0.83205029433784372</v>
-      </c>
-      <c r="P37" s="20">
-        <f t="shared" si="23"/>
-        <v>-0.55470019622522915</v>
-      </c>
-      <c r="Q37" s="20">
-        <f t="shared" si="24"/>
-        <v>-0.55470019622522915</v>
-      </c>
-      <c r="R37" s="20">
-        <f t="shared" si="25"/>
-        <v>-0.83205029433784372</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
-        <v>3</v>
-      </c>
-      <c r="B38" s="5">
-        <v>4</v>
-      </c>
-      <c r="C38" s="5">
-        <v>1</v>
-      </c>
-      <c r="D38" s="5">
-        <v>2</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="15"/>
-        <v>-1</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="H38" s="11">
-        <f t="shared" ref="H38:H41" si="26">A38+J38*(C38-A38)</f>
-        <v>2</v>
-      </c>
-      <c r="I38" s="11">
-        <f t="shared" ref="I38:I41" si="27">B38+J38*(D38-B38)</f>
-        <v>3</v>
-      </c>
-      <c r="J38" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="19"/>
-        <v>-2</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="20"/>
-        <v>-2</v>
-      </c>
-      <c r="N38">
-        <f t="shared" si="21"/>
-        <v>2.8284271247461903</v>
-      </c>
-      <c r="O38" s="20">
-        <f t="shared" si="22"/>
-        <v>0.70710678118654746</v>
-      </c>
-      <c r="P38" s="20">
-        <f t="shared" si="23"/>
-        <v>-0.70710678118654746</v>
-      </c>
-      <c r="Q38" s="20">
-        <f t="shared" si="24"/>
-        <v>-0.70710678118654746</v>
-      </c>
-      <c r="R38" s="20">
-        <f t="shared" si="25"/>
-        <v>-0.70710678118654746</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
@@ -2307,60 +2172,64 @@
         <v>1</v>
       </c>
       <c r="C39" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39" s="5">
         <v>1</v>
       </c>
       <c r="E39">
-        <f t="shared" si="14"/>
+        <f>(D39-B39)/(C39-A39)</f>
         <v>0</v>
       </c>
       <c r="F39" t="e">
-        <f t="shared" si="15"/>
+        <f>A39-B39/E39</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G39">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="H39" s="11">
-        <f t="shared" si="26"/>
-        <v>2</v>
-      </c>
-      <c r="I39" s="11">
-        <f t="shared" si="27"/>
+        <f>B39-A39*E39</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="13">
+        <f>A39+J39*(C39-A39)</f>
+        <v>1.25</v>
+      </c>
+      <c r="I39" s="13">
+        <f>B39+J39*(D39-B39)</f>
         <v>1</v>
       </c>
       <c r="J39" s="5">
-        <v>0.5</v>
+        <v>0.25</v>
+      </c>
+      <c r="K39" s="13">
+        <f>SQRT((H39-A39)^2+(I39-B39)^2)/SQRT((C39-A39)^2+(D39-B39)^2)</f>
+        <v>0.25</v>
       </c>
       <c r="L39">
-        <f t="shared" si="19"/>
-        <v>2</v>
+        <f>C39-A39</f>
+        <v>1</v>
       </c>
       <c r="M39">
-        <f t="shared" si="20"/>
+        <f>D39-B39</f>
         <v>0</v>
       </c>
       <c r="N39">
-        <f t="shared" si="21"/>
-        <v>2</v>
-      </c>
-      <c r="O39" s="20">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="P39" s="20">
-        <f t="shared" si="23"/>
-        <v>1</v>
-      </c>
-      <c r="Q39" s="20">
-        <f t="shared" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="R39" s="20">
-        <f t="shared" si="25"/>
+        <f>SQRT(L39^2+M39^2)</f>
+        <v>1</v>
+      </c>
+      <c r="O39" s="13">
+        <f>-M39/$N39</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="13">
+        <f>L39/$N39</f>
+        <v>1</v>
+      </c>
+      <c r="Q39" s="13">
+        <f>L39/$N39</f>
+        <v>1</v>
+      </c>
+      <c r="R39" s="13">
+        <f>M39/$N39</f>
         <v>0</v>
       </c>
     </row>
@@ -2369,63 +2238,67 @@
         <v>1</v>
       </c>
       <c r="B40" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" s="5">
         <v>1</v>
       </c>
       <c r="D40" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E40" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="E40:E47" si="14">(D40-B40)/(C40-A40)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F40" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="F40:F47" si="15">A40-B40/E40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G40" t="e">
-        <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H40" s="11">
-        <f t="shared" si="26"/>
-        <v>1</v>
-      </c>
-      <c r="I40" s="11">
-        <f t="shared" si="27"/>
-        <v>3</v>
+        <f t="shared" ref="G40:G47" si="16">B40-A40*E40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="13">
+        <f t="shared" ref="H40:H43" si="17">A40+J40*(C40-A40)</f>
+        <v>1</v>
+      </c>
+      <c r="I40" s="13">
+        <f t="shared" ref="I40:I43" si="18">B40+J40*(D40-B40)</f>
+        <v>1.25</v>
       </c>
       <c r="J40" s="5">
-        <v>0.5</v>
+        <v>0.25</v>
+      </c>
+      <c r="K40" s="13">
+        <f>SQRT((H40-A40)^2+(I40-B40)^2)/SQRT((C40-A40)^2+(D40-B40)^2)</f>
+        <v>0.25</v>
       </c>
       <c r="L40">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="L40:L47" si="19">C40-A40</f>
         <v>0</v>
       </c>
       <c r="M40">
-        <f t="shared" si="20"/>
-        <v>2</v>
+        <f t="shared" ref="M40:M47" si="20">D40-B40</f>
+        <v>1</v>
       </c>
       <c r="N40">
-        <f t="shared" si="21"/>
-        <v>2</v>
-      </c>
-      <c r="O40" s="20">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="N40:N47" si="21">SQRT(L40^2+M40^2)</f>
+        <v>1</v>
+      </c>
+      <c r="O40" s="13">
+        <f t="shared" ref="O40:O47" si="22">-M40/$N40</f>
         <v>-1</v>
       </c>
-      <c r="P40" s="20">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="Q40" s="20">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="R40" s="20">
-        <f t="shared" si="25"/>
+      <c r="P40" s="13">
+        <f t="shared" ref="P40:P47" si="23">L40/$N40</f>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="13">
+        <f t="shared" ref="Q40:Q47" si="24">L40/$N40</f>
+        <v>0</v>
+      </c>
+      <c r="R40" s="13">
+        <f t="shared" ref="R40:R47" si="25">M40/$N40</f>
         <v>1</v>
       </c>
     </row>
@@ -2454,16 +2327,20 @@
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="H41" s="11">
-        <f t="shared" si="26"/>
-        <v>2</v>
-      </c>
-      <c r="I41" s="11">
-        <f>B41+J41*(D41-B41)</f>
-        <v>3</v>
+      <c r="H41" s="13">
+        <f t="shared" si="17"/>
+        <v>1.5</v>
+      </c>
+      <c r="I41" s="13">
+        <f t="shared" si="18"/>
+        <v>2.5</v>
       </c>
       <c r="J41" s="5">
-        <v>0.5</v>
+        <v>0.25</v>
+      </c>
+      <c r="K41" s="13">
+        <f>SQRT((H41-A41)^2+(I41-B41)^2)/SQRT((C41-A41)^2+(D41-B41)^2)</f>
+        <v>0.25</v>
       </c>
       <c r="L41">
         <f t="shared" si="19"/>
@@ -2477,69 +2354,467 @@
         <f t="shared" si="21"/>
         <v>2.8284271247461903</v>
       </c>
-      <c r="O41" s="20">
+      <c r="O41" s="22">
         <f t="shared" si="22"/>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="P41" s="20">
+      <c r="P41" s="22">
         <f t="shared" si="23"/>
         <v>0.70710678118654746</v>
       </c>
-      <c r="Q41" s="20">
+      <c r="Q41" s="13">
         <f t="shared" si="24"/>
         <v>0.70710678118654746</v>
       </c>
-      <c r="R41" s="20">
+      <c r="R41" s="13">
         <f t="shared" si="25"/>
         <v>0.70710678118654746</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B42" s="5">
+        <v>-2</v>
+      </c>
+      <c r="C42" s="5">
+        <v>-3</v>
+      </c>
+      <c r="D42" s="5">
+        <v>-4</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="H42" s="13">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
+      <c r="I42" s="13">
+        <f t="shared" si="18"/>
+        <v>-2.5</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="K42" s="13">
+        <f>SQRT((H42-A42)^2+(I42-B42)^2)/SQRT((C42-A42)^2+(D42-B42)^2)</f>
+        <v>0.25</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="19"/>
+        <v>-2</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="20"/>
+        <v>-2</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="21"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="O42" s="22">
+        <f t="shared" si="22"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="P42" s="22">
+        <f t="shared" si="23"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="Q42" s="22">
+        <f t="shared" si="24"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="R42" s="22">
+        <f t="shared" si="25"/>
+        <v>-0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
+        <v>1</v>
+      </c>
+      <c r="B43" s="5">
+        <v>2</v>
+      </c>
+      <c r="C43" s="5">
+        <v>-3</v>
+      </c>
+      <c r="D43" s="5">
+        <v>-4</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="14"/>
+        <v>1.5</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="15"/>
+        <v>-0.33333333333333326</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="H43" s="13">
+        <f t="shared" si="17"/>
+        <v>-0.19999999999999996</v>
+      </c>
+      <c r="I43" s="13">
+        <f t="shared" si="18"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="K43" s="13">
+        <f>SQRT((H43-A43)^2+(I43-B43)^2)/SQRT((C43-A43)^2+(D43-B43)^2)</f>
+        <v>0.3</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="19"/>
+        <v>-4</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="20"/>
+        <v>-6</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="21"/>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="O43" s="22">
+        <f t="shared" si="22"/>
+        <v>0.83205029433784372</v>
+      </c>
+      <c r="P43" s="22">
+        <f t="shared" si="23"/>
+        <v>-0.55470019622522915</v>
+      </c>
+      <c r="Q43" s="22">
+        <f t="shared" si="24"/>
+        <v>-0.55470019622522915</v>
+      </c>
+      <c r="R43" s="22">
+        <f t="shared" si="25"/>
+        <v>-0.83205029433784372</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <v>3</v>
+      </c>
+      <c r="B44" s="5">
+        <v>4</v>
+      </c>
+      <c r="C44" s="5">
+        <v>1</v>
+      </c>
+      <c r="D44" s="5">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="H44" s="13">
+        <f t="shared" ref="H44:H47" si="26">A44+J44*(C44-A44)</f>
+        <v>2</v>
+      </c>
+      <c r="I44" s="13">
+        <f t="shared" ref="I44:I46" si="27">B44+J44*(D44-B44)</f>
+        <v>3</v>
+      </c>
+      <c r="J44" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="19"/>
+        <v>-2</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="20"/>
+        <v>-2</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="21"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="O44" s="22">
+        <f t="shared" si="22"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="P44" s="22">
+        <f t="shared" si="23"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="Q44" s="22">
+        <f t="shared" si="24"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="R44" s="22">
+        <f t="shared" si="25"/>
+        <v>-0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="5">
+        <v>1</v>
+      </c>
+      <c r="B45" s="5">
+        <v>1</v>
+      </c>
+      <c r="C45" s="5">
+        <v>3</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="F45" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="H45" s="13">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="I45" s="13">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="J45" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="O45" s="22">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="P45" s="22">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="Q45" s="22">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="R45" s="22">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" s="5">
+        <v>1</v>
+      </c>
+      <c r="B46" s="5">
+        <v>2</v>
+      </c>
+      <c r="C46" s="5">
+        <v>1</v>
+      </c>
+      <c r="D46" s="5">
+        <v>4</v>
+      </c>
+      <c r="E46" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F46" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H46" s="13">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="I46" s="13">
+        <f t="shared" si="27"/>
+        <v>3</v>
+      </c>
+      <c r="J46" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="O46" s="22">
+        <f t="shared" si="22"/>
+        <v>-1</v>
+      </c>
+      <c r="P46" s="22">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="22">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="R46" s="22">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
+        <v>1</v>
+      </c>
+      <c r="B47" s="5">
+        <v>2</v>
+      </c>
+      <c r="C47" s="5">
+        <v>3</v>
+      </c>
+      <c r="D47" s="5">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="H47" s="13">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="I47" s="13">
+        <f>B47+J47*(D47-B47)</f>
+        <v>3</v>
+      </c>
+      <c r="J47" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="21"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="O47" s="22">
+        <f t="shared" si="22"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="P47" s="22">
+        <f t="shared" si="23"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="Q47" s="22">
+        <f t="shared" si="24"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="R47" s="22">
+        <f t="shared" si="25"/>
+        <v>0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A48" s="5">
         <v>1.2</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B48" s="5">
         <v>3.4</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C48" s="5">
         <v>6.7</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D48" s="5">
         <v>9.1</v>
       </c>
-      <c r="E42">
-        <f t="shared" ref="E42" si="28">(D42-B42)/(C42-A42)</f>
+      <c r="E48">
+        <f t="shared" ref="E48" si="28">(D48-B48)/(C48-A48)</f>
         <v>1.0363636363636362</v>
       </c>
-      <c r="F42">
-        <f t="shared" ref="F42" si="29">A42-B42/E42</f>
+      <c r="F48">
+        <f t="shared" ref="F48" si="29">A48-B48/E48</f>
         <v>-2.0807017543859656</v>
       </c>
-      <c r="G42">
-        <f t="shared" ref="G42" si="30">B42-A42*E42</f>
+      <c r="G48">
+        <f t="shared" ref="G48" si="30">B48-A48*E48</f>
         <v>2.1563636363636363</v>
       </c>
-      <c r="H42" s="11">
-        <f t="shared" ref="H42" si="31">A42+J42*(C42-A42)</f>
+      <c r="H48" s="13">
+        <f t="shared" ref="H48" si="31">A48+J48*(C48-A48)</f>
         <v>2.8499999999999996</v>
       </c>
-      <c r="I42" s="11">
-        <f t="shared" ref="I42" si="32">B42+J42*(D42-B42)</f>
+      <c r="I48" s="13">
+        <f t="shared" ref="I48" si="32">B48+J48*(D48-B48)</f>
         <v>5.1099999999999994</v>
       </c>
-      <c r="J42" s="5">
+      <c r="J48" s="5">
         <v>0.3</v>
       </c>
-      <c r="L42">
-        <f t="shared" ref="L42" si="33">C42-A42</f>
+      <c r="L48">
+        <f t="shared" ref="L48" si="33">C48-A48</f>
         <v>5.5</v>
       </c>
-      <c r="M42">
-        <f t="shared" ref="M42" si="34">D42-B42</f>
+      <c r="M48">
+        <f t="shared" ref="M48" si="34">D48-B48</f>
         <v>5.6999999999999993</v>
       </c>
-      <c r="N42">
-        <f t="shared" ref="N42" si="35">SQRT(L42^2+M42^2)</f>
+      <c r="N48">
+        <f t="shared" ref="N48" si="35">SQRT(L48^2+M48^2)</f>
         <v>7.9208585393251401</v>
       </c>
     </row>
@@ -2547,8 +2822,8 @@
   <mergeCells count="4">
     <mergeCell ref="H13:N13"/>
     <mergeCell ref="A13:G13"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="Q37:R37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fleshing out polyline and related objects.
Most work is done on Segments.
</commit_message>
<xml_diff>
--- a/docs/Geometry Tests.xlsx
+++ b/docs/Geometry Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\personal\MPT.Net\MPT\Geometry\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8565F5EE-CCAF-4F95-8369-FF46B2B36D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C003C7-0536-4E27-9BF4-98EA7147A9C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12048" yWindow="300" windowWidth="10764" windowHeight="11592" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extents" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
   <si>
     <t>X</t>
   </si>
@@ -164,6 +164,33 @@
   </si>
   <si>
     <t>Tangent Vector</t>
+  </si>
+  <si>
+    <t>RotateSegmentFromI</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Rotation</t>
+  </si>
+  <si>
+    <t>I'</t>
+  </si>
+  <si>
+    <t>J'</t>
+  </si>
+  <si>
+    <t>RotateSegmentFromJ</t>
+  </si>
+  <si>
+    <t>RotateSegmentFromPoint</t>
+  </si>
+  <si>
+    <t>Center of Rotation</t>
   </si>
 </sst>
 </file>
@@ -171,7 +198,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -254,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -269,12 +296,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -284,12 +314,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,7 +662,7 @@
         <v>2.5</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E11" si="0">PI()/4</f>
+        <f t="shared" ref="E3" si="0">PI()/4</f>
         <v>0.78539816339744828</v>
       </c>
       <c r="F3">
@@ -728,7 +759,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F7">
@@ -741,7 +772,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F8">
@@ -874,7 +905,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F13">
@@ -887,7 +918,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F14">
@@ -913,14 +944,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E420A0-5044-4817-9532-D9946D0E8FC8}">
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="F67" workbookViewId="0">
+      <selection activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.44140625" customWidth="1"/>
@@ -1253,24 +1285,24 @@
       </c>
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="16" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="18"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -1336,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="e">
-        <f>(D15-B15)/(C15-A15)</f>
+        <f t="shared" ref="E15:E23" si="7">(D15-B15)/(C15-A15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F15" t="e">
@@ -1344,23 +1376,23 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G15" t="e">
-        <f>B15-A15*E15</f>
+        <f t="shared" ref="G15:G23" si="8">B15-A15*E15</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="19">
-        <v>0</v>
-      </c>
-      <c r="I15" s="20">
-        <v>0</v>
-      </c>
-      <c r="J15" s="20">
-        <v>0</v>
-      </c>
-      <c r="K15" s="20">
+      <c r="H15" s="15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0</v>
+      </c>
+      <c r="K15" s="16">
         <v>0</v>
       </c>
       <c r="L15" s="8" t="e">
-        <f>(K15-I15)/(J15-H15)</f>
+        <f t="shared" ref="L15:L23" si="9">(K15-I15)/(J15-H15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M15" s="8" t="e">
@@ -1368,7 +1400,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N15" s="10" t="e">
-        <f>I15-H15*L15</f>
+        <f t="shared" ref="N15:N23" si="10">I15-H15*L15</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O15" t="e">
@@ -1394,39 +1426,39 @@
         <v>4</v>
       </c>
       <c r="E16">
-        <f>(D16-B16)/(C16-A16)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F23" si="7">A16-B16/E16</f>
+        <f t="shared" ref="F16:F23" si="11">A16-B16/E16</f>
         <v>-1</v>
       </c>
       <c r="G16">
-        <f>B16-A16*E16</f>
-        <v>1</v>
-      </c>
-      <c r="H16" s="19">
-        <v>1</v>
-      </c>
-      <c r="I16" s="20">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="H16" s="15">
+        <v>1</v>
+      </c>
+      <c r="I16" s="16">
         <v>3</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="16">
         <v>3</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K16" s="16">
         <v>5</v>
       </c>
       <c r="L16" s="8">
-        <f>(K16-I16)/(J16-H16)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M16" s="8">
-        <f t="shared" ref="M16:M23" si="8">H16-I16/L16</f>
+        <f t="shared" ref="M16:M23" si="12">H16-I16/L16</f>
         <v>-2</v>
       </c>
       <c r="N16" s="10">
-        <f>I16-H16*L16</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="O16" t="e">
@@ -1455,38 +1487,38 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <f>(D17-B17)/(C17-A17)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F17" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G17">
-        <f>B17-A17*E17</f>
-        <v>1</v>
-      </c>
-      <c r="H17" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="H17" s="15">
         <v>3.3</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="16">
         <v>-2.4</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="16">
         <v>3.3</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="16">
         <v>6.6</v>
       </c>
       <c r="L17" s="8" t="e">
-        <f>(K17-I17)/(J17-H17)</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M17" s="20">
+      <c r="M17" s="16">
         <v>3.3</v>
       </c>
       <c r="N17" s="10" t="e">
-        <f>I17-H17*L17</f>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O17" s="5">
@@ -1513,47 +1545,47 @@
         <v>4</v>
       </c>
       <c r="E18">
-        <f>(D18-B18)/(C18-A18)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="G18">
-        <f>B18-A18*E18</f>
-        <v>1</v>
-      </c>
-      <c r="H18" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="H18" s="15">
         <v>3.3</v>
       </c>
-      <c r="I18" s="20">
+      <c r="I18" s="16">
         <v>-2.4</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="16">
         <v>-5.7</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18" s="16">
         <v>6.6</v>
       </c>
       <c r="L18" s="8">
-        <f>(K18-I18)/(J18-H18)</f>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="M18" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="N18" s="10">
-        <f>I18-H18*L18</f>
+        <f t="shared" si="10"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="O18">
-        <f>(G18-N18)/(L18-E18)</f>
+        <f t="shared" ref="O18:O23" si="13">(G18-N18)/(L18-E18)</f>
         <v>-5.0000000000000044E-2</v>
       </c>
       <c r="P18">
-        <f>G18+E18*(G18-N18)/(L18-E18)</f>
+        <f t="shared" ref="P18:P23" si="14">G18+E18*(G18-N18)/(L18-E18)</f>
         <v>0.95</v>
       </c>
       <c r="Q18" t="s">
@@ -1574,47 +1606,47 @@
         <v>4</v>
       </c>
       <c r="E19">
-        <f>(D19-B19)/(C19-A19)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="G19">
-        <f>B19-A19*E19</f>
-        <v>1</v>
-      </c>
-      <c r="H19" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="H19" s="15">
         <v>3.3</v>
       </c>
-      <c r="I19" s="20">
+      <c r="I19" s="16">
         <v>-2.4</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="16">
         <v>-1</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19" s="16">
         <v>6.6</v>
       </c>
       <c r="L19" s="8">
-        <f>(K19-I19)/(J19-H19)</f>
+        <f t="shared" si="9"/>
         <v>-2.0930232558139537</v>
       </c>
       <c r="M19" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2.1533333333333333</v>
       </c>
       <c r="N19" s="10">
-        <f>I19-H19*L19</f>
+        <f t="shared" si="10"/>
         <v>4.506976744186046</v>
       </c>
       <c r="O19">
-        <f>(G19-N19)/(L19-E19)</f>
+        <f t="shared" si="13"/>
         <v>1.1338345864661652</v>
       </c>
       <c r="P19">
-        <f>G19+E19*(G19-N19)/(L19-E19)</f>
+        <f t="shared" si="14"/>
         <v>2.1338345864661652</v>
       </c>
     </row>
@@ -1632,47 +1664,47 @@
         <v>-2</v>
       </c>
       <c r="E20">
-        <f>(D20-B20)/(C20-A20)</f>
+        <f t="shared" si="7"/>
         <v>-4</v>
       </c>
       <c r="F20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.5</v>
       </c>
       <c r="G20">
-        <f>B20-A20*E20</f>
+        <f t="shared" si="8"/>
         <v>-14</v>
       </c>
-      <c r="H20" s="23">
-        <v>1</v>
-      </c>
-      <c r="I20" s="24">
+      <c r="H20" s="19">
+        <v>1</v>
+      </c>
+      <c r="I20" s="20">
         <v>5</v>
       </c>
-      <c r="J20" s="24">
+      <c r="J20" s="20">
         <v>-7</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="20">
         <v>3</v>
       </c>
       <c r="L20" s="11">
-        <f>(K20-I20)/(J20-H20)</f>
+        <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
       <c r="M20" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>-19</v>
       </c>
       <c r="N20" s="12">
-        <f>I20-H20*L20</f>
+        <f t="shared" si="10"/>
         <v>4.75</v>
       </c>
       <c r="O20">
-        <f>(G20-N20)/(L20-E20)</f>
+        <f t="shared" si="13"/>
         <v>-4.4117647058823533</v>
       </c>
       <c r="P20">
-        <f>G20+E20*(G20-N20)/(L20-E20)</f>
+        <f t="shared" si="14"/>
         <v>3.647058823529413</v>
       </c>
     </row>
@@ -1690,47 +1722,47 @@
         <v>8</v>
       </c>
       <c r="E21" t="e">
-        <f>(D21-B21)/(C21-A21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F21" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="F21" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G21" t="e">
-        <f>B21-A21*E21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="24">
-        <v>-5</v>
-      </c>
-      <c r="I21" s="24">
-        <v>6</v>
-      </c>
-      <c r="J21" s="24">
-        <v>5</v>
-      </c>
-      <c r="K21" s="24">
-        <v>6</v>
-      </c>
-      <c r="L21" s="11">
-        <f>(K21-I21)/(J21-H21)</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="11" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="H21" s="20">
+        <v>-5</v>
+      </c>
+      <c r="I21" s="20">
+        <v>6</v>
+      </c>
+      <c r="J21" s="20">
+        <v>5</v>
+      </c>
+      <c r="K21" s="20">
+        <v>6</v>
+      </c>
+      <c r="L21" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="11" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N21" s="12">
-        <f>I21-H21*L21</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="O21" t="e">
-        <f>(G21-N21)/(L21-E21)</f>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P21" t="e">
-        <f>G21+E21*(G21-N21)/(L21-E21)</f>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1748,47 +1780,47 @@
         <v>2</v>
       </c>
       <c r="E22" t="e">
-        <f>(D22-B22)/(C22-A22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="F22" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G22" s="11" t="e">
-        <f>B22-A22*E22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H22" s="24">
-        <v>-5</v>
-      </c>
-      <c r="I22" s="24">
-        <v>6</v>
-      </c>
-      <c r="J22" s="24">
-        <v>5</v>
-      </c>
-      <c r="K22" s="24">
-        <v>6</v>
-      </c>
-      <c r="L22" s="11">
-        <f>(K22-I22)/(J22-H22)</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="11" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="H22" s="20">
+        <v>-5</v>
+      </c>
+      <c r="I22" s="20">
+        <v>6</v>
+      </c>
+      <c r="J22" s="20">
+        <v>5</v>
+      </c>
+      <c r="K22" s="20">
+        <v>6</v>
+      </c>
+      <c r="L22" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="11" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N22" s="12">
-        <f>I22-H22*L22</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="O22" t="e">
-        <f>(G22-N22)/(L22-E22)</f>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P22" t="e">
-        <f>G22+E22*(G22-N22)/(L22-E22)</f>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1806,47 +1838,47 @@
         <v>-2</v>
       </c>
       <c r="E23">
-        <f>(D23-B23)/(C23-A23)</f>
+        <f t="shared" si="7"/>
         <v>-4</v>
       </c>
       <c r="F23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.5</v>
       </c>
       <c r="G23" s="11">
-        <f>B23-A23*E23</f>
+        <f t="shared" si="8"/>
         <v>-14</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H23" s="20">
         <v>5.2</v>
       </c>
-      <c r="I23" s="24">
+      <c r="I23" s="20">
         <v>6.1</v>
       </c>
-      <c r="J23" s="24">
+      <c r="J23" s="20">
         <v>7.7</v>
       </c>
-      <c r="K23" s="24">
+      <c r="K23" s="20">
         <v>-1.3</v>
       </c>
       <c r="L23" s="11">
-        <f>(K23-I23)/(J23-H23)</f>
+        <f t="shared" si="9"/>
         <v>-2.96</v>
       </c>
       <c r="M23" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7.2608108108108107</v>
       </c>
       <c r="N23" s="12">
-        <f>I23-H23*L23</f>
+        <f t="shared" si="10"/>
         <v>21.491999999999997</v>
       </c>
       <c r="O23">
-        <f>(G23-N23)/(L23-E23)</f>
+        <f t="shared" si="13"/>
         <v>-34.12692307692307</v>
       </c>
       <c r="P23">
-        <f>G23+E23*(G23-N23)/(L23-E23)</f>
+        <f t="shared" si="14"/>
         <v>122.50769230769228</v>
       </c>
     </row>
@@ -1855,10 +1887,10 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
@@ -1868,10 +1900,10 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
@@ -1881,10 +1913,10 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
@@ -1971,23 +2003,23 @@
         <v>2</v>
       </c>
       <c r="E31">
-        <f t="shared" ref="E31:E34" si="9">C31-A31</f>
+        <f t="shared" ref="E31:E34" si="15">C31-A31</f>
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" ref="F31:F34" si="10">D31-B31</f>
+        <f t="shared" ref="F31:F34" si="16">D31-B31</f>
         <v>1</v>
       </c>
       <c r="G31">
-        <f t="shared" ref="G31:G34" si="11">SQRT(E31^2+F31^2)</f>
+        <f t="shared" ref="G31:G34" si="17">SQRT(E31^2+F31^2)</f>
         <v>1</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31:H34" si="12">0.5*(A31+C31)</f>
+        <f t="shared" ref="H31:H34" si="18">0.5*(A31+C31)</f>
         <v>1</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:I34" si="13">0.5*(B31+D31)</f>
+        <f t="shared" ref="I31:I34" si="19">0.5*(B31+D31)</f>
         <v>1.5</v>
       </c>
     </row>
@@ -2005,23 +2037,23 @@
         <v>4</v>
       </c>
       <c r="E32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="F32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="G32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>2.8284271247461903</v>
       </c>
       <c r="H32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="I32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -2039,23 +2071,23 @@
         <v>-4</v>
       </c>
       <c r="E33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-2</v>
       </c>
       <c r="F33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-2</v>
       </c>
       <c r="G33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>2.8284271247461903</v>
       </c>
       <c r="H33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>-2</v>
       </c>
       <c r="I33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>-3</v>
       </c>
     </row>
@@ -2073,23 +2105,23 @@
         <v>-4</v>
       </c>
       <c r="E34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-4</v>
       </c>
       <c r="F34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-6</v>
       </c>
       <c r="G34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>7.2111025509279782</v>
       </c>
       <c r="H34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>-1</v>
       </c>
       <c r="I34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>-1</v>
       </c>
     </row>
@@ -2099,14 +2131,14 @@
       </c>
     </row>
     <row r="37" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O37" s="14" t="s">
+      <c r="O37" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14" t="s">
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="R37" s="14"/>
+      <c r="R37" s="24"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
@@ -2130,16 +2162,16 @@
       <c r="G38" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H38" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="I38" s="21" t="s">
+      <c r="H38" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="17" t="s">
         <v>3</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K38" s="21" t="s">
+      <c r="K38" s="17" t="s">
         <v>12</v>
       </c>
       <c r="L38" s="4" t="s">
@@ -2151,16 +2183,16 @@
       <c r="N38" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O38" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="P38" s="21" t="s">
+      <c r="O38" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P38" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="Q38" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="R38" s="21" t="s">
+      <c r="Q38" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R38" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2247,23 +2279,23 @@
         <v>2</v>
       </c>
       <c r="E40" t="e">
-        <f t="shared" ref="E40:E47" si="14">(D40-B40)/(C40-A40)</f>
+        <f t="shared" ref="E40:E47" si="20">(D40-B40)/(C40-A40)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F40" t="e">
-        <f t="shared" ref="F40:F47" si="15">A40-B40/E40</f>
+        <f t="shared" ref="F40:F47" si="21">A40-B40/E40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G40" t="e">
-        <f t="shared" ref="G40:G47" si="16">B40-A40*E40</f>
+        <f t="shared" ref="G40:G47" si="22">B40-A40*E40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H40" s="13">
-        <f t="shared" ref="H40:H43" si="17">A40+J40*(C40-A40)</f>
+        <f t="shared" ref="H40:H43" si="23">A40+J40*(C40-A40)</f>
         <v>1</v>
       </c>
       <c r="I40" s="13">
-        <f t="shared" ref="I40:I43" si="18">B40+J40*(D40-B40)</f>
+        <f t="shared" ref="I40:I43" si="24">B40+J40*(D40-B40)</f>
         <v>1.25</v>
       </c>
       <c r="J40" s="5">
@@ -2274,31 +2306,31 @@
         <v>0.25</v>
       </c>
       <c r="L40">
-        <f t="shared" ref="L40:L47" si="19">C40-A40</f>
+        <f t="shared" ref="L40:L47" si="25">C40-A40</f>
         <v>0</v>
       </c>
       <c r="M40">
-        <f t="shared" ref="M40:M47" si="20">D40-B40</f>
+        <f t="shared" ref="M40:M47" si="26">D40-B40</f>
         <v>1</v>
       </c>
       <c r="N40">
-        <f t="shared" ref="N40:N47" si="21">SQRT(L40^2+M40^2)</f>
+        <f t="shared" ref="N40:N47" si="27">SQRT(L40^2+M40^2)</f>
         <v>1</v>
       </c>
       <c r="O40" s="13">
-        <f t="shared" ref="O40:O47" si="22">-M40/$N40</f>
+        <f t="shared" ref="O40:O47" si="28">-M40/$N40</f>
         <v>-1</v>
       </c>
       <c r="P40" s="13">
-        <f t="shared" ref="P40:P47" si="23">L40/$N40</f>
+        <f t="shared" ref="P40:P47" si="29">L40/$N40</f>
         <v>0</v>
       </c>
       <c r="Q40" s="13">
-        <f t="shared" ref="Q40:Q47" si="24">L40/$N40</f>
+        <f t="shared" ref="Q40:Q47" si="30">L40/$N40</f>
         <v>0</v>
       </c>
       <c r="R40" s="13">
-        <f t="shared" ref="R40:R47" si="25">M40/$N40</f>
+        <f t="shared" ref="R40:R47" si="31">M40/$N40</f>
         <v>1</v>
       </c>
     </row>
@@ -2316,23 +2348,23 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="F41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
       <c r="G41">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="H41" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1.5</v>
       </c>
       <c r="I41" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2.5</v>
       </c>
       <c r="J41" s="5">
@@ -2343,31 +2375,31 @@
         <v>0.25</v>
       </c>
       <c r="L41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="M41">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>2</v>
       </c>
       <c r="N41">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>2.8284271247461903</v>
       </c>
-      <c r="O41" s="22">
-        <f t="shared" si="22"/>
+      <c r="O41" s="18">
+        <f t="shared" si="28"/>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="P41" s="22">
-        <f t="shared" si="23"/>
+      <c r="P41" s="18">
+        <f t="shared" si="29"/>
         <v>0.70710678118654746</v>
       </c>
       <c r="Q41" s="13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.70710678118654746</v>
       </c>
       <c r="R41" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654746</v>
       </c>
     </row>
@@ -2385,23 +2417,23 @@
         <v>-4</v>
       </c>
       <c r="E42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="F42">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="G42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>-1</v>
       </c>
       <c r="H42" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>-1.5</v>
       </c>
       <c r="I42" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>-2.5</v>
       </c>
       <c r="J42" s="5">
@@ -2412,31 +2444,31 @@
         <v>0.25</v>
       </c>
       <c r="L42">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>-2</v>
       </c>
       <c r="M42">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>-2</v>
       </c>
       <c r="N42">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>2.8284271247461903</v>
       </c>
-      <c r="O42" s="22">
-        <f t="shared" si="22"/>
+      <c r="O42" s="18">
+        <f t="shared" si="28"/>
         <v>0.70710678118654746</v>
       </c>
-      <c r="P42" s="22">
-        <f t="shared" si="23"/>
+      <c r="P42" s="18">
+        <f t="shared" si="29"/>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="Q42" s="22">
-        <f t="shared" si="24"/>
+      <c r="Q42" s="18">
+        <f t="shared" si="30"/>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="R42" s="22">
-        <f t="shared" si="25"/>
+      <c r="R42" s="18">
+        <f t="shared" si="31"/>
         <v>-0.70710678118654746</v>
       </c>
     </row>
@@ -2454,23 +2486,23 @@
         <v>-4</v>
       </c>
       <c r="E43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>1.5</v>
       </c>
       <c r="F43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>-0.33333333333333326</v>
       </c>
       <c r="G43">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.5</v>
       </c>
       <c r="H43" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>-0.19999999999999996</v>
       </c>
       <c r="I43" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="J43" s="5">
@@ -2481,31 +2513,31 @@
         <v>0.3</v>
       </c>
       <c r="L43">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>-4</v>
       </c>
       <c r="M43">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>-6</v>
       </c>
       <c r="N43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>7.2111025509279782</v>
       </c>
-      <c r="O43" s="22">
-        <f t="shared" si="22"/>
+      <c r="O43" s="18">
+        <f t="shared" si="28"/>
         <v>0.83205029433784372</v>
       </c>
-      <c r="P43" s="22">
-        <f t="shared" si="23"/>
+      <c r="P43" s="18">
+        <f t="shared" si="29"/>
         <v>-0.55470019622522915</v>
       </c>
-      <c r="Q43" s="22">
-        <f t="shared" si="24"/>
+      <c r="Q43" s="18">
+        <f t="shared" si="30"/>
         <v>-0.55470019622522915</v>
       </c>
-      <c r="R43" s="22">
-        <f t="shared" si="25"/>
+      <c r="R43" s="18">
+        <f t="shared" si="31"/>
         <v>-0.83205029433784372</v>
       </c>
     </row>
@@ -2523,54 +2555,54 @@
         <v>2</v>
       </c>
       <c r="E44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="F44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
       <c r="G44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="H44" s="13">
-        <f t="shared" ref="H44:H47" si="26">A44+J44*(C44-A44)</f>
+        <f t="shared" ref="H44:H47" si="32">A44+J44*(C44-A44)</f>
         <v>2</v>
       </c>
       <c r="I44" s="13">
-        <f t="shared" ref="I44:I46" si="27">B44+J44*(D44-B44)</f>
+        <f t="shared" ref="I44:I46" si="33">B44+J44*(D44-B44)</f>
         <v>3</v>
       </c>
       <c r="J44" s="5">
         <v>0.5</v>
       </c>
       <c r="L44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>-2</v>
       </c>
       <c r="M44">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>-2</v>
       </c>
       <c r="N44">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>2.8284271247461903</v>
       </c>
-      <c r="O44" s="22">
-        <f t="shared" si="22"/>
+      <c r="O44" s="18">
+        <f t="shared" si="28"/>
         <v>0.70710678118654746</v>
       </c>
-      <c r="P44" s="22">
-        <f t="shared" si="23"/>
+      <c r="P44" s="18">
+        <f t="shared" si="29"/>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="Q44" s="22">
-        <f t="shared" si="24"/>
+      <c r="Q44" s="18">
+        <f t="shared" si="30"/>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="R44" s="22">
-        <f t="shared" si="25"/>
+      <c r="R44" s="18">
+        <f t="shared" si="31"/>
         <v>-0.70710678118654746</v>
       </c>
     </row>
@@ -2588,54 +2620,54 @@
         <v>1</v>
       </c>
       <c r="E45">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F45" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G45">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="H45" s="13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="I45" s="13">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="J45" s="5">
         <v>0.5</v>
       </c>
       <c r="L45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="M45">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="N45">
-        <f t="shared" si="21"/>
-        <v>2</v>
-      </c>
-      <c r="O45" s="22">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="P45" s="22">
-        <f t="shared" si="23"/>
-        <v>1</v>
-      </c>
-      <c r="Q45" s="22">
-        <f t="shared" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="R45" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="O45" s="18">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="P45" s="18">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="Q45" s="18">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="R45" s="18">
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -2653,54 +2685,54 @@
         <v>4</v>
       </c>
       <c r="E46" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F46" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G46" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H46" s="13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="I46" s="13">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>3</v>
       </c>
       <c r="J46" s="5">
         <v>0.5</v>
       </c>
       <c r="L46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M46">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>2</v>
       </c>
       <c r="N46">
-        <f t="shared" si="21"/>
-        <v>2</v>
-      </c>
-      <c r="O46" s="22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="O46" s="18">
+        <f t="shared" si="28"/>
         <v>-1</v>
       </c>
-      <c r="P46" s="22">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="Q46" s="22">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="R46" s="22">
-        <f t="shared" si="25"/>
+      <c r="P46" s="18">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="18">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="R46" s="18">
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
     </row>
@@ -2718,19 +2750,19 @@
         <v>4</v>
       </c>
       <c r="E47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="F47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
       <c r="G47">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="H47" s="13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="I47" s="13">
@@ -2741,31 +2773,31 @@
         <v>0.5</v>
       </c>
       <c r="L47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="M47">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>2</v>
       </c>
       <c r="N47">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>2.8284271247461903</v>
       </c>
-      <c r="O47" s="22">
-        <f t="shared" si="22"/>
+      <c r="O47" s="18">
+        <f t="shared" si="28"/>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="P47" s="22">
-        <f t="shared" si="23"/>
+      <c r="P47" s="18">
+        <f t="shared" si="29"/>
         <v>0.70710678118654746</v>
       </c>
-      <c r="Q47" s="22">
-        <f t="shared" si="24"/>
+      <c r="Q47" s="18">
+        <f t="shared" si="30"/>
         <v>0.70710678118654746</v>
       </c>
-      <c r="R47" s="22">
-        <f t="shared" si="25"/>
+      <c r="R47" s="18">
+        <f t="shared" si="31"/>
         <v>0.70710678118654746</v>
       </c>
     </row>
@@ -2783,48 +2815,1197 @@
         <v>9.1</v>
       </c>
       <c r="E48">
-        <f t="shared" ref="E48" si="28">(D48-B48)/(C48-A48)</f>
+        <f t="shared" ref="E48" si="34">(D48-B48)/(C48-A48)</f>
         <v>1.0363636363636362</v>
       </c>
       <c r="F48">
-        <f t="shared" ref="F48" si="29">A48-B48/E48</f>
+        <f t="shared" ref="F48" si="35">A48-B48/E48</f>
         <v>-2.0807017543859656</v>
       </c>
       <c r="G48">
-        <f t="shared" ref="G48" si="30">B48-A48*E48</f>
+        <f t="shared" ref="G48" si="36">B48-A48*E48</f>
         <v>2.1563636363636363</v>
       </c>
       <c r="H48" s="13">
-        <f t="shared" ref="H48" si="31">A48+J48*(C48-A48)</f>
+        <f t="shared" ref="H48" si="37">A48+J48*(C48-A48)</f>
         <v>2.8499999999999996</v>
       </c>
       <c r="I48" s="13">
-        <f t="shared" ref="I48" si="32">B48+J48*(D48-B48)</f>
+        <f t="shared" ref="I48" si="38">B48+J48*(D48-B48)</f>
         <v>5.1099999999999994</v>
       </c>
       <c r="J48" s="5">
         <v>0.3</v>
       </c>
       <c r="L48">
-        <f t="shared" ref="L48" si="33">C48-A48</f>
+        <f t="shared" ref="L48" si="39">C48-A48</f>
         <v>5.5</v>
       </c>
       <c r="M48">
-        <f t="shared" ref="M48" si="34">D48-B48</f>
+        <f t="shared" ref="M48" si="40">D48-B48</f>
         <v>5.6999999999999993</v>
       </c>
       <c r="N48">
-        <f t="shared" ref="N48" si="35">SQRT(L48^2+M48^2)</f>
+        <f t="shared" ref="N48" si="41">SQRT(L48^2+M48^2)</f>
         <v>7.9208585393251401</v>
       </c>
     </row>
+    <row r="50" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="25"/>
+      <c r="F51" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I51" s="25"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="5">
+        <v>2</v>
+      </c>
+      <c r="B53" s="5">
+        <v>1</v>
+      </c>
+      <c r="C53" s="5">
+        <v>8</v>
+      </c>
+      <c r="D53" s="5">
+        <v>4</v>
+      </c>
+      <c r="E53" s="5">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f>A53</f>
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <f>B53</f>
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <f>ROUND(A53+((C53-A53)*COS(E53)-(D53-B53)*SIN(E53)), 6)</f>
+        <v>8</v>
+      </c>
+      <c r="I53">
+        <f>ROUND(B53+((C53-A53)*SIN(E53)+(D53-B53)*COS(E53)),6)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="5">
+        <v>2</v>
+      </c>
+      <c r="B54" s="5">
+        <v>1</v>
+      </c>
+      <c r="C54" s="5">
+        <v>8</v>
+      </c>
+      <c r="D54" s="5">
+        <v>4</v>
+      </c>
+      <c r="E54" s="5">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="F54">
+        <f>A54</f>
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <f>B54</f>
+        <v>1</v>
+      </c>
+      <c r="H54" s="26">
+        <f>ROUND(A54+((C54-A54)*COS(E54)-(D54-B54)*SIN(E54)), 6)</f>
+        <v>4.1213199999999999</v>
+      </c>
+      <c r="I54">
+        <f>ROUND(B54+((C54-A54)*SIN(E54)+(D54-B54)*COS(E54)),6)</f>
+        <v>7.3639609999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="5">
+        <v>2</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1</v>
+      </c>
+      <c r="C55" s="5">
+        <v>8</v>
+      </c>
+      <c r="D55" s="5">
+        <v>4</v>
+      </c>
+      <c r="E55" s="5">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="F55">
+        <f>A55</f>
+        <v>2</v>
+      </c>
+      <c r="G55">
+        <f>B55</f>
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <f>ROUND(A55+((C55-A55)*COS(E55)-(D55-B55)*SIN(E55)), 6)</f>
+        <v>-1</v>
+      </c>
+      <c r="I55">
+        <f>ROUND(B55+((C55-A55)*SIN(E55)+(D55-B55)*COS(E55)),6)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
+        <v>2</v>
+      </c>
+      <c r="B56" s="5">
+        <v>1</v>
+      </c>
+      <c r="C56" s="5">
+        <v>8</v>
+      </c>
+      <c r="D56" s="5">
+        <v>4</v>
+      </c>
+      <c r="E56" s="5">
+        <f>(3/4)*PI()</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="F56">
+        <f>A56</f>
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <f>B56</f>
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <f>ROUND(A56+((C56-A56)*COS(E56)-(D56-B56)*SIN(E56)), 6)</f>
+        <v>-4.3639609999999998</v>
+      </c>
+      <c r="I56" s="26">
+        <f>ROUND(B56+((C56-A56)*SIN(E56)+(D56-B56)*COS(E56)),6)</f>
+        <v>3.1213199999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="5">
+        <v>2</v>
+      </c>
+      <c r="B57" s="5">
+        <v>1</v>
+      </c>
+      <c r="C57" s="5">
+        <v>8</v>
+      </c>
+      <c r="D57" s="5">
+        <v>4</v>
+      </c>
+      <c r="E57" s="5">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="F57">
+        <f>A57</f>
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <f>B57</f>
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <f>ROUND(A57+((C57-A57)*COS(E57)-(D57-B57)*SIN(E57)), 6)</f>
+        <v>-4</v>
+      </c>
+      <c r="I57">
+        <f>ROUND(B57+((C57-A57)*SIN(E57)+(D57-B57)*COS(E57)),6)</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="5">
+        <v>2</v>
+      </c>
+      <c r="B58" s="5">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5">
+        <v>8</v>
+      </c>
+      <c r="D58" s="5">
+        <v>4</v>
+      </c>
+      <c r="E58" s="5">
+        <f>(5/4)*PI()</f>
+        <v>3.9269908169872414</v>
+      </c>
+      <c r="F58">
+        <f>A58</f>
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <f>B58</f>
+        <v>1</v>
+      </c>
+      <c r="H58" s="26">
+        <f>ROUND(A58+((C58-A58)*COS(E58)-(D58-B58)*SIN(E58)), 6)</f>
+        <v>-0.12132</v>
+      </c>
+      <c r="I58">
+        <f>ROUND(B58+((C58-A58)*SIN(E58)+(D58-B58)*COS(E58)),6)</f>
+        <v>-5.3639609999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="5">
+        <v>2</v>
+      </c>
+      <c r="B59" s="5">
+        <v>1</v>
+      </c>
+      <c r="C59" s="5">
+        <v>8</v>
+      </c>
+      <c r="D59" s="5">
+        <v>4</v>
+      </c>
+      <c r="E59" s="5">
+        <f>(3/2)*PI()</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="F59">
+        <f>A59</f>
+        <v>2</v>
+      </c>
+      <c r="G59">
+        <f>B59</f>
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <f>ROUND(A59+((C59-A59)*COS(E59)-(D59-B59)*SIN(E59)), 6)</f>
+        <v>5</v>
+      </c>
+      <c r="I59">
+        <f>ROUND(B59+((C59-A59)*SIN(E59)+(D59-B59)*COS(E59)),6)</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
+        <v>2</v>
+      </c>
+      <c r="B60" s="5">
+        <v>1</v>
+      </c>
+      <c r="C60" s="5">
+        <v>8</v>
+      </c>
+      <c r="D60" s="5">
+        <v>4</v>
+      </c>
+      <c r="E60" s="5">
+        <f>(7/4)*PI()</f>
+        <v>5.497787143782138</v>
+      </c>
+      <c r="F60">
+        <f>A60</f>
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <f>B60</f>
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <f>ROUND(A60+((C60-A60)*COS(E60)-(D60-B60)*SIN(E60)), 6)</f>
+        <v>8.3639609999999998</v>
+      </c>
+      <c r="I60" s="26">
+        <f>ROUND(B60+((C60-A60)*SIN(E60)+(D60-B60)*COS(E60)),6)</f>
+        <v>-1.1213200000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="5">
+        <v>2</v>
+      </c>
+      <c r="B61" s="5">
+        <v>1</v>
+      </c>
+      <c r="C61" s="5">
+        <v>8</v>
+      </c>
+      <c r="D61" s="5">
+        <v>4</v>
+      </c>
+      <c r="E61" s="5">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="F61">
+        <f>A61</f>
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <f>B61</f>
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <f>ROUND(A61+((C61-A61)*COS(E61)-(D61-B61)*SIN(E61)), 6)</f>
+        <v>8.3639609999999998</v>
+      </c>
+      <c r="I61" s="26">
+        <f>ROUND(B61+((C61-A61)*SIN(E61)+(D61-B61)*COS(E61)),6)</f>
+        <v>-1.1213200000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="25"/>
+      <c r="F64" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I64" s="25"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="5">
+        <v>2</v>
+      </c>
+      <c r="B66" s="5">
+        <v>1</v>
+      </c>
+      <c r="C66" s="5">
+        <v>8</v>
+      </c>
+      <c r="D66" s="5">
+        <v>4</v>
+      </c>
+      <c r="E66" s="5">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <f>ROUND(C66+((A66-C66)*COS(E66)-(B66-D66)*SIN(E66)), 6)</f>
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <f>ROUND(D66+((A66-C66)*SIN(E66)+(B66-D66)*COS(E66)),6)</f>
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <f>C66</f>
+        <v>8</v>
+      </c>
+      <c r="I66">
+        <f>D66</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="5">
+        <v>2</v>
+      </c>
+      <c r="B67" s="5">
+        <v>1</v>
+      </c>
+      <c r="C67" s="5">
+        <v>8</v>
+      </c>
+      <c r="D67" s="5">
+        <v>4</v>
+      </c>
+      <c r="E67" s="5">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="F67" s="26">
+        <f>ROUND(C67+((A67-C67)*COS(E67)-(B67-D67)*SIN(E67)), 6)</f>
+        <v>5.8786800000000001</v>
+      </c>
+      <c r="G67">
+        <f>ROUND(D67+((A67-C67)*SIN(E67)+(B67-D67)*COS(E67)),6)</f>
+        <v>-2.3639610000000002</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ref="H67:H74" si="42">C67</f>
+        <v>8</v>
+      </c>
+      <c r="I67">
+        <f t="shared" ref="I67:I74" si="43">D67</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="5">
+        <v>2</v>
+      </c>
+      <c r="B68" s="5">
+        <v>1</v>
+      </c>
+      <c r="C68" s="5">
+        <v>8</v>
+      </c>
+      <c r="D68" s="5">
+        <v>4</v>
+      </c>
+      <c r="E68" s="5">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="F68">
+        <f>ROUND(C68+((A68-C68)*COS(E68)-(B68-D68)*SIN(E68)), 6)</f>
+        <v>11</v>
+      </c>
+      <c r="G68">
+        <f>ROUND(D68+((A68-C68)*SIN(E68)+(B68-D68)*COS(E68)),6)</f>
+        <v>-2</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="43"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="5">
+        <v>2</v>
+      </c>
+      <c r="B69" s="5">
+        <v>1</v>
+      </c>
+      <c r="C69" s="5">
+        <v>8</v>
+      </c>
+      <c r="D69" s="5">
+        <v>4</v>
+      </c>
+      <c r="E69" s="5">
+        <f>(3/4)*PI()</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="F69">
+        <f>ROUND(C69+((A69-C69)*COS(E69)-(B69-D69)*SIN(E69)), 6)</f>
+        <v>14.363961</v>
+      </c>
+      <c r="G69" s="26">
+        <f>ROUND(D69+((A69-C69)*SIN(E69)+(B69-D69)*COS(E69)),6)</f>
+        <v>1.8786799999999999</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="43"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" s="5">
+        <v>2</v>
+      </c>
+      <c r="B70" s="5">
+        <v>1</v>
+      </c>
+      <c r="C70" s="5">
+        <v>8</v>
+      </c>
+      <c r="D70" s="5">
+        <v>4</v>
+      </c>
+      <c r="E70" s="5">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="F70">
+        <f>ROUND(C70+((A70-C70)*COS(E70)-(B70-D70)*SIN(E70)), 6)</f>
+        <v>14</v>
+      </c>
+      <c r="G70">
+        <f>ROUND(D70+((A70-C70)*SIN(E70)+(B70-D70)*COS(E70)),6)</f>
+        <v>7</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="43"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="5">
+        <v>2</v>
+      </c>
+      <c r="B71" s="5">
+        <v>1</v>
+      </c>
+      <c r="C71" s="5">
+        <v>8</v>
+      </c>
+      <c r="D71" s="5">
+        <v>4</v>
+      </c>
+      <c r="E71" s="5">
+        <f>(5/4)*PI()</f>
+        <v>3.9269908169872414</v>
+      </c>
+      <c r="F71" s="26">
+        <f>ROUND(C71+((A71-C71)*COS(E71)-(B71-D71)*SIN(E71)), 6)</f>
+        <v>10.121320000000001</v>
+      </c>
+      <c r="G71">
+        <f>ROUND(D71+((A71-C71)*SIN(E71)+(B71-D71)*COS(E71)),6)</f>
+        <v>10.363961</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="43"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" s="5">
+        <v>2</v>
+      </c>
+      <c r="B72" s="5">
+        <v>1</v>
+      </c>
+      <c r="C72" s="5">
+        <v>8</v>
+      </c>
+      <c r="D72" s="5">
+        <v>4</v>
+      </c>
+      <c r="E72" s="5">
+        <f>(3/2)*PI()</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="F72">
+        <f>ROUND(C72+((A72-C72)*COS(E72)-(B72-D72)*SIN(E72)), 6)</f>
+        <v>5</v>
+      </c>
+      <c r="G72">
+        <f>ROUND(D72+((A72-C72)*SIN(E72)+(B72-D72)*COS(E72)),6)</f>
+        <v>10</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="43"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="5">
+        <v>2</v>
+      </c>
+      <c r="B73" s="5">
+        <v>1</v>
+      </c>
+      <c r="C73" s="5">
+        <v>8</v>
+      </c>
+      <c r="D73" s="5">
+        <v>4</v>
+      </c>
+      <c r="E73" s="5">
+        <f>(7/4)*PI()</f>
+        <v>5.497787143782138</v>
+      </c>
+      <c r="F73">
+        <f>ROUND(C73+((A73-C73)*COS(E73)-(B73-D73)*SIN(E73)), 6)</f>
+        <v>1.636039</v>
+      </c>
+      <c r="G73" s="26">
+        <f>ROUND(D73+((A73-C73)*SIN(E73)+(B73-D73)*COS(E73)),6)</f>
+        <v>6.1213199999999999</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="43"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" s="5">
+        <v>2</v>
+      </c>
+      <c r="B74" s="5">
+        <v>1</v>
+      </c>
+      <c r="C74" s="5">
+        <v>8</v>
+      </c>
+      <c r="D74" s="5">
+        <v>4</v>
+      </c>
+      <c r="E74" s="5">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="F74">
+        <f>ROUND(C74+((A74-C74)*COS(E74)-(B74-D74)*SIN(E74)), 6)</f>
+        <v>1.636039</v>
+      </c>
+      <c r="G74" s="26">
+        <f>ROUND(D74+((A74-C74)*SIN(E74)+(B74-D74)*COS(E74)),6)</f>
+        <v>6.1213199999999999</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="43"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D77" s="25"/>
+      <c r="E77" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F77" s="25"/>
+      <c r="H77" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I77" s="25"/>
+      <c r="J77" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="K77" s="25"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="5">
+        <v>2</v>
+      </c>
+      <c r="B79" s="5">
+        <v>1</v>
+      </c>
+      <c r="C79" s="5">
+        <v>8</v>
+      </c>
+      <c r="D79" s="5">
+        <v>4</v>
+      </c>
+      <c r="E79" s="5">
+        <v>13</v>
+      </c>
+      <c r="F79" s="5">
+        <v>-12</v>
+      </c>
+      <c r="G79" s="5">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <f>ROUND(E79+((A79-E79)*COS(G79)-(B79-F79)*SIN(G79)), 6)</f>
+        <v>2</v>
+      </c>
+      <c r="I79">
+        <f>ROUND(F79+((A79-E79)*SIN(G79)+(B79-F79)*COS(G79)),6)</f>
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <f>ROUND(E79+((C79-E79)*COS(G79)-(D79-F79)*SIN(G79)), 6)</f>
+        <v>8</v>
+      </c>
+      <c r="K79">
+        <f>ROUND(F79+((C79-E79)*SIN(G79)+(D79-F79)*COS(G79)),6)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="5">
+        <v>2</v>
+      </c>
+      <c r="B80" s="5">
+        <v>1</v>
+      </c>
+      <c r="C80" s="5">
+        <v>8</v>
+      </c>
+      <c r="D80" s="5">
+        <v>4</v>
+      </c>
+      <c r="E80" s="5">
+        <v>13</v>
+      </c>
+      <c r="F80" s="5">
+        <v>-12</v>
+      </c>
+      <c r="G80" s="5">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="H80">
+        <f t="shared" ref="H80:H87" si="44">ROUND(E80+((A80-E80)*COS(G80)-(B80-F80)*SIN(G80)), 6)</f>
+        <v>-3.9705629999999998</v>
+      </c>
+      <c r="I80">
+        <f t="shared" ref="I80:I87" si="45">ROUND(F80+((A80-E80)*SIN(G80)+(B80-F80)*COS(G80)),6)</f>
+        <v>-10.585786000000001</v>
+      </c>
+      <c r="J80" s="26">
+        <f t="shared" ref="J80:J87" si="46">ROUND(E80+((C80-E80)*COS(G80)-(D80-F80)*SIN(G80)), 6)</f>
+        <v>-1.8492420000000001</v>
+      </c>
+      <c r="K80">
+        <f t="shared" ref="K80:K87" si="47">ROUND(F80+((C80-E80)*SIN(G80)+(D80-F80)*COS(G80)),6)</f>
+        <v>-4.2218249999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="5">
+        <v>2</v>
+      </c>
+      <c r="B81" s="5">
+        <v>1</v>
+      </c>
+      <c r="C81" s="5">
+        <v>8</v>
+      </c>
+      <c r="D81" s="5">
+        <v>4</v>
+      </c>
+      <c r="E81" s="5">
+        <v>13</v>
+      </c>
+      <c r="F81" s="5">
+        <v>-12</v>
+      </c>
+      <c r="G81" s="5">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="45"/>
+        <v>-23</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="46"/>
+        <v>-3</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="47"/>
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="5">
+        <v>2</v>
+      </c>
+      <c r="B82" s="5">
+        <v>1</v>
+      </c>
+      <c r="C82" s="5">
+        <v>8</v>
+      </c>
+      <c r="D82" s="5">
+        <v>4</v>
+      </c>
+      <c r="E82" s="5">
+        <v>13</v>
+      </c>
+      <c r="F82" s="5">
+        <v>-12</v>
+      </c>
+      <c r="G82" s="5">
+        <f>(3/4)*PI()</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="44"/>
+        <v>11.585786000000001</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="45"/>
+        <v>-28.970562999999999</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="46"/>
+        <v>5.2218249999999999</v>
+      </c>
+      <c r="K82" s="26">
+        <f t="shared" si="47"/>
+        <v>-26.849242</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="5">
+        <v>2</v>
+      </c>
+      <c r="B83" s="5">
+        <v>1</v>
+      </c>
+      <c r="C83" s="5">
+        <v>8</v>
+      </c>
+      <c r="D83" s="5">
+        <v>4</v>
+      </c>
+      <c r="E83" s="5">
+        <v>13</v>
+      </c>
+      <c r="F83" s="5">
+        <v>-12</v>
+      </c>
+      <c r="G83" s="5">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="44"/>
+        <v>24</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="45"/>
+        <v>-25</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="46"/>
+        <v>18</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="47"/>
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" s="5">
+        <v>2</v>
+      </c>
+      <c r="B84" s="5">
+        <v>1</v>
+      </c>
+      <c r="C84" s="5">
+        <v>8</v>
+      </c>
+      <c r="D84" s="5">
+        <v>4</v>
+      </c>
+      <c r="E84" s="5">
+        <v>13</v>
+      </c>
+      <c r="F84" s="5">
+        <v>-12</v>
+      </c>
+      <c r="G84" s="5">
+        <f>(5/4)*PI()</f>
+        <v>3.9269908169872414</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="44"/>
+        <v>29.970562999999999</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="45"/>
+        <v>-13.414213999999999</v>
+      </c>
+      <c r="J84" s="26">
+        <f t="shared" si="46"/>
+        <v>27.849242</v>
+      </c>
+      <c r="K84" s="26">
+        <f t="shared" si="47"/>
+        <v>-19.778175000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="5">
+        <v>2</v>
+      </c>
+      <c r="B85" s="5">
+        <v>1</v>
+      </c>
+      <c r="C85" s="5">
+        <v>8</v>
+      </c>
+      <c r="D85" s="5">
+        <v>4</v>
+      </c>
+      <c r="E85" s="5">
+        <v>13</v>
+      </c>
+      <c r="F85" s="5">
+        <v>-12</v>
+      </c>
+      <c r="G85" s="5">
+        <f>(3/2)*PI()</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="44"/>
+        <v>26</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="45"/>
+        <v>-1</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="46"/>
+        <v>29</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="47"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" s="5">
+        <v>2</v>
+      </c>
+      <c r="B86" s="5">
+        <v>1</v>
+      </c>
+      <c r="C86" s="5">
+        <v>8</v>
+      </c>
+      <c r="D86" s="5">
+        <v>4</v>
+      </c>
+      <c r="E86" s="5">
+        <v>13</v>
+      </c>
+      <c r="F86" s="5">
+        <v>-12</v>
+      </c>
+      <c r="G86" s="5">
+        <f>(7/4)*PI()</f>
+        <v>5.497787143782138</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="44"/>
+        <v>14.414213999999999</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="45"/>
+        <v>4.9705630000000003</v>
+      </c>
+      <c r="J86" s="26">
+        <f t="shared" si="46"/>
+        <v>20.778175000000001</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="47"/>
+        <v>2.8492419999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" s="5">
+        <v>2</v>
+      </c>
+      <c r="B87" s="5">
+        <v>1</v>
+      </c>
+      <c r="C87" s="5">
+        <v>8</v>
+      </c>
+      <c r="D87" s="5">
+        <v>4</v>
+      </c>
+      <c r="E87" s="5">
+        <v>13</v>
+      </c>
+      <c r="F87" s="5">
+        <v>-12</v>
+      </c>
+      <c r="G87" s="5">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="44"/>
+        <v>14.414213999999999</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="45"/>
+        <v>4.9705630000000003</v>
+      </c>
+      <c r="J87" s="26">
+        <f t="shared" si="46"/>
+        <v>20.778175000000001</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="47"/>
+        <v>2.8492419999999998</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="17">
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="E77:F77"/>
     <mergeCell ref="H13:N13"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="O37:P37"/>
     <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Unit Testing of Straight Segmented Shapes
All shapes comprised solely of straight segments have been fully unit tested and validated.
</commit_message>
<xml_diff>
--- a/docs/Geometry Tests.xlsx
+++ b/docs/Geometry Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\personal\MPT.Net\MPT\Geometry\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42B5F2E-F380-46FD-8F6C-A81167246C71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468329D3-9EBE-46FB-9FCC-E338C728DA0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="824" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extents" sheetId="4" r:id="rId1"/>
@@ -23,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="148">
   <si>
     <t>X</t>
   </si>
@@ -353,15 +347,144 @@
   <si>
     <t>Pentagon</t>
   </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>Pt A</t>
+  </si>
+  <si>
+    <t>Pt B</t>
+  </si>
+  <si>
+    <t>Pt C</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Side Lengths</t>
+  </si>
+  <si>
+    <t>30-60-90</t>
+  </si>
+  <si>
+    <t>60-60-60</t>
+  </si>
+  <si>
+    <t>Area (K)</t>
+  </si>
+  <si>
+    <t>Altitude</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Angle Bisecor</t>
+  </si>
+  <si>
+    <t>Semiperimeter</t>
+  </si>
+  <si>
+    <t>45-45-90</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Perpendiculat Side Bisector</t>
+  </si>
+  <si>
+    <t>a'</t>
+  </si>
+  <si>
+    <t>b'</t>
+  </si>
+  <si>
+    <t>c'</t>
+  </si>
+  <si>
+    <t>a''</t>
+  </si>
+  <si>
+    <t>b''</t>
+  </si>
+  <si>
+    <t>c''</t>
+  </si>
+  <si>
+    <t>InCenter</t>
+  </si>
+  <si>
+    <t>CircumCenter</t>
+  </si>
+  <si>
+    <t>OrthoCenter</t>
+  </si>
+  <si>
+    <t>Centroid</t>
+  </si>
+  <si>
+    <t>a-Radians</t>
+  </si>
+  <si>
+    <t>b-Radians</t>
+  </si>
+  <si>
+    <t>c-Radians</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Outside</t>
+  </si>
+  <si>
+    <t>On vertex</t>
+  </si>
+  <si>
+    <t>Inside</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Right Isosceles</t>
+  </si>
+  <si>
+    <t>Isosceles</t>
+  </si>
+  <si>
+    <t>Right Triangle</t>
+  </si>
+  <si>
+    <t>Triangle 345</t>
+  </si>
+  <si>
+    <t>Triangle 306090</t>
+  </si>
+  <si>
+    <t>Equilateral Triangle</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,8 +521,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,8 +563,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -445,12 +596,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -475,9 +763,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,11 +813,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4982,7 +5372,7 @@
       <xdr:rowOff>148590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
       <xdr:row>102</xdr:row>
       <xdr:rowOff>148590</xdr:rowOff>
@@ -5018,7 +5408,7 @@
       <xdr:rowOff>148590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
       <xdr:row>118</xdr:row>
       <xdr:rowOff>148590</xdr:rowOff>
@@ -5056,7 +5446,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
       <xdr:row>136</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5094,7 +5484,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
       <xdr:row>155</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5132,7 +5522,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
       <xdr:row>174</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6111,24 +6501,24 @@
       </c>
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="24" t="s">
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="26"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="63"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -6957,14 +7347,14 @@
       </c>
     </row>
     <row r="37" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O37" s="22" t="s">
+      <c r="O37" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22" t="s">
+      <c r="P37" s="64"/>
+      <c r="Q37" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="R37" s="22"/>
+      <c r="R37" s="64"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
@@ -7682,22 +8072,22 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23" t="s">
+      <c r="B51" s="60"/>
+      <c r="C51" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="D51" s="23"/>
-      <c r="F51" s="23" t="s">
+      <c r="D51" s="60"/>
+      <c r="F51" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="G51" s="23"/>
-      <c r="H51" s="23" t="s">
+      <c r="G51" s="60"/>
+      <c r="H51" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="I51" s="23"/>
+      <c r="I51" s="60"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
@@ -8039,22 +8429,22 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="23" t="s">
+      <c r="A64" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="B64" s="23"/>
-      <c r="C64" s="23" t="s">
+      <c r="B64" s="60"/>
+      <c r="C64" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="D64" s="23"/>
-      <c r="F64" s="23" t="s">
+      <c r="D64" s="60"/>
+      <c r="F64" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="G64" s="23"/>
-      <c r="H64" s="23" t="s">
+      <c r="G64" s="60"/>
+      <c r="H64" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="I64" s="23"/>
+      <c r="I64" s="60"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
@@ -8396,26 +8786,26 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="23" t="s">
+      <c r="A77" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="B77" s="23"/>
-      <c r="C77" s="23" t="s">
+      <c r="B77" s="60"/>
+      <c r="C77" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="D77" s="23"/>
-      <c r="E77" s="23" t="s">
+      <c r="D77" s="60"/>
+      <c r="E77" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="F77" s="23"/>
-      <c r="H77" s="23" t="s">
+      <c r="F77" s="60"/>
+      <c r="H77" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="I77" s="23"/>
-      <c r="J77" s="23" t="s">
+      <c r="I77" s="60"/>
+      <c r="J77" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="K77" s="23"/>
+      <c r="K77" s="60"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
@@ -8813,6 +9203,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
     <mergeCell ref="J77:K77"/>
     <mergeCell ref="E77:F77"/>
     <mergeCell ref="H13:N13"/>
@@ -8825,11 +9220,6 @@
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="H77:I77"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8838,60 +9228,67 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AE85C4-CC88-430A-A443-610E34209E7B}">
-  <dimension ref="A2:Y177"/>
+  <dimension ref="A2:BE195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="I178" sqref="I178"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AK159" sqref="AK159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.88671875" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
     <col min="4" max="4" width="9.109375" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.77734375" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="33" max="34" width="12.44140625" customWidth="1"/>
+    <col min="35" max="36" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="E2" s="27" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="E2" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27" t="s">
+      <c r="F2" s="65"/>
+      <c r="G2" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="27"/>
+      <c r="H2" s="65"/>
       <c r="I2" t="s">
         <v>58</v>
       </c>
       <c r="L2" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="Q2" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" t="s">
+      <c r="R2" s="65"/>
+      <c r="S2" t="s">
         <v>59</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>66</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -8931,35 +9328,35 @@
       <c r="M3" t="s">
         <v>3</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>64</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>65</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>3</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
         <v>61</v>
       </c>
-      <c r="V3" t="s">
+      <c r="Y3" t="s">
         <v>60</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
         <v>62</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AB3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -9008,51 +9405,51 @@
         <f t="shared" ref="M4:M9" si="5">I4/K4</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N9" si="6">ATAN(M4/L4)</f>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q9" si="6">ATAN(M4/L4)</f>
         <v>0.78539816339744828</v>
       </c>
-      <c r="O4">
-        <f>DEGREES(N4)</f>
+      <c r="R4">
+        <f t="shared" ref="R4:R9" si="7">DEGREES(Q4)</f>
         <v>45</v>
       </c>
-      <c r="P4">
-        <f>L4*COS(-N9)-M4*SIN(-N9)</f>
+      <c r="S4">
+        <f>L4*COS(-Q9)-M4*SIN(-Q9)</f>
         <v>0</v>
       </c>
-      <c r="Q4">
-        <f>L4*SIN(-N9)+M4*COS(-N9)</f>
+      <c r="T4">
+        <f>L4*SIN(-Q9)+M4*COS(-Q9)</f>
         <v>-0.99999999999999989</v>
       </c>
-      <c r="R4" t="str">
-        <f t="shared" ref="R4:R9" si="7">IF(Q4&lt;0,"CW","CCW")</f>
+      <c r="U4" t="str">
+        <f t="shared" ref="U4:U9" si="8">IF(T4&lt;0,"CW","CCW")</f>
         <v>CW</v>
       </c>
-      <c r="S4" t="s">
+      <c r="V4" t="s">
         <v>67</v>
       </c>
-      <c r="U4">
+      <c r="X4">
         <f>K4*K5</f>
         <v>3.1112698372208096</v>
       </c>
-      <c r="V4">
+      <c r="Y4">
         <f>L4*L5+M4*M5</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="W4">
-        <f t="shared" ref="W4:W9" si="8">V4/U4</f>
+      <c r="Z4">
+        <f t="shared" ref="Z4:Z9" si="9">Y4/X4</f>
         <v>-0.22727272727272721</v>
       </c>
-      <c r="X4">
-        <f t="shared" ref="X4:X9" si="9">ACOS(W4)</f>
+      <c r="AA4">
+        <f t="shared" ref="AA4:AA9" si="10">ACOS(Z4)</f>
         <v>1.8000725300088765</v>
       </c>
-      <c r="Y4">
-        <f t="shared" ref="Y4:Y9" si="10">DEGREES(X4)</f>
+      <c r="AB4">
+        <f t="shared" ref="AB4:AB9" si="11">DEGREES(AA4)</f>
         <v>103.13655878694485</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -9101,51 +9498,51 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N5">
+      <c r="Q5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O5">
-        <f t="shared" ref="O5:O9" si="11">DEGREES(N5)</f>
+      <c r="R5">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P5">
-        <f>L5*COS(-N4)-M5*SIN(-N4)</f>
+      <c r="S5">
+        <f>L5*COS(-Q4)-M5*SIN(-Q4)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="Q5">
-        <f>L5*SIN(-N4)+M5*COS(-N4)</f>
+      <c r="T5">
+        <f>L5*SIN(-Q4)+M5*COS(-Q4)</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="R5" t="str">
-        <f t="shared" si="7"/>
+      <c r="U5" t="str">
+        <f t="shared" si="8"/>
         <v>CW</v>
       </c>
-      <c r="S5" t="s">
+      <c r="V5" t="s">
         <v>67</v>
       </c>
-      <c r="U5">
+      <c r="X5">
         <f>K5*K6</f>
         <v>3.1112698372208092</v>
       </c>
-      <c r="V5">
+      <c r="Y5">
         <f>L5*L6+M5*M6</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="W5">
-        <f t="shared" si="8"/>
+      <c r="Z5">
+        <f t="shared" si="9"/>
         <v>-0.22727272727272724</v>
       </c>
-      <c r="X5">
-        <f t="shared" si="9"/>
+      <c r="AA5">
+        <f t="shared" si="10"/>
         <v>1.8000725300088765</v>
       </c>
-      <c r="Y5">
-        <f t="shared" si="10"/>
+      <c r="AB5">
+        <f t="shared" si="11"/>
         <v>103.13655878694485</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -9194,51 +9591,51 @@
         <f t="shared" si="5"/>
         <v>0.70710678118654757</v>
       </c>
-      <c r="N6">
+      <c r="Q6">
         <f t="shared" si="6"/>
         <v>-0.78539816339744839</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="11"/>
+      <c r="R6">
+        <f t="shared" si="7"/>
         <v>-45.000000000000007</v>
       </c>
-      <c r="P6">
-        <f>L6*COS(-N5)-M6*SIN(-N5)</f>
+      <c r="S6">
+        <f>L6*COS(-Q5)-M6*SIN(-Q5)</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="Q6">
-        <f>L6*SIN(-N5)+M6*COS(-N5)</f>
+      <c r="T6">
+        <f>L6*SIN(-Q5)+M6*COS(-Q5)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="R6" t="str">
-        <f t="shared" si="7"/>
+      <c r="U6" t="str">
+        <f t="shared" si="8"/>
         <v>CCW</v>
       </c>
-      <c r="S6" t="s">
+      <c r="V6" t="s">
         <v>67</v>
       </c>
-      <c r="U6">
+      <c r="X6">
         <f>K6*K7</f>
         <v>1.9999999999999996</v>
       </c>
-      <c r="V6">
+      <c r="Y6">
         <f>L6*L7+M6*M7</f>
         <v>0</v>
       </c>
-      <c r="W6">
-        <f t="shared" si="8"/>
+      <c r="Z6">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="X6">
-        <f t="shared" si="9"/>
+      <c r="AA6">
+        <f t="shared" si="10"/>
         <v>1.5707963267948966</v>
       </c>
-      <c r="Y6">
-        <f t="shared" si="10"/>
+      <c r="AB6">
+        <f t="shared" si="11"/>
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -9287,51 +9684,51 @@
         <f t="shared" si="5"/>
         <v>0.70710678118654757</v>
       </c>
-      <c r="N7">
+      <c r="Q7">
         <f t="shared" si="6"/>
         <v>0.78539816339744839</v>
       </c>
-      <c r="O7">
-        <f t="shared" si="11"/>
+      <c r="R7">
+        <f t="shared" si="7"/>
         <v>45.000000000000007</v>
       </c>
-      <c r="P7">
-        <f>L7*COS(-N6)-M7*SIN(-N6)</f>
+      <c r="S7">
+        <f>L7*COS(-Q6)-M7*SIN(-Q6)</f>
         <v>0</v>
       </c>
-      <c r="Q7">
-        <f>L7*SIN(-N6)+M7*COS(-N6)</f>
-        <v>1</v>
-      </c>
-      <c r="R7" t="str">
-        <f t="shared" si="7"/>
+      <c r="T7">
+        <f>L7*SIN(-Q6)+M7*COS(-Q6)</f>
+        <v>1</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="8"/>
         <v>CCW</v>
       </c>
-      <c r="S7" t="s">
+      <c r="V7" t="s">
         <v>67</v>
       </c>
-      <c r="U7">
+      <c r="X7">
         <f>K7*K8</f>
         <v>3.1112698372208092</v>
       </c>
-      <c r="V7">
+      <c r="Y7">
         <f>L7*L8+M7*M8</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="W7">
-        <f t="shared" si="8"/>
+      <c r="Z7">
+        <f t="shared" si="9"/>
         <v>-0.22727272727272724</v>
       </c>
-      <c r="X7">
-        <f t="shared" si="9"/>
+      <c r="AA7">
+        <f t="shared" si="10"/>
         <v>1.8000725300088765</v>
       </c>
-      <c r="Y7">
-        <f t="shared" si="10"/>
+      <c r="AB7">
+        <f t="shared" si="11"/>
         <v>103.13655878694485</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -9380,51 +9777,51 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N8">
+      <c r="Q8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O8">
-        <f t="shared" si="11"/>
+      <c r="R8">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P8">
-        <f>L8*COS(-N7)-M8*SIN(-N7)</f>
+      <c r="S8">
+        <f>L8*COS(-Q7)-M8*SIN(-Q7)</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="Q8">
-        <f>L8*SIN(-N7)+M8*COS(-N7)</f>
+      <c r="T8">
+        <f>L8*SIN(-Q7)+M8*COS(-Q7)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="R8" t="str">
-        <f t="shared" si="7"/>
+      <c r="U8" t="str">
+        <f t="shared" si="8"/>
         <v>CCW</v>
       </c>
-      <c r="S8" t="s">
+      <c r="V8" t="s">
         <v>67</v>
       </c>
-      <c r="U8">
+      <c r="X8">
         <f>K8*K9</f>
         <v>3.1112698372208096</v>
       </c>
-      <c r="V8">
+      <c r="Y8">
         <f>L8*L9+M8*M9</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="W8">
-        <f t="shared" si="8"/>
+      <c r="Z8">
+        <f t="shared" si="9"/>
         <v>-0.22727272727272721</v>
       </c>
-      <c r="X8">
-        <f t="shared" si="9"/>
+      <c r="AA8">
+        <f t="shared" si="10"/>
         <v>1.8000725300088765</v>
       </c>
-      <c r="Y8">
-        <f t="shared" si="10"/>
+      <c r="AB8">
+        <f t="shared" si="11"/>
         <v>103.13655878694485</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -9473,51 +9870,51 @@
         <f t="shared" si="5"/>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="N9">
+      <c r="Q9">
         <f t="shared" si="6"/>
         <v>-0.78539816339744828</v>
       </c>
-      <c r="O9">
-        <f t="shared" si="11"/>
+      <c r="R9">
+        <f t="shared" si="7"/>
         <v>-45</v>
       </c>
-      <c r="P9">
-        <f>L9*COS(-N8)-M9*SIN(-N8)</f>
+      <c r="S9">
+        <f>L9*COS(-Q8)-M9*SIN(-Q8)</f>
         <v>0.70710678118654746</v>
       </c>
-      <c r="Q9">
-        <f>L9*SIN(-N8)+M9*COS(-N8)</f>
+      <c r="T9">
+        <f>L9*SIN(-Q8)+M9*COS(-Q8)</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="R9" t="str">
-        <f t="shared" si="7"/>
+      <c r="U9" t="str">
+        <f t="shared" si="8"/>
         <v>CW</v>
       </c>
-      <c r="S9" t="s">
+      <c r="V9" t="s">
         <v>67</v>
       </c>
-      <c r="U9">
+      <c r="X9">
         <f>K9*K4</f>
         <v>2.0000000000000004</v>
       </c>
-      <c r="V9">
+      <c r="Y9">
         <f>L9*L4+M9*M4</f>
         <v>0</v>
       </c>
-      <c r="W9">
-        <f t="shared" si="8"/>
+      <c r="Z9">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="X9">
-        <f t="shared" si="9"/>
+      <c r="AA9">
+        <f t="shared" si="10"/>
         <v>1.5707963267948966</v>
       </c>
-      <c r="Y9">
-        <f t="shared" si="10"/>
+      <c r="AB9">
+        <f t="shared" si="11"/>
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -9566,51 +9963,51 @@
         <f t="shared" ref="M11:M16" si="17">I11/K11</f>
         <v>0</v>
       </c>
-      <c r="N11">
-        <f t="shared" ref="N11:N16" si="18">ATAN(M11/L11)</f>
+      <c r="Q11">
+        <f t="shared" ref="Q11:Q16" si="18">ATAN(M11/L11)</f>
         <v>0</v>
       </c>
-      <c r="O11">
-        <f>DEGREES(N11)</f>
+      <c r="R11">
+        <f t="shared" ref="R11:R16" si="19">DEGREES(Q11)</f>
         <v>0</v>
       </c>
-      <c r="P11">
-        <f>L11*COS(-N16)-M11*SIN(-N16)</f>
+      <c r="S11">
+        <f>L11*COS(-Q16)-M11*SIN(-Q16)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="Q11">
-        <f>L11*SIN(-N16)+M11*COS(-N16)</f>
+      <c r="T11">
+        <f>L11*SIN(-Q16)+M11*COS(-Q16)</f>
         <v>0.70710678118654746</v>
       </c>
-      <c r="R11" t="str">
-        <f t="shared" ref="R11:R16" si="19">IF(Q11&lt;0,"CW","CCW")</f>
+      <c r="U11" t="str">
+        <f t="shared" ref="U11:U16" si="20">IF(T11&lt;0,"CW","CCW")</f>
         <v>CCW</v>
       </c>
-      <c r="S11" t="s">
+      <c r="V11" t="s">
         <v>68</v>
       </c>
-      <c r="U11">
+      <c r="X11">
         <f>K11*K12</f>
         <v>3.1112698372208092</v>
       </c>
-      <c r="V11">
+      <c r="Y11">
         <f>L11*L12+M11*M12</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="W11">
-        <f t="shared" ref="W11:W16" si="20">V11/U11</f>
+      <c r="Z11">
+        <f t="shared" ref="Z11:Z16" si="21">Y11/X11</f>
         <v>-0.22727272727272724</v>
       </c>
-      <c r="X11">
-        <f t="shared" ref="X11:X16" si="21">ACOS(W11)</f>
+      <c r="AA11">
+        <f t="shared" ref="AA11:AA16" si="22">ACOS(Z11)</f>
         <v>1.8000725300088765</v>
       </c>
-      <c r="Y11">
-        <f t="shared" ref="Y11:Y16" si="22">DEGREES(X11)</f>
+      <c r="AB11">
+        <f t="shared" ref="AB11:AB16" si="23">DEGREES(AA11)</f>
         <v>103.13655878694485</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -9659,51 +10056,51 @@
         <f t="shared" si="17"/>
         <v>-0.70710678118654757</v>
       </c>
-      <c r="N12">
+      <c r="Q12">
         <f t="shared" si="18"/>
         <v>0.78539816339744839</v>
       </c>
-      <c r="O12">
-        <f t="shared" ref="O12:O16" si="23">DEGREES(N12)</f>
+      <c r="R12">
+        <f t="shared" si="19"/>
         <v>45.000000000000007</v>
       </c>
-      <c r="P12">
-        <f>L12*COS(-N11)-M12*SIN(-N11)</f>
+      <c r="S12">
+        <f>L12*COS(-Q11)-M12*SIN(-Q11)</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="Q12">
-        <f>L12*SIN(-N11)+M12*COS(-N11)</f>
+      <c r="T12">
+        <f>L12*SIN(-Q11)+M12*COS(-Q11)</f>
         <v>-0.70710678118654757</v>
       </c>
-      <c r="R12" t="str">
-        <f t="shared" si="19"/>
+      <c r="U12" t="str">
+        <f t="shared" si="20"/>
         <v>CW</v>
       </c>
-      <c r="S12" t="s">
+      <c r="V12" t="s">
         <v>68</v>
       </c>
-      <c r="U12">
+      <c r="X12">
         <f>K12*K13</f>
         <v>1.9999999999999996</v>
       </c>
-      <c r="V12">
+      <c r="Y12">
         <f>L12*L13+M12*M13</f>
         <v>0</v>
       </c>
-      <c r="W12">
-        <f t="shared" si="20"/>
+      <c r="Z12">
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="X12">
-        <f t="shared" si="21"/>
+      <c r="AA12">
+        <f t="shared" si="22"/>
         <v>1.5707963267948966</v>
       </c>
-      <c r="Y12">
-        <f t="shared" si="22"/>
+      <c r="AB12">
+        <f t="shared" si="23"/>
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -9752,51 +10149,51 @@
         <f t="shared" si="17"/>
         <v>-0.70710678118654757</v>
       </c>
-      <c r="N13">
+      <c r="Q13">
         <f t="shared" si="18"/>
         <v>-0.78539816339744839</v>
       </c>
-      <c r="O13">
-        <f t="shared" si="23"/>
+      <c r="R13">
+        <f t="shared" si="19"/>
         <v>-45.000000000000007</v>
       </c>
-      <c r="P13">
-        <f>L13*COS(-N12)-M13*SIN(-N12)</f>
+      <c r="S13">
+        <f>L13*COS(-Q12)-M13*SIN(-Q12)</f>
         <v>0</v>
       </c>
-      <c r="Q13">
-        <f>L13*SIN(-N12)+M13*COS(-N12)</f>
+      <c r="T13">
+        <f>L13*SIN(-Q12)+M13*COS(-Q12)</f>
         <v>-1</v>
       </c>
-      <c r="R13" t="str">
-        <f t="shared" si="19"/>
+      <c r="U13" t="str">
+        <f t="shared" si="20"/>
         <v>CW</v>
       </c>
-      <c r="S13" t="s">
+      <c r="V13" t="s">
         <v>68</v>
       </c>
-      <c r="U13">
+      <c r="X13">
         <f>K13*K14</f>
         <v>3.1112698372208092</v>
       </c>
-      <c r="V13">
+      <c r="Y13">
         <f>L13*L14+M13*M14</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="W13">
-        <f t="shared" si="20"/>
+      <c r="Z13">
+        <f t="shared" si="21"/>
         <v>-0.22727272727272724</v>
       </c>
-      <c r="X13">
-        <f t="shared" si="21"/>
+      <c r="AA13">
+        <f t="shared" si="22"/>
         <v>1.8000725300088765</v>
       </c>
-      <c r="Y13">
-        <f t="shared" si="22"/>
+      <c r="AB13">
+        <f t="shared" si="23"/>
         <v>103.13655878694485</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -9845,51 +10242,51 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="N14">
+      <c r="Q14">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="O14">
-        <f t="shared" si="23"/>
+      <c r="R14">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P14">
-        <f>L14*COS(-N13)-M14*SIN(-N13)</f>
+      <c r="S14">
+        <f>L14*COS(-Q13)-M14*SIN(-Q13)</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="Q14">
-        <f>L14*SIN(-N13)+M14*COS(-N13)</f>
+      <c r="T14">
+        <f>L14*SIN(-Q13)+M14*COS(-Q13)</f>
         <v>-0.70710678118654757</v>
       </c>
-      <c r="R14" t="str">
-        <f t="shared" si="19"/>
+      <c r="U14" t="str">
+        <f t="shared" si="20"/>
         <v>CW</v>
       </c>
-      <c r="S14" t="s">
+      <c r="V14" t="s">
         <v>68</v>
       </c>
-      <c r="U14">
+      <c r="X14">
         <f>K14*K15</f>
         <v>3.1112698372208096</v>
       </c>
-      <c r="V14">
+      <c r="Y14">
         <f>L14*L15+M14*M15</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="W14">
-        <f t="shared" si="20"/>
+      <c r="Z14">
+        <f t="shared" si="21"/>
         <v>-0.22727272727272721</v>
       </c>
-      <c r="X14">
-        <f t="shared" si="21"/>
+      <c r="AA14">
+        <f t="shared" si="22"/>
         <v>1.8000725300088765</v>
       </c>
-      <c r="Y14">
-        <f t="shared" si="22"/>
+      <c r="AB14">
+        <f t="shared" si="23"/>
         <v>103.13655878694485</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -9938,51 +10335,51 @@
         <f t="shared" si="17"/>
         <v>0.70710678118654746</v>
       </c>
-      <c r="N15">
+      <c r="Q15">
         <f t="shared" si="18"/>
         <v>0.78539816339744828</v>
       </c>
-      <c r="O15">
-        <f t="shared" si="23"/>
+      <c r="R15">
+        <f t="shared" si="19"/>
         <v>45</v>
       </c>
-      <c r="P15">
-        <f>L15*COS(-N14)-M15*SIN(-N14)</f>
+      <c r="S15">
+        <f>L15*COS(-Q14)-M15*SIN(-Q14)</f>
         <v>0.70710678118654746</v>
       </c>
-      <c r="Q15">
-        <f>L15*SIN(-N14)+M15*COS(-N14)</f>
+      <c r="T15">
+        <f>L15*SIN(-Q14)+M15*COS(-Q14)</f>
         <v>0.70710678118654746</v>
       </c>
-      <c r="R15" t="str">
-        <f t="shared" si="19"/>
+      <c r="U15" t="str">
+        <f t="shared" si="20"/>
         <v>CCW</v>
       </c>
-      <c r="S15" t="s">
+      <c r="V15" t="s">
         <v>68</v>
       </c>
-      <c r="U15">
+      <c r="X15">
         <f>K15*K16</f>
         <v>2.0000000000000004</v>
       </c>
-      <c r="V15">
+      <c r="Y15">
         <f>L15*L16+M15*M16</f>
         <v>0</v>
       </c>
-      <c r="W15">
-        <f t="shared" si="20"/>
+      <c r="Z15">
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="X15">
-        <f t="shared" si="21"/>
+      <c r="AA15">
+        <f t="shared" si="22"/>
         <v>1.5707963267948966</v>
       </c>
-      <c r="Y15">
-        <f t="shared" si="22"/>
+      <c r="AB15">
+        <f t="shared" si="23"/>
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -10031,47 +10428,47 @@
         <f t="shared" si="17"/>
         <v>0.70710678118654746</v>
       </c>
-      <c r="N16">
+      <c r="Q16">
         <f t="shared" si="18"/>
         <v>-0.78539816339744828</v>
       </c>
-      <c r="O16">
-        <f t="shared" si="23"/>
+      <c r="R16">
+        <f t="shared" si="19"/>
         <v>-45</v>
       </c>
-      <c r="P16">
-        <f>L16*COS(-N15)-M16*SIN(-N15)</f>
+      <c r="S16">
+        <f>L16*COS(-Q15)-M16*SIN(-Q15)</f>
         <v>0</v>
       </c>
-      <c r="Q16">
-        <f>L16*SIN(-N15)+M16*COS(-N15)</f>
+      <c r="T16">
+        <f>L16*SIN(-Q15)+M16*COS(-Q15)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="R16" t="str">
-        <f t="shared" si="19"/>
+      <c r="U16" t="str">
+        <f t="shared" si="20"/>
         <v>CCW</v>
       </c>
-      <c r="S16" t="s">
+      <c r="V16" t="s">
         <v>68</v>
       </c>
-      <c r="U16">
+      <c r="X16">
         <f>K16*K11</f>
         <v>3.1112698372208096</v>
       </c>
-      <c r="V16">
+      <c r="Y16">
         <f>L16*L11+M16*M11</f>
         <v>-0.70710678118654746</v>
       </c>
-      <c r="W16">
-        <f t="shared" si="20"/>
+      <c r="Z16">
+        <f t="shared" si="21"/>
         <v>-0.22727272727272721</v>
       </c>
-      <c r="X16">
-        <f t="shared" si="21"/>
+      <c r="AA16">
+        <f t="shared" si="22"/>
         <v>1.8000725300088765</v>
       </c>
-      <c r="Y16">
-        <f t="shared" si="22"/>
+      <c r="AB16">
+        <f t="shared" si="23"/>
         <v>103.13655878694485</v>
       </c>
     </row>
@@ -10186,7 +10583,7 @@
       <c r="A30" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="22">
         <f>B28/2</f>
         <v>5</v>
       </c>
@@ -10438,7 +10835,7 @@
       <c r="A54" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="28">
+      <c r="B54" s="22">
         <f>B53</f>
         <v>10</v>
       </c>
@@ -10485,7 +10882,7 @@
       <c r="A61" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="29">
+      <c r="B61" s="23">
         <f>0.5*(B59-B58)</f>
         <v>1</v>
       </c>
@@ -10580,7 +10977,7 @@
       <c r="A70" t="s">
         <v>84</v>
       </c>
-      <c r="B70" s="28">
+      <c r="B70" s="22">
         <f>B69</f>
         <v>10</v>
       </c>
@@ -10597,7 +10994,7 @@
       <c r="A72" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="29">
+      <c r="B72" s="23">
         <f>0.5*(B70-B69)</f>
         <v>0</v>
       </c>
@@ -10683,7 +11080,7 @@
       <c r="A80" t="s">
         <v>84</v>
       </c>
-      <c r="B80" s="28">
+      <c r="B80" s="22">
         <f>B79</f>
         <v>10</v>
       </c>
@@ -10692,7 +11089,7 @@
       <c r="A81" t="s">
         <v>71</v>
       </c>
-      <c r="B81" s="28">
+      <c r="B81" s="22">
         <f>B79</f>
         <v>10</v>
       </c>
@@ -10701,7 +11098,7 @@
       <c r="A82" t="s">
         <v>72</v>
       </c>
-      <c r="B82" s="29">
+      <c r="B82" s="23">
         <f>0.5*(B80-B79)</f>
         <v>0</v>
       </c>
@@ -10889,7 +11286,7 @@
         <v>1</v>
       </c>
       <c r="E97">
-        <f t="shared" ref="E97:E99" si="24">(D97/$B$89)*2*PI()</f>
+        <f>(D97/$B$89)*2*PI()</f>
         <v>1.2566370614359172</v>
       </c>
       <c r="F97">
@@ -10897,7 +11294,7 @@
         <v>3.0901699437494745</v>
       </c>
       <c r="G97">
-        <f t="shared" ref="G97:G100" si="25">$B$90*SIN(E97)</f>
+        <f>$B$90*SIN(E97)</f>
         <v>9.5105651629515346</v>
       </c>
     </row>
@@ -10906,15 +11303,15 @@
         <v>2</v>
       </c>
       <c r="E98">
-        <f t="shared" si="24"/>
+        <f>(D98/$B$89)*2*PI()</f>
         <v>2.5132741228718345</v>
       </c>
       <c r="F98">
-        <f t="shared" ref="F98:F100" si="26">$B$90*COS(E98)</f>
+        <f>$B$90*COS(E98)</f>
         <v>-8.0901699437494727</v>
       </c>
       <c r="G98">
-        <f t="shared" si="25"/>
+        <f>$B$90*SIN(E98)</f>
         <v>5.8778525229247327</v>
       </c>
     </row>
@@ -10923,15 +11320,15 @@
         <v>3</v>
       </c>
       <c r="E99">
-        <f t="shared" si="24"/>
+        <f>(D99/$B$89)*2*PI()</f>
         <v>3.7699111843077517</v>
       </c>
       <c r="F99">
-        <f t="shared" si="26"/>
+        <f>$B$90*COS(E99)</f>
         <v>-8.0901699437494763</v>
       </c>
       <c r="G99">
-        <f t="shared" si="25"/>
+        <f>$B$90*SIN(E99)</f>
         <v>-5.87785252292473</v>
       </c>
     </row>
@@ -10944,11 +11341,11 @@
         <v>5.026548245743669</v>
       </c>
       <c r="F100">
-        <f t="shared" si="26"/>
+        <f>$B$90*COS(E100)</f>
         <v>3.0901699437494723</v>
       </c>
       <c r="G100">
-        <f t="shared" si="25"/>
+        <f>$B$90*SIN(E100)</f>
         <v>-9.5105651629515364</v>
       </c>
     </row>
@@ -11074,15 +11471,15 @@
         <v>1</v>
       </c>
       <c r="E113">
-        <f t="shared" ref="E113:E116" si="27">(D113/$B$105)*2*PI()</f>
+        <f>(D113/$B$105)*2*PI()</f>
         <v>1.2566370614359172</v>
       </c>
       <c r="F113">
-        <f t="shared" ref="F113:F116" si="28">$B$106*COS(E113)</f>
+        <f>$B$106*COS(E113)</f>
         <v>3.0901699437494745</v>
       </c>
       <c r="G113">
-        <f t="shared" ref="G113:G116" si="29">$B$106*SIN(E113)</f>
+        <f>$B$106*SIN(E113)</f>
         <v>9.5105651629515346</v>
       </c>
     </row>
@@ -11091,15 +11488,15 @@
         <v>2</v>
       </c>
       <c r="E114">
-        <f t="shared" si="27"/>
+        <f>(D114/$B$105)*2*PI()</f>
         <v>2.5132741228718345</v>
       </c>
       <c r="F114">
-        <f t="shared" si="28"/>
+        <f>$B$106*COS(E114)</f>
         <v>-8.0901699437494727</v>
       </c>
       <c r="G114">
-        <f t="shared" si="29"/>
+        <f>$B$106*SIN(E114)</f>
         <v>5.8778525229247327</v>
       </c>
     </row>
@@ -11108,15 +11505,15 @@
         <v>3</v>
       </c>
       <c r="E115">
-        <f t="shared" si="27"/>
+        <f>(D115/$B$105)*2*PI()</f>
         <v>3.7699111843077517</v>
       </c>
       <c r="F115">
-        <f t="shared" si="28"/>
+        <f>$B$106*COS(E115)</f>
         <v>-8.0901699437494763</v>
       </c>
       <c r="G115">
-        <f t="shared" si="29"/>
+        <f>$B$106*SIN(E115)</f>
         <v>-5.87785252292473</v>
       </c>
     </row>
@@ -11125,15 +11522,15 @@
         <v>4</v>
       </c>
       <c r="E116">
-        <f t="shared" si="27"/>
+        <f>(D116/$B$105)*2*PI()</f>
         <v>5.026548245743669</v>
       </c>
       <c r="F116">
-        <f t="shared" si="28"/>
+        <f>$B$106*COS(E116)</f>
         <v>3.0901699437494723</v>
       </c>
       <c r="G116">
-        <f t="shared" si="29"/>
+        <f>$B$106*SIN(E116)</f>
         <v>-9.5105651629515364</v>
       </c>
     </row>
@@ -11242,15 +11639,15 @@
         <v>0</v>
       </c>
       <c r="E129">
-        <f>(D129/$B$122)*2*PI()</f>
+        <f t="shared" ref="E129:E134" si="24">(D129/$B$122)*2*PI()</f>
         <v>0</v>
       </c>
       <c r="F129">
-        <f>$B$123*COS(E129)</f>
+        <f t="shared" ref="F129:F134" si="25">$B$123*COS(E129)</f>
         <v>10</v>
       </c>
       <c r="G129">
-        <f>$B$123*SIN(E129)</f>
+        <f t="shared" ref="G129:G134" si="26">$B$123*SIN(E129)</f>
         <v>0</v>
       </c>
     </row>
@@ -11259,15 +11656,15 @@
         <v>1</v>
       </c>
       <c r="E130">
-        <f t="shared" ref="E130:E134" si="30">(D130/$B$122)*2*PI()</f>
+        <f t="shared" si="24"/>
         <v>1.0471975511965976</v>
       </c>
       <c r="F130">
-        <f t="shared" ref="F130:F134" si="31">$B$123*COS(E130)</f>
+        <f t="shared" si="25"/>
         <v>5.0000000000000009</v>
       </c>
       <c r="G130">
-        <f t="shared" ref="G130:G134" si="32">$B$123*SIN(E130)</f>
+        <f t="shared" si="26"/>
         <v>8.6602540378443855</v>
       </c>
     </row>
@@ -11276,15 +11673,15 @@
         <v>2</v>
       </c>
       <c r="E131">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>2.0943951023931953</v>
       </c>
       <c r="F131">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>-4.9999999999999982</v>
       </c>
       <c r="G131">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>8.6602540378443873</v>
       </c>
     </row>
@@ -11293,15 +11690,15 @@
         <v>3</v>
       </c>
       <c r="E132">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>3.1415926535897931</v>
       </c>
       <c r="F132">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>-10</v>
       </c>
       <c r="G132">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>1.22514845490862E-15</v>
       </c>
     </row>
@@ -11310,15 +11707,15 @@
         <v>4</v>
       </c>
       <c r="E133">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>4.1887902047863905</v>
       </c>
       <c r="F133">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>-5.0000000000000044</v>
       </c>
       <c r="G133">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>-8.6602540378443837</v>
       </c>
     </row>
@@ -11327,15 +11724,15 @@
         <v>5</v>
       </c>
       <c r="E134">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>5.2359877559829888</v>
       </c>
       <c r="F134">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>5.0000000000000009</v>
       </c>
       <c r="G134">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>-8.6602540378443855</v>
       </c>
     </row>
@@ -11461,15 +11858,15 @@
         <v>1</v>
       </c>
       <c r="E148">
-        <f t="shared" ref="E148:E154" si="33">(D148/$B$140)*2*PI()</f>
+        <f t="shared" ref="E148:E154" si="27">(D148/$B$140)*2*PI()</f>
         <v>0.78539816339744828</v>
       </c>
       <c r="F148">
-        <f t="shared" ref="F148:F154" si="34">$B$141*COS(E148)</f>
+        <f t="shared" ref="F148:F154" si="28">$B$141*COS(E148)</f>
         <v>7.0710678118654755</v>
       </c>
       <c r="G148">
-        <f t="shared" ref="G148:G154" si="35">$B$141*SIN(E148)</f>
+        <f t="shared" ref="G148:G154" si="29">$B$141*SIN(E148)</f>
         <v>7.0710678118654746</v>
       </c>
     </row>
@@ -11478,15 +11875,15 @@
         <v>2</v>
       </c>
       <c r="E149">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="F149">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>6.1257422745431001E-16</v>
       </c>
       <c r="G149">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>10</v>
       </c>
     </row>
@@ -11495,15 +11892,15 @@
         <v>3</v>
       </c>
       <c r="E150">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>2.3561944901923448</v>
       </c>
       <c r="F150">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>-7.0710678118654746</v>
       </c>
       <c r="G150">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>7.0710678118654755</v>
       </c>
     </row>
@@ -11512,15 +11909,15 @@
         <v>4</v>
       </c>
       <c r="E151">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>3.1415926535897931</v>
       </c>
       <c r="F151">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>-10</v>
       </c>
       <c r="G151">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>1.22514845490862E-15</v>
       </c>
     </row>
@@ -11529,15 +11926,15 @@
         <v>5</v>
       </c>
       <c r="E152">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>3.9269908169872414</v>
       </c>
       <c r="F152">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>-7.0710678118654773</v>
       </c>
       <c r="G152">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>-7.0710678118654746</v>
       </c>
     </row>
@@ -11546,15 +11943,15 @@
         <v>6</v>
       </c>
       <c r="E153">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>4.7123889803846897</v>
       </c>
       <c r="F153">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>-1.83772268236293E-15</v>
       </c>
       <c r="G153">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>-10</v>
       </c>
     </row>
@@ -11563,15 +11960,15 @@
         <v>7</v>
       </c>
       <c r="E154">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>5.497787143782138</v>
       </c>
       <c r="F154">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>7.0710678118654737</v>
       </c>
       <c r="G154">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>-7.0710678118654773</v>
       </c>
     </row>
@@ -11697,15 +12094,15 @@
         <v>1</v>
       </c>
       <c r="E168">
-        <f t="shared" ref="E168:E176" si="36">(D168/$B$160)*2*PI()</f>
+        <f t="shared" ref="E168:E176" si="30">(D168/$B$160)*2*PI()</f>
         <v>0.62831853071795862</v>
       </c>
       <c r="F168">
-        <f t="shared" ref="F168:F176" si="37">$B$161*COS(E168)</f>
+        <f t="shared" ref="F168:F176" si="31">$B$161*COS(E168)</f>
         <v>8.0901699437494745</v>
       </c>
       <c r="G168">
-        <f t="shared" ref="G168:G176" si="38">$B$161*SIN(E168)</f>
+        <f t="shared" ref="G168:G176" si="32">$B$161*SIN(E168)</f>
         <v>5.8778525229247318</v>
       </c>
     </row>
@@ -11714,15 +12111,15 @@
         <v>2</v>
       </c>
       <c r="E169">
-        <f t="shared" si="36"/>
+        <f t="shared" si="30"/>
         <v>1.2566370614359172</v>
       </c>
       <c r="F169">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>3.0901699437494745</v>
       </c>
       <c r="G169">
-        <f t="shared" si="38"/>
+        <f t="shared" si="32"/>
         <v>9.5105651629515346</v>
       </c>
     </row>
@@ -11731,15 +12128,15 @@
         <v>3</v>
       </c>
       <c r="E170">
-        <f t="shared" si="36"/>
+        <f t="shared" si="30"/>
         <v>1.8849555921538759</v>
       </c>
       <c r="F170">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>-3.0901699437494736</v>
       </c>
       <c r="G170">
-        <f t="shared" si="38"/>
+        <f t="shared" si="32"/>
         <v>9.5105651629515364</v>
       </c>
     </row>
@@ -11748,15 +12145,15 @@
         <v>4</v>
       </c>
       <c r="E171">
-        <f t="shared" si="36"/>
+        <f t="shared" si="30"/>
         <v>2.5132741228718345</v>
       </c>
       <c r="F171">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>-8.0901699437494727</v>
       </c>
       <c r="G171">
-        <f t="shared" si="38"/>
+        <f t="shared" si="32"/>
         <v>5.8778525229247327</v>
       </c>
     </row>
@@ -11765,15 +12162,15 @@
         <v>5</v>
       </c>
       <c r="E172">
-        <f t="shared" si="36"/>
+        <f t="shared" si="30"/>
         <v>3.1415926535897931</v>
       </c>
       <c r="F172">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>-10</v>
       </c>
       <c r="G172">
-        <f t="shared" si="38"/>
+        <f t="shared" si="32"/>
         <v>1.22514845490862E-15</v>
       </c>
     </row>
@@ -11782,15 +12179,15 @@
         <v>6</v>
       </c>
       <c r="E173">
-        <f t="shared" si="36"/>
+        <f t="shared" si="30"/>
         <v>3.7699111843077517</v>
       </c>
       <c r="F173">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>-8.0901699437494763</v>
       </c>
       <c r="G173">
-        <f t="shared" si="38"/>
+        <f t="shared" si="32"/>
         <v>-5.87785252292473</v>
       </c>
     </row>
@@ -11799,15 +12196,15 @@
         <v>7</v>
       </c>
       <c r="E174">
-        <f t="shared" si="36"/>
+        <f t="shared" si="30"/>
         <v>4.3982297150257104</v>
       </c>
       <c r="F174">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>-3.0901699437494754</v>
       </c>
       <c r="G174">
-        <f t="shared" si="38"/>
+        <f t="shared" si="32"/>
         <v>-9.5105651629515346</v>
       </c>
     </row>
@@ -11816,15 +12213,15 @@
         <v>8</v>
       </c>
       <c r="E175">
-        <f t="shared" si="36"/>
+        <f t="shared" si="30"/>
         <v>5.026548245743669</v>
       </c>
       <c r="F175">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>3.0901699437494723</v>
       </c>
       <c r="G175">
-        <f t="shared" si="38"/>
+        <f t="shared" si="32"/>
         <v>-9.5105651629515364</v>
       </c>
     </row>
@@ -11833,19 +12230,19 @@
         <v>9</v>
       </c>
       <c r="E176">
-        <f t="shared" si="36"/>
+        <f t="shared" si="30"/>
         <v>5.6548667764616276</v>
       </c>
       <c r="F176">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>8.0901699437494727</v>
       </c>
       <c r="G176">
-        <f t="shared" si="38"/>
+        <f t="shared" si="32"/>
         <v>-5.8778525229247336</v>
       </c>
     </row>
-    <row r="177" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:57" x14ac:dyDescent="0.3">
       <c r="F177">
         <f>F167</f>
         <v>10</v>
@@ -11855,11 +12252,2595 @@
         <v>0</v>
       </c>
     </row>
+    <row r="179" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="180" spans="1:57" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C180" s="60"/>
+      <c r="D180" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="E180" s="60"/>
+      <c r="F180" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="G180" s="60"/>
+      <c r="H180" s="111" t="s">
+        <v>111</v>
+      </c>
+      <c r="I180" s="112"/>
+      <c r="J180" s="113"/>
+      <c r="K180" s="111" t="s">
+        <v>63</v>
+      </c>
+      <c r="L180" s="112"/>
+      <c r="M180" s="112"/>
+      <c r="N180" s="112"/>
+      <c r="O180" s="112"/>
+      <c r="P180" s="113"/>
+      <c r="Q180" s="111" t="s">
+        <v>115</v>
+      </c>
+      <c r="R180" s="112"/>
+      <c r="S180" s="113"/>
+      <c r="U180" s="111" t="s">
+        <v>116</v>
+      </c>
+      <c r="V180" s="112"/>
+      <c r="W180" s="113"/>
+      <c r="X180" s="111" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y180" s="112"/>
+      <c r="Z180" s="113"/>
+      <c r="AA180" s="111" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB180" s="112"/>
+      <c r="AC180" s="112"/>
+      <c r="AD180" s="112"/>
+      <c r="AE180" s="112"/>
+      <c r="AF180" s="112"/>
+      <c r="AG180" s="112"/>
+      <c r="AH180" s="112"/>
+      <c r="AI180" s="113"/>
+      <c r="AN180" s="114"/>
+      <c r="AP180" s="112" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ180" s="112"/>
+      <c r="AR180" s="114"/>
+      <c r="AT180" s="112" t="s">
+        <v>129</v>
+      </c>
+      <c r="AU180" s="112"/>
+      <c r="AV180" s="113"/>
+      <c r="AW180" s="111" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX180" s="112"/>
+      <c r="AY180" s="115"/>
+      <c r="AZ180" s="111" t="s">
+        <v>131</v>
+      </c>
+      <c r="BA180" s="113"/>
+    </row>
+    <row r="181" spans="1:57" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B181" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D181" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E181" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F181" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G181" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H181" s="116" t="s">
+        <v>77</v>
+      </c>
+      <c r="I181" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J181" s="117" t="s">
+        <v>110</v>
+      </c>
+      <c r="K181" s="116" t="s">
+        <v>77</v>
+      </c>
+      <c r="L181" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M181" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N181" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="O181" s="119" t="s">
+        <v>133</v>
+      </c>
+      <c r="P181" s="119" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q181" s="116" t="s">
+        <v>77</v>
+      </c>
+      <c r="R181" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="S181" s="117" t="s">
+        <v>110</v>
+      </c>
+      <c r="T181" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="U181" s="116" t="s">
+        <v>77</v>
+      </c>
+      <c r="V181" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="W181" s="117" t="s">
+        <v>110</v>
+      </c>
+      <c r="X181" s="116" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y181" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z181" s="117" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA181" s="116" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB181" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC181" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD181" s="120" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE181" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF181" s="121" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG181" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH181" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI181" s="117" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ181" s="119" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK181" s="119" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL181" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN181" s="114" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP181" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ181" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR181" s="114" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT181" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AU181" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV181" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW181" s="116" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX181" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY181" s="122" t="s">
+        <v>135</v>
+      </c>
+      <c r="AZ181" s="116" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA181" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC181" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD181" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="182" spans="1:57" s="42" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B182" s="43">
+        <v>1</v>
+      </c>
+      <c r="C182" s="43">
+        <v>2</v>
+      </c>
+      <c r="D182" s="43">
+        <v>3</v>
+      </c>
+      <c r="E182" s="43">
+        <v>4</v>
+      </c>
+      <c r="F182" s="43">
+        <v>-1</v>
+      </c>
+      <c r="G182" s="43">
+        <v>1</v>
+      </c>
+      <c r="H182" s="68">
+        <f>SQRT((B182-D182)^2+(C182-E182)^2)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="I182" s="104">
+        <f>SQRT((F182-D182)^2+(G182-E182)^2)</f>
+        <v>5</v>
+      </c>
+      <c r="J182" s="67">
+        <f>SQRT((F182-B182)^2+(G182-C182)^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="K182" s="105">
+        <f>DEGREES(ACOS((I182^2+J182^2-H182^2)/(2*I182*J182)))</f>
+        <v>10.304846468766035</v>
+      </c>
+      <c r="L182" s="106">
+        <f>DEGREES(ACOS((J182^2+H182^2-I182^2)/(2*J182*H182)))</f>
+        <v>161.56505117707795</v>
+      </c>
+      <c r="M182" s="106">
+        <f>DEGREES(ACOS((I182^2+H182^2-J182^2)/(2*I182*H182)))</f>
+        <v>8.1301023541559978</v>
+      </c>
+      <c r="N182" s="107">
+        <f>RADIANS(K182)</f>
+        <v>0.17985349979247833</v>
+      </c>
+      <c r="O182" s="106">
+        <f>RADIANS(L182)</f>
+        <v>2.8198420991931501</v>
+      </c>
+      <c r="P182" s="108">
+        <f>RADIANS(M182)</f>
+        <v>0.14189705460416424</v>
+      </c>
+      <c r="Q182" s="109">
+        <f>2*$AL182/H182</f>
+        <v>0.70710678118654657</v>
+      </c>
+      <c r="R182" s="104">
+        <f>2*$AL182/I182</f>
+        <v>0.39999999999999952</v>
+      </c>
+      <c r="S182" s="110">
+        <f>2*$AL182/J182</f>
+        <v>0.89442719099991475</v>
+      </c>
+      <c r="T182" s="51"/>
+      <c r="U182" s="44">
+        <f>0.5*SQRT(2*J182^2+2*I182^2-H182^2)</f>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="V182" s="51">
+        <f>0.5*SQRT(2*J182^2+2*H182^2-I182^2)</f>
+        <v>0.50000000000000178</v>
+      </c>
+      <c r="W182" s="47">
+        <f>0.5*SQRT(2*I182^2+2*H182^2-J182^2)</f>
+        <v>3.905124837953327</v>
+      </c>
+      <c r="X182" s="44">
+        <f>SQRT(J182*I182*(1-H182^2/(J182+I182)^2))</f>
+        <v>3.0776835371752536</v>
+      </c>
+      <c r="Y182" s="46">
+        <f>SQRT(J182*H182*(1-I182^2/(J182+H182)^2))</f>
+        <v>0.40007204539852875</v>
+      </c>
+      <c r="Z182" s="47">
+        <f>SQRT(I182*H182*(1-J182^2/(I182+H182)^2))</f>
+        <v>3.6039313488571842</v>
+      </c>
+      <c r="AA182" s="44">
+        <f>MAX(H182:J182)</f>
+        <v>5</v>
+      </c>
+      <c r="AB182" s="42">
+        <f>IF(RANK(I182,$H182:$J182)+COUNTIF($H182:I182,I182)-1=2,I182,IF(RANK(J182,$H182:$J182)+COUNTIF($H182:J182,J182)-1=2,J182,H182))</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="AC182" s="46">
+        <f>MIN(H182:J182)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AD182" s="48">
+        <f>2*AA182*$AL182/($AA182^2+$AB182^2-$AC182^2)</f>
+        <v>0.35714285714285671</v>
+      </c>
+      <c r="AE182" s="42">
+        <f>2*AB182*$AL182/($AA182^2+$AB182^2-$AC182^2)</f>
+        <v>0.20203050891044191</v>
+      </c>
+      <c r="AF182" s="49">
+        <f>2*AC182*$AL182/($AA182^2-$AB182^2+$AC182^2)</f>
+        <v>0.20327890704543519</v>
+      </c>
+      <c r="AG182" s="42">
+        <f>INDEX($AD182:$AF182,1,MATCH(H182,$AA182:$AC182,0))</f>
+        <v>0.20203050891044191</v>
+      </c>
+      <c r="AH182" s="42">
+        <f>INDEX($AD182:$AF182,1,MATCH(I182,$AA182:$AC182,0))</f>
+        <v>0.35714285714285671</v>
+      </c>
+      <c r="AI182" s="45">
+        <f>INDEX($AD182:$AF182,1,MATCH(J182,$AA182:$AC182,0))</f>
+        <v>0.20327890704543519</v>
+      </c>
+      <c r="AJ182" s="50">
+        <f>I182+J182+H182</f>
+        <v>10.06449510224598</v>
+      </c>
+      <c r="AK182" s="50">
+        <f>AJ182/2</f>
+        <v>5.0322475511229898</v>
+      </c>
+      <c r="AL182" s="51">
+        <f>SQRT(AK182*(AK182-I182)*(AK182-J182)*(AK182-H182))</f>
+        <v>0.99999999999999878</v>
+      </c>
+      <c r="AN182" s="52">
+        <f>AL182/AK182</f>
+        <v>0.19871836388033814</v>
+      </c>
+      <c r="AP182" s="58">
+        <f>($I182*B182+$J182*D182+$H182*F182)/$AJ182</f>
+        <v>0.88228735942964298</v>
+      </c>
+      <c r="AQ182" s="58">
+        <f>($I182*C182+$J182*E182+$H182*G182)/$AJ182</f>
+        <v>2.1633175647218095</v>
+      </c>
+      <c r="AR182" s="52">
+        <f>I182*J182*H182/(4*AL182)</f>
+        <v>7.9056941504209588</v>
+      </c>
+      <c r="AT182" s="42">
+        <f>2*(B182*(E182-G182)+D182*(G182-C182)+F182*(C182-E182))</f>
+        <v>4</v>
+      </c>
+      <c r="AU182" s="42">
+        <f>((B182^2+C182^2)*(E182-G182)+(D182^2+E182^2)*(G182-C182)+(F182^2+G182^2)*(C182-E182))/AT182</f>
+        <v>-3.5</v>
+      </c>
+      <c r="AV182" s="45">
+        <f>-((B182^2+C182^2)*(D182-F182)+(D182^2+E182^2)*(F182-B182)+(F182^2+G182^2)*(B182-D182))/AT182</f>
+        <v>8.5</v>
+      </c>
+      <c r="AW182" s="53">
+        <f>(B182*TAN($O182)+D182*TAN($P182)+F182*TAN($N182))/(TAN($O182)+TAN($P182)+TAN($N182))</f>
+        <v>9.9999999999992628</v>
+      </c>
+      <c r="AX182" s="42">
+        <f>(C182*TAN($O182)+E182*TAN($P182)+G182*TAN($N182))/(TAN($O182)+TAN($P182)+TAN($N182))</f>
+        <v>-9.9999999999991669</v>
+      </c>
+      <c r="AY182" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ182" s="53">
+        <f>(B182+D182+F182)/3</f>
+        <v>1</v>
+      </c>
+      <c r="BA182" s="45">
+        <f>(C182+E182+G182)/3</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="BB182" s="42" t="str">
+        <f>A182</f>
+        <v>Random</v>
+      </c>
+    </row>
+    <row r="183" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>119</v>
+      </c>
+      <c r="B183" s="5">
+        <v>1</v>
+      </c>
+      <c r="C183" s="5">
+        <v>2</v>
+      </c>
+      <c r="D183" s="5">
+        <v>4</v>
+      </c>
+      <c r="E183" s="5">
+        <v>2</v>
+      </c>
+      <c r="F183" s="5">
+        <v>4</v>
+      </c>
+      <c r="G183" s="5">
+        <v>5</v>
+      </c>
+      <c r="H183" s="59">
+        <f>SQRT((B183-D183)^2+(C183-E183)^2)</f>
+        <v>3</v>
+      </c>
+      <c r="I183" s="11">
+        <f>SQRT((F183-D183)^2+(G183-E183)^2)</f>
+        <v>3</v>
+      </c>
+      <c r="J183" s="66">
+        <f>SQRT((F183-B183)^2+(G183-C183)^2)</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="K183" s="70">
+        <f>DEGREES(ACOS((I183^2+J183^2-H183^2)/(2*I183*J183)))</f>
+        <v>45.000000000000021</v>
+      </c>
+      <c r="L183" s="71">
+        <f>DEGREES(ACOS((J183^2+H183^2-I183^2)/(2*J183*H183)))</f>
+        <v>45.000000000000021</v>
+      </c>
+      <c r="M183" s="71">
+        <f>DEGREES(ACOS((I183^2+H183^2-J183^2)/(2*I183*H183)))</f>
+        <v>89.999999999999986</v>
+      </c>
+      <c r="N183" s="72">
+        <f>RADIANS(K183)</f>
+        <v>0.78539816339744872</v>
+      </c>
+      <c r="O183" s="71">
+        <f>RADIANS(L183)</f>
+        <v>0.78539816339744872</v>
+      </c>
+      <c r="P183" s="73">
+        <f>RADIANS(M183)</f>
+        <v>1.5707963267948963</v>
+      </c>
+      <c r="Q183" s="74">
+        <f>2*$AL183/H183</f>
+        <v>2.9999999999999982</v>
+      </c>
+      <c r="R183" s="69">
+        <f>2*$AL183/I183</f>
+        <v>2.9999999999999982</v>
+      </c>
+      <c r="S183" s="75">
+        <f>2*$AL183/J183</f>
+        <v>2.1213203435596415</v>
+      </c>
+      <c r="T183" s="123">
+        <f>H183/SQRT(2)</f>
+        <v>2.1213203435596424</v>
+      </c>
+      <c r="U183" s="33">
+        <f>0.5*SQRT(2*J183^2+2*I183^2-H183^2)</f>
+        <v>3.3541019662496843</v>
+      </c>
+      <c r="V183" s="34">
+        <f>0.5*SQRT(2*J183^2+2*H183^2-I183^2)</f>
+        <v>3.3541019662496843</v>
+      </c>
+      <c r="W183" s="35">
+        <f>0.5*SQRT(2*I183^2+2*H183^2-J183^2)</f>
+        <v>2.1213203435596428</v>
+      </c>
+      <c r="X183" s="33">
+        <f>SQRT(J183*I183*(1-H183^2/(J183+I183)^2))</f>
+        <v>3.2471766008771819</v>
+      </c>
+      <c r="Y183" s="34">
+        <f>SQRT(J183*H183*(1-I183^2/(J183+H183)^2))</f>
+        <v>3.2471766008771819</v>
+      </c>
+      <c r="Z183" s="35">
+        <f>SQRT(I183*H183*(1-J183^2/(I183+H183)^2))</f>
+        <v>2.1213203435596428</v>
+      </c>
+      <c r="AA183" s="36">
+        <f>MAX(H183:J183)</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="AB183" s="8">
+        <f>IF(RANK(I183,$H183:$J183)+COUNTIF($H183:I183,I183)-1=2,I183,IF(RANK(J183,$H183:$J183)+COUNTIF($H183:J183,J183)-1=2,J183,H183))</f>
+        <v>3</v>
+      </c>
+      <c r="AC183" s="37">
+        <f>MIN(H183:J183)</f>
+        <v>3</v>
+      </c>
+      <c r="AD183" s="39">
+        <f>2*AA183*$AL183/($AA183^2+$AB183^2-$AC183^2)</f>
+        <v>2.1213203435596415</v>
+      </c>
+      <c r="AE183" s="8">
+        <f>2*AB183*$AL183/($AA183^2+$AB183^2-$AC183^2)</f>
+        <v>1.4999999999999996</v>
+      </c>
+      <c r="AF183" s="40">
+        <f>2*AC183*$AL183/($AA183^2-$AB183^2+$AC183^2)</f>
+        <v>1.4999999999999996</v>
+      </c>
+      <c r="AG183" s="8">
+        <f>INDEX($AD183:$AF183,1,MATCH(H183,$AA183:$AC183,0))</f>
+        <v>1.4999999999999996</v>
+      </c>
+      <c r="AH183" s="8">
+        <f>INDEX($AD183:$AF183,1,MATCH(I183,$AA183:$AC183,0))</f>
+        <v>1.4999999999999996</v>
+      </c>
+      <c r="AI183" s="28">
+        <f>INDEX($AD183:$AF183,1,MATCH(J183,$AA183:$AC183,0))</f>
+        <v>2.1213203435596415</v>
+      </c>
+      <c r="AJ183" s="26">
+        <f>I183+J183+H183</f>
+        <v>10.242640687119284</v>
+      </c>
+      <c r="AK183" s="26">
+        <f>AJ183/2</f>
+        <v>5.1213203435596419</v>
+      </c>
+      <c r="AL183" s="26">
+        <f>SQRT(AK183*(AK183-I183)*(AK183-J183)*(AK183-H183))</f>
+        <v>4.4999999999999973</v>
+      </c>
+      <c r="AM183" s="13">
+        <f>0.5*H183^2</f>
+        <v>4.5</v>
+      </c>
+      <c r="AN183" s="41">
+        <f>AL183/AK183</f>
+        <v>0.87867965644035706</v>
+      </c>
+      <c r="AO183" s="13">
+        <f>0.5*H183*(2-SQRT(2))</f>
+        <v>0.87867965644035728</v>
+      </c>
+      <c r="AP183" s="11">
+        <f>($I183*B183+$J183*D183+$H183*F183)/$AJ183</f>
+        <v>3.1213203435596428</v>
+      </c>
+      <c r="AQ183" s="11">
+        <f>($I183*C183+$J183*E183+$H183*G183)/$AJ183</f>
+        <v>2.8786796564403576</v>
+      </c>
+      <c r="AR183" s="41">
+        <f>I183*J183*H183/(4*AL183)</f>
+        <v>2.1213203435596437</v>
+      </c>
+      <c r="AS183" s="13">
+        <f>0.5*J183</f>
+        <v>2.1213203435596424</v>
+      </c>
+      <c r="AT183" s="8">
+        <f>2*(B183*(E183-G183)+D183*(G183-C183)+F183*(C183-E183))</f>
+        <v>18</v>
+      </c>
+      <c r="AU183" s="8">
+        <f>((B183^2+C183^2)*(E183-G183)+(D183^2+E183^2)*(G183-C183)+(F183^2+G183^2)*(C183-E183))/AT183</f>
+        <v>2.5</v>
+      </c>
+      <c r="AV183" s="28">
+        <f>-((B183^2+C183^2)*(D183-F183)+(D183^2+E183^2)*(F183-B183)+(F183^2+G183^2)*(B183-D183))/AT183</f>
+        <v>3.5</v>
+      </c>
+      <c r="AW183" s="27">
+        <f>(B183*TAN($O183)+D183*TAN($P183)+F183*TAN($N183))/(TAN($O183)+TAN($P183)+TAN($N183))</f>
+        <v>3.9999999999999987</v>
+      </c>
+      <c r="AX183" s="8">
+        <f>(C183*TAN($O183)+E183*TAN($P183)+G183*TAN($N183))/(TAN($O183)+TAN($P183)+TAN($N183))</f>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="AY183" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ183" s="27">
+        <f>(B183+D183+F183)/3</f>
+        <v>3</v>
+      </c>
+      <c r="BA183" s="28">
+        <f>(C183+E183+G183)/3</f>
+        <v>3</v>
+      </c>
+      <c r="BB183" t="str">
+        <f>A183</f>
+        <v>45-45-90</v>
+      </c>
+    </row>
+    <row r="184" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>113</v>
+      </c>
+      <c r="B184" s="5">
+        <v>1</v>
+      </c>
+      <c r="C184" s="5">
+        <v>2</v>
+      </c>
+      <c r="D184" s="5">
+        <v>7</v>
+      </c>
+      <c r="E184" s="5">
+        <v>2</v>
+      </c>
+      <c r="F184" s="5">
+        <v>4</v>
+      </c>
+      <c r="G184" s="25">
+        <f>C184+SQRT(6^2-3^2)</f>
+        <v>7.196152422706632</v>
+      </c>
+      <c r="H184" s="59">
+        <f>SQRT((B184-D184)^2+(C184-E184)^2)</f>
+        <v>6</v>
+      </c>
+      <c r="I184" s="11">
+        <f>SQRT((F184-D184)^2+(G184-E184)^2)</f>
+        <v>6</v>
+      </c>
+      <c r="J184" s="66">
+        <f>SQRT((F184-B184)^2+(G184-C184)^2)</f>
+        <v>6</v>
+      </c>
+      <c r="K184" s="70">
+        <f>DEGREES(ACOS((I184^2+J184^2-H184^2)/(2*I184*J184)))</f>
+        <v>59.999999999999993</v>
+      </c>
+      <c r="L184" s="71">
+        <f>DEGREES(ACOS((J184^2+H184^2-I184^2)/(2*J184*H184)))</f>
+        <v>59.999999999999993</v>
+      </c>
+      <c r="M184" s="71">
+        <f>DEGREES(ACOS((I184^2+H184^2-J184^2)/(2*I184*H184)))</f>
+        <v>59.999999999999993</v>
+      </c>
+      <c r="N184" s="72">
+        <f>RADIANS(K184)</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="O184" s="71">
+        <f>RADIANS(L184)</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="P184" s="73">
+        <f>RADIANS(M184)</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="Q184" s="74">
+        <f>2*$AL184/H184</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="R184" s="69">
+        <f>2*$AL184/I184</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="S184" s="75">
+        <f>2*$AL184/J184</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="T184" s="13">
+        <f>0.5*I184*SQRT(3)</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="U184" s="33">
+        <f>0.5*SQRT(2*J184^2+2*I184^2-H184^2)</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="V184" s="34">
+        <f>0.5*SQRT(2*J184^2+2*H184^2-I184^2)</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="W184" s="35">
+        <f>0.5*SQRT(2*I184^2+2*H184^2-J184^2)</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="X184" s="33">
+        <f>SQRT(J184*I184*(1-H184^2/(J184+I184)^2))</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="Y184" s="34">
+        <f>SQRT(J184*H184*(1-I184^2/(J184+H184)^2))</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="Z184" s="35">
+        <f>SQRT(I184*H184*(1-J184^2/(I184+H184)^2))</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AA184" s="36">
+        <f>MAX(H184:J184)</f>
+        <v>6</v>
+      </c>
+      <c r="AB184" s="8">
+        <f>IF(RANK(I184,$H184:$J184)+COUNTIF($H184:I184,I184)-1=2,I184,IF(RANK(J184,$H184:$J184)+COUNTIF($H184:J184,J184)-1=2,J184,H184))</f>
+        <v>6</v>
+      </c>
+      <c r="AC184" s="37">
+        <f>MIN(H184:J184)</f>
+        <v>6</v>
+      </c>
+      <c r="AD184" s="39">
+        <f>2*AA184*$AL184/($AA184^2+$AB184^2-$AC184^2)</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AE184" s="8">
+        <f>2*AB184*$AL184/($AA184^2+$AB184^2-$AC184^2)</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AF184" s="40">
+        <f>2*AC184*$AL184/($AA184^2-$AB184^2+$AC184^2)</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AG184" s="8">
+        <f>INDEX($AD184:$AF184,1,MATCH(H184,$AA184:$AC184,0))</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AH184" s="8">
+        <f>INDEX($AD184:$AF184,1,MATCH(I184,$AA184:$AC184,0))</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AI184" s="28">
+        <f>INDEX($AD184:$AF184,1,MATCH(J184,$AA184:$AC184,0))</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AJ184" s="26">
+        <f>I184+J184+H184</f>
+        <v>18</v>
+      </c>
+      <c r="AK184" s="26">
+        <f>AJ184/2</f>
+        <v>9</v>
+      </c>
+      <c r="AL184" s="26">
+        <f>SQRT(AK184*(AK184-I184)*(AK184-J184)*(AK184-H184))</f>
+        <v>15.588457268119896</v>
+      </c>
+      <c r="AM184" s="13">
+        <f>0.25*I184^2*SQRT(3)</f>
+        <v>15.588457268119894</v>
+      </c>
+      <c r="AN184" s="41">
+        <f>AL184/AK184</f>
+        <v>1.7320508075688774</v>
+      </c>
+      <c r="AO184" s="13">
+        <f>I184*SQRT(3)/6</f>
+        <v>1.7320508075688774</v>
+      </c>
+      <c r="AP184" s="11">
+        <f>($I184*B184+$J184*D184+$H184*F184)/$AJ184</f>
+        <v>4</v>
+      </c>
+      <c r="AQ184" s="11">
+        <f>($I184*C184+$J184*E184+$H184*G184)/$AJ184</f>
+        <v>3.7320508075688772</v>
+      </c>
+      <c r="AR184" s="41">
+        <f>I184*J184*H184/(4*AL184)</f>
+        <v>3.4641016151377544</v>
+      </c>
+      <c r="AS184" s="13">
+        <f>I184/SQRT(3)</f>
+        <v>3.4641016151377548</v>
+      </c>
+      <c r="AT184" s="8">
+        <f>2*(B184*(E184-G184)+D184*(G184-C184)+F184*(C184-E184))</f>
+        <v>62.353829072479584</v>
+      </c>
+      <c r="AU184" s="8">
+        <f>((B184^2+C184^2)*(E184-G184)+(D184^2+E184^2)*(G184-C184)+(F184^2+G184^2)*(C184-E184))/AT184</f>
+        <v>4</v>
+      </c>
+      <c r="AV184" s="28">
+        <f>-((B184^2+C184^2)*(D184-F184)+(D184^2+E184^2)*(F184-B184)+(F184^2+G184^2)*(B184-D184))/AT184</f>
+        <v>3.7320508075688772</v>
+      </c>
+      <c r="AW184" s="27">
+        <f>(B184*TAN($O184)+D184*TAN($P184)+F184*TAN($N184))/(TAN($O184)+TAN($P184)+TAN($N184))</f>
+        <v>4</v>
+      </c>
+      <c r="AX184" s="8">
+        <f>(C184*TAN($O184)+E184*TAN($P184)+G184*TAN($N184))/(TAN($O184)+TAN($P184)+TAN($N184))</f>
+        <v>3.7320508075688772</v>
+      </c>
+      <c r="AY184" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="AZ184" s="27">
+        <f>(B184+D184+F184)/3</f>
+        <v>4</v>
+      </c>
+      <c r="BA184" s="28">
+        <f>(C184+E184+G184)/3</f>
+        <v>3.7320508075688772</v>
+      </c>
+      <c r="BB184" t="str">
+        <f>A184</f>
+        <v>60-60-60</v>
+      </c>
+    </row>
+    <row r="185" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>112</v>
+      </c>
+      <c r="B185" s="5">
+        <v>1</v>
+      </c>
+      <c r="C185" s="5">
+        <v>2</v>
+      </c>
+      <c r="D185" s="5">
+        <v>4</v>
+      </c>
+      <c r="E185" s="5">
+        <v>2</v>
+      </c>
+      <c r="F185" s="5">
+        <v>4</v>
+      </c>
+      <c r="G185" s="25">
+        <f>C185+SQRT(6^2-3^2)</f>
+        <v>7.196152422706632</v>
+      </c>
+      <c r="H185" s="59">
+        <f>SQRT((B185-D185)^2+(C185-E185)^2)</f>
+        <v>3</v>
+      </c>
+      <c r="I185" s="11">
+        <f>SQRT((F185-D185)^2+(G185-E185)^2)</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="J185" s="66">
+        <f>SQRT((F185-B185)^2+(G185-C185)^2)</f>
+        <v>6</v>
+      </c>
+      <c r="K185" s="70">
+        <f>DEGREES(ACOS((I185^2+J185^2-H185^2)/(2*I185*J185)))</f>
+        <v>30.000000000000004</v>
+      </c>
+      <c r="L185" s="71">
+        <f>DEGREES(ACOS((J185^2+H185^2-I185^2)/(2*J185*H185)))</f>
+        <v>59.999999999999993</v>
+      </c>
+      <c r="M185" s="71">
+        <f>DEGREES(ACOS((I185^2+H185^2-J185^2)/(2*I185*H185)))</f>
+        <v>90</v>
+      </c>
+      <c r="N185" s="72">
+        <f>RADIANS(K185)</f>
+        <v>0.52359877559829893</v>
+      </c>
+      <c r="O185" s="71">
+        <f>RADIANS(L185)</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="P185" s="73">
+        <f>RADIANS(M185)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="Q185" s="74">
+        <f>2*$AL185/H185</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="R185" s="69">
+        <f>2*$AL185/I185</f>
+        <v>3</v>
+      </c>
+      <c r="S185" s="75">
+        <f>2*$AL185/J185</f>
+        <v>2.598076211353316</v>
+      </c>
+      <c r="T185" s="13">
+        <f>H185*I185/J185</f>
+        <v>2.598076211353316</v>
+      </c>
+      <c r="U185" s="33">
+        <f>0.5*SQRT(2*J185^2+2*I185^2-H185^2)</f>
+        <v>5.4083269131959844</v>
+      </c>
+      <c r="V185" s="34">
+        <f>0.5*SQRT(2*J185^2+2*H185^2-I185^2)</f>
+        <v>3.9686269665968861</v>
+      </c>
+      <c r="W185" s="35">
+        <f>0.5*SQRT(2*I185^2+2*H185^2-J185^2)</f>
+        <v>3</v>
+      </c>
+      <c r="X185" s="33">
+        <f>SQRT(J185*I185*(1-H185^2/(J185+I185)^2))</f>
+        <v>5.3794528330083216</v>
+      </c>
+      <c r="Y185" s="37">
+        <f>SQRT(J185*H185*(1-I185^2/(J185+H185)^2))</f>
+        <v>3.4641016151377548</v>
+      </c>
+      <c r="Z185" s="35">
+        <f>SQRT(I185*H185*(1-J185^2/(I185+H185)^2))</f>
+        <v>2.6897264165041608</v>
+      </c>
+      <c r="AA185" s="36">
+        <f>MAX(H185:J185)</f>
+        <v>6</v>
+      </c>
+      <c r="AB185" s="8">
+        <f>IF(RANK(I185,$H185:$J185)+COUNTIF($H185:I185,I185)-1=2,I185,IF(RANK(J185,$H185:$J185)+COUNTIF($H185:J185,J185)-1=2,J185,H185))</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AC185" s="37">
+        <f>MIN(H185:J185)</f>
+        <v>3</v>
+      </c>
+      <c r="AD185" s="39">
+        <f>2*AA185*$AL185/($AA185^2+$AB185^2-$AC185^2)</f>
+        <v>1.7320508075688774</v>
+      </c>
+      <c r="AE185" s="8">
+        <f>2*AB185*$AL185/($AA185^2+$AB185^2-$AC185^2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AF185" s="40">
+        <f>2*AC185*$AL185/($AA185^2-$AB185^2+$AC185^2)</f>
+        <v>2.598076211353316</v>
+      </c>
+      <c r="AG185" s="8">
+        <f>INDEX($AD185:$AF185,1,MATCH(H185,$AA185:$AC185,0))</f>
+        <v>2.598076211353316</v>
+      </c>
+      <c r="AH185" s="8">
+        <f>INDEX($AD185:$AF185,1,MATCH(I185,$AA185:$AC185,0))</f>
+        <v>1.5</v>
+      </c>
+      <c r="AI185" s="28">
+        <f>INDEX($AD185:$AF185,1,MATCH(J185,$AA185:$AC185,0))</f>
+        <v>1.7320508075688774</v>
+      </c>
+      <c r="AJ185" s="26">
+        <f>I185+J185+H185</f>
+        <v>14.196152422706632</v>
+      </c>
+      <c r="AK185" s="26">
+        <f>AJ185/2</f>
+        <v>7.098076211353316</v>
+      </c>
+      <c r="AL185" s="26">
+        <f>SQRT(AK185*(AK185-I185)*(AK185-J185)*(AK185-H185))</f>
+        <v>7.794228634059948</v>
+      </c>
+      <c r="AM185" s="13">
+        <f>(1/8)*J185^2*SQRT(3)</f>
+        <v>7.7942286340599471</v>
+      </c>
+      <c r="AN185" s="41">
+        <f>AL185/AK185</f>
+        <v>1.098076211353316</v>
+      </c>
+      <c r="AO185" s="13">
+        <f>0.25*J185*(SQRT(3)-1)</f>
+        <v>1.0980762113533158</v>
+      </c>
+      <c r="AP185" s="11">
+        <f>($I185*B185+$J185*D185+$H185*F185)/$AJ185</f>
+        <v>2.901923788646684</v>
+      </c>
+      <c r="AQ185" s="11">
+        <f>($I185*C185+$J185*E185+$H185*G185)/$AJ185</f>
+        <v>3.098076211353316</v>
+      </c>
+      <c r="AR185" s="41">
+        <f>I185*J185*H185/(4*AL185)</f>
+        <v>3</v>
+      </c>
+      <c r="AS185" s="13">
+        <f>0.5*J185</f>
+        <v>3</v>
+      </c>
+      <c r="AT185" s="8">
+        <f>2*(B185*(E185-G185)+D185*(G185-C185)+F185*(C185-E185))</f>
+        <v>31.176914536239792</v>
+      </c>
+      <c r="AU185" s="8">
+        <f>((B185^2+C185^2)*(E185-G185)+(D185^2+E185^2)*(G185-C185)+(F185^2+G185^2)*(C185-E185))/AT185</f>
+        <v>2.5</v>
+      </c>
+      <c r="AV185" s="28">
+        <f>-((B185^2+C185^2)*(D185-F185)+(D185^2+E185^2)*(F185-B185)+(F185^2+G185^2)*(B185-D185))/AT185</f>
+        <v>4.598076211353316</v>
+      </c>
+      <c r="AW185" s="27">
+        <f>(B185*TAN($O185)+D185*TAN($P185)+F185*TAN($N185))/(TAN($O185)+TAN($P185)+TAN($N185))</f>
+        <v>3.9999999999999996</v>
+      </c>
+      <c r="AX185" s="8">
+        <f>(C185*TAN($O185)+E185*TAN($P185)+G185*TAN($N185))/(TAN($O185)+TAN($P185)+TAN($N185))</f>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="AY185" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ185" s="27">
+        <f>(B185+D185+F185)/3</f>
+        <v>3</v>
+      </c>
+      <c r="BA185" s="28">
+        <f>(C185+E185+G185)/3</f>
+        <v>3.7320508075688772</v>
+      </c>
+      <c r="BB185" t="str">
+        <f>A185</f>
+        <v>30-60-90</v>
+      </c>
+    </row>
+    <row r="186" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>141</v>
+      </c>
+      <c r="B186" s="5">
+        <v>2</v>
+      </c>
+      <c r="C186" s="5">
+        <v>5.6568550000000002</v>
+      </c>
+      <c r="D186" s="5">
+        <v>0</v>
+      </c>
+      <c r="E186" s="5">
+        <v>0</v>
+      </c>
+      <c r="F186" s="5">
+        <v>4</v>
+      </c>
+      <c r="G186" s="5">
+        <v>0</v>
+      </c>
+      <c r="H186" s="59">
+        <f>SQRT((B186-D186)^2+(C186-E186)^2)</f>
+        <v>6.0000007075853752</v>
+      </c>
+      <c r="I186" s="11">
+        <f>SQRT((F186-D186)^2+(G186-E186)^2)</f>
+        <v>4</v>
+      </c>
+      <c r="J186" s="66">
+        <f>SQRT((F186-B186)^2+(G186-C186)^2)</f>
+        <v>6.0000007075853752</v>
+      </c>
+      <c r="K186" s="70">
+        <f>DEGREES(ACOS((I186^2+J186^2-H186^2)/(2*I186*J186)))</f>
+        <v>70.528781754448971</v>
+      </c>
+      <c r="L186" s="71">
+        <f>DEGREES(ACOS((J186^2+H186^2-I186^2)/(2*J186*H186)))</f>
+        <v>38.942436491102043</v>
+      </c>
+      <c r="M186" s="71">
+        <f>DEGREES(ACOS((I186^2+H186^2-J186^2)/(2*I186*H186)))</f>
+        <v>70.528781754448971</v>
+      </c>
+      <c r="N186" s="72">
+        <f>RADIANS(K186)</f>
+        <v>1.2309594590356374</v>
+      </c>
+      <c r="O186" s="71">
+        <f>RADIANS(L186)</f>
+        <v>0.67967373551851817</v>
+      </c>
+      <c r="P186" s="73">
+        <f>RADIANS(M186)</f>
+        <v>1.2309594590356374</v>
+      </c>
+      <c r="Q186" s="74">
+        <f>2*$AL186/H186</f>
+        <v>3.7712362219214008</v>
+      </c>
+      <c r="R186" s="69">
+        <f>2*$AL186/I186</f>
+        <v>5.6568550000000002</v>
+      </c>
+      <c r="S186" s="75">
+        <f>2*$AL186/J186</f>
+        <v>3.7712362219214008</v>
+      </c>
+      <c r="T186" s="123">
+        <f>0.5*SQRT(4*H186^2-I186^2)</f>
+        <v>5.6568550000000002</v>
+      </c>
+      <c r="U186" s="33">
+        <f>0.5*SQRT(2*J186^2+2*I186^2-H186^2)</f>
+        <v>4.1231058830396599</v>
+      </c>
+      <c r="V186" s="34">
+        <f>0.5*SQRT(2*J186^2+2*H186^2-I186^2)</f>
+        <v>5.6568550000000002</v>
+      </c>
+      <c r="W186" s="35">
+        <f>0.5*SQRT(2*I186^2+2*H186^2-J186^2)</f>
+        <v>4.1231058830396599</v>
+      </c>
+      <c r="X186" s="33">
+        <f>SQRT(J186*I186*(1-H186^2/(J186+I186)^2))</f>
+        <v>3.9191837155561045</v>
+      </c>
+      <c r="Y186" s="37">
+        <f>SQRT(J186*H186*(1-I186^2/(J186+H186)^2))</f>
+        <v>5.6568550000000002</v>
+      </c>
+      <c r="Z186" s="35">
+        <f>SQRT(I186*H186*(1-J186^2/(I186+H186)^2))</f>
+        <v>3.9191837155561045</v>
+      </c>
+      <c r="AA186" s="36">
+        <f>MAX(H186:J186)</f>
+        <v>6.0000007075853752</v>
+      </c>
+      <c r="AB186" s="8">
+        <f>IF(RANK(I186,$H186:$J186)+COUNTIF($H186:I186,I186)-1=2,I186,IF(RANK(J186,$H186:$J186)+COUNTIF($H186:J186,J186)-1=2,J186,H186))</f>
+        <v>6.0000007075853752</v>
+      </c>
+      <c r="AC186" s="37">
+        <f>MIN(H186:J186)</f>
+        <v>4</v>
+      </c>
+      <c r="AD186" s="39">
+        <f>2*AA186*$AL186/($AA186^2+$AB186^2-$AC186^2)</f>
+        <v>2.4243659792879857</v>
+      </c>
+      <c r="AE186" s="8">
+        <f>2*AB186*$AL186/($AA186^2+$AB186^2-$AC186^2)</f>
+        <v>2.4243659792879857</v>
+      </c>
+      <c r="AF186" s="40">
+        <f>2*AC186*$AL186/($AA186^2-$AB186^2+$AC186^2)</f>
+        <v>5.6568550000000002</v>
+      </c>
+      <c r="AG186" s="8">
+        <f>INDEX($AD186:$AF186,1,MATCH(H186,$AA186:$AC186,0))</f>
+        <v>2.4243659792879857</v>
+      </c>
+      <c r="AH186" s="8">
+        <f>INDEX($AD186:$AF186,1,MATCH(I186,$AA186:$AC186,0))</f>
+        <v>5.6568550000000002</v>
+      </c>
+      <c r="AI186" s="28">
+        <f>INDEX($AD186:$AF186,1,MATCH(J186,$AA186:$AC186,0))</f>
+        <v>2.4243659792879857</v>
+      </c>
+      <c r="AJ186" s="26">
+        <f>I186+J186+H186</f>
+        <v>16.00000141517075</v>
+      </c>
+      <c r="AK186" s="26">
+        <f>AJ186/2</f>
+        <v>8.0000007075853752</v>
+      </c>
+      <c r="AL186" s="32">
+        <f>SQRT(AK186*(AK186-I186)*(AK186-J186)*(AK186-H186))</f>
+        <v>11.31371</v>
+      </c>
+      <c r="AM186" s="13">
+        <f>0.25*I186*SQRT(4*H186^2-I186^2)</f>
+        <v>11.31371</v>
+      </c>
+      <c r="AN186" s="41">
+        <f>AL186/AK186</f>
+        <v>1.4142136249153903</v>
+      </c>
+      <c r="AO186" s="13">
+        <f>I186*(SQRT(I186^2+4*T186^2)-I186)/(4*T186)</f>
+        <v>1.4142136249153903</v>
+      </c>
+      <c r="AP186" s="11">
+        <f>($I186*B186+$J186*D186+$H186*F186)/$AJ186</f>
+        <v>2</v>
+      </c>
+      <c r="AQ186" s="11">
+        <f>($I186*C186+$J186*E186+$H186*G186)/$AJ186</f>
+        <v>1.4142136249153903</v>
+      </c>
+      <c r="AR186" s="41">
+        <f>I186*J186*H186/(4*AL186)</f>
+        <v>3.1819808436865538</v>
+      </c>
+      <c r="AS186" s="13">
+        <f>(1/8)*(I186^2/T186+4*T186)</f>
+        <v>3.1819808436865538</v>
+      </c>
+      <c r="AT186" s="8">
+        <f>2*(B186*(E186-G186)+D186*(G186-C186)+F186*(C186-E186))</f>
+        <v>45.254840000000002</v>
+      </c>
+      <c r="AU186" s="8">
+        <f>((B186^2+C186^2)*(E186-G186)+(D186^2+E186^2)*(G186-C186)+(F186^2+G186^2)*(C186-E186))/AT186</f>
+        <v>2</v>
+      </c>
+      <c r="AV186" s="28">
+        <f>-((B186^2+C186^2)*(D186-F186)+(D186^2+E186^2)*(F186-B186)+(F186^2+G186^2)*(B186-D186))/AT186</f>
+        <v>2.474874156313446</v>
+      </c>
+      <c r="AW186" s="27">
+        <f>(B186*TAN($O186)+D186*TAN($P186)+F186*TAN($N186))/(TAN($O186)+TAN($P186)+TAN($N186))</f>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="AX186" s="8">
+        <f>(C186*TAN($O186)+E186*TAN($P186)+G186*TAN($N186))/(TAN($O186)+TAN($P186)+TAN($N186))</f>
+        <v>0.70710668737310767</v>
+      </c>
+      <c r="AY186" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ186" s="27">
+        <f>(B186+D186+F186)/3</f>
+        <v>2</v>
+      </c>
+      <c r="BA186" s="28">
+        <f>(C186+E186+G186)/3</f>
+        <v>1.8856183333333334</v>
+      </c>
+      <c r="BB186" t="str">
+        <f>A186</f>
+        <v>Isosceles</v>
+      </c>
+    </row>
+    <row r="187" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>140</v>
+      </c>
+      <c r="B187" s="5">
+        <v>0</v>
+      </c>
+      <c r="C187" s="5">
+        <v>0</v>
+      </c>
+      <c r="D187" s="5">
+        <v>4</v>
+      </c>
+      <c r="E187" s="5">
+        <v>0</v>
+      </c>
+      <c r="F187" s="5">
+        <v>0</v>
+      </c>
+      <c r="G187" s="5">
+        <v>4</v>
+      </c>
+      <c r="H187" s="27">
+        <f>SQRT((B187-D187)^2+(C187-E187)^2)</f>
+        <v>4</v>
+      </c>
+      <c r="I187" s="8">
+        <f>SQRT((F187-D187)^2+(G187-E187)^2)</f>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="J187" s="28">
+        <f>SQRT((F187-B187)^2+(G187-C187)^2)</f>
+        <v>4</v>
+      </c>
+      <c r="K187" s="29">
+        <f>DEGREES(ACOS((I187^2+J187^2-H187^2)/(2*I187*J187)))</f>
+        <v>44.999999999999986</v>
+      </c>
+      <c r="L187" s="30">
+        <f>DEGREES(ACOS((J187^2+H187^2-I187^2)/(2*J187*H187)))</f>
+        <v>90.000000000000014</v>
+      </c>
+      <c r="M187" s="30">
+        <f>DEGREES(ACOS((I187^2+H187^2-J187^2)/(2*I187*H187)))</f>
+        <v>44.999999999999986</v>
+      </c>
+      <c r="N187" s="55">
+        <f>RADIANS(K187)</f>
+        <v>0.78539816339744806</v>
+      </c>
+      <c r="O187" s="30">
+        <f>RADIANS(L187)</f>
+        <v>1.5707963267948968</v>
+      </c>
+      <c r="P187" s="31">
+        <f>RADIANS(M187)</f>
+        <v>0.78539816339744806</v>
+      </c>
+      <c r="Q187" s="36">
+        <f>2*$AL187/H187</f>
+        <v>3.9999999999999982</v>
+      </c>
+      <c r="R187" s="37">
+        <f>2*$AL187/I187</f>
+        <v>2.8284271247461885</v>
+      </c>
+      <c r="S187" s="38">
+        <f>2*$AL187/J187</f>
+        <v>3.9999999999999982</v>
+      </c>
+      <c r="T187" s="123">
+        <f>H187/SQRT(2)</f>
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="U187" s="33">
+        <f>0.5*SQRT(2*J187^2+2*I187^2-H187^2)</f>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="V187" s="34">
+        <f>0.5*SQRT(2*J187^2+2*H187^2-I187^2)</f>
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="W187" s="35">
+        <f>0.5*SQRT(2*I187^2+2*H187^2-J187^2)</f>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="X187" s="33">
+        <f>SQRT(J187*I187*(1-H187^2/(J187+I187)^2))</f>
+        <v>4.3295688011695761</v>
+      </c>
+      <c r="Y187" s="37">
+        <f>SQRT(J187*H187*(1-I187^2/(J187+H187)^2))</f>
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="Z187" s="35">
+        <f>SQRT(I187*H187*(1-J187^2/(I187+H187)^2))</f>
+        <v>4.3295688011695761</v>
+      </c>
+      <c r="AA187" s="36">
+        <f>MAX(H187:J187)</f>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="AB187" s="8">
+        <f>IF(RANK(I187,$H187:$J187)+COUNTIF($H187:I187,I187)-1=2,I187,IF(RANK(J187,$H187:$J187)+COUNTIF($H187:J187,J187)-1=2,J187,H187))</f>
+        <v>4</v>
+      </c>
+      <c r="AC187" s="37">
+        <f>MIN(H187:J187)</f>
+        <v>4</v>
+      </c>
+      <c r="AD187" s="39">
+        <f>2*AA187*$AL187/($AA187^2+$AB187^2-$AC187^2)</f>
+        <v>2.8284271247461885</v>
+      </c>
+      <c r="AE187" s="8">
+        <f>2*AB187*$AL187/($AA187^2+$AB187^2-$AC187^2)</f>
+        <v>1.9999999999999987</v>
+      </c>
+      <c r="AF187" s="40">
+        <f>2*AC187*$AL187/($AA187^2-$AB187^2+$AC187^2)</f>
+        <v>1.9999999999999987</v>
+      </c>
+      <c r="AG187" s="8">
+        <f>INDEX($AD187:$AF187,1,MATCH(H187,$AA187:$AC187,0))</f>
+        <v>1.9999999999999987</v>
+      </c>
+      <c r="AH187" s="8">
+        <f>INDEX($AD187:$AF187,1,MATCH(I187,$AA187:$AC187,0))</f>
+        <v>2.8284271247461885</v>
+      </c>
+      <c r="AI187" s="28">
+        <f>INDEX($AD187:$AF187,1,MATCH(J187,$AA187:$AC187,0))</f>
+        <v>1.9999999999999987</v>
+      </c>
+      <c r="AJ187" s="26">
+        <f>I187+J187+H187</f>
+        <v>13.65685424949238</v>
+      </c>
+      <c r="AK187" s="26">
+        <f>AJ187/2</f>
+        <v>6.8284271247461898</v>
+      </c>
+      <c r="AL187" s="26">
+        <f>SQRT(AK187*(AK187-I187)*(AK187-J187)*(AK187-H187))</f>
+        <v>7.9999999999999964</v>
+      </c>
+      <c r="AM187" s="13">
+        <f>0.5*H187^2</f>
+        <v>8</v>
+      </c>
+      <c r="AN187" s="41">
+        <f>AL187/AK187</f>
+        <v>1.1715728752538095</v>
+      </c>
+      <c r="AO187" s="13">
+        <f>0.5*H187*(2-SQRT(2))</f>
+        <v>1.1715728752538097</v>
+      </c>
+      <c r="AP187" s="11">
+        <f>($I187*B187+$J187*D187+$H187*F187)/$AJ187</f>
+        <v>1.1715728752538099</v>
+      </c>
+      <c r="AQ187" s="11">
+        <f>($I187*C187+$J187*E187+$H187*G187)/$AJ187</f>
+        <v>1.1715728752538099</v>
+      </c>
+      <c r="AR187" s="41">
+        <f>I187*J187*H187/(4*AL187)</f>
+        <v>2.8284271247461916</v>
+      </c>
+      <c r="AS187" s="13">
+        <f>(1/8)*(I187^2/T187+4*T187)</f>
+        <v>2.8284271247461907</v>
+      </c>
+      <c r="AT187" s="8">
+        <f>2*(B187*(E187-G187)+D187*(G187-C187)+F187*(C187-E187))</f>
+        <v>32</v>
+      </c>
+      <c r="AU187" s="8">
+        <f>((B187^2+C187^2)*(E187-G187)+(D187^2+E187^2)*(G187-C187)+(F187^2+G187^2)*(C187-E187))/AT187</f>
+        <v>2</v>
+      </c>
+      <c r="AV187" s="28">
+        <f>-((B187^2+C187^2)*(D187-F187)+(D187^2+E187^2)*(F187-B187)+(F187^2+G187^2)*(B187-D187))/AT187</f>
+        <v>2</v>
+      </c>
+      <c r="AW187" s="27">
+        <f>(B187*TAN($O187)+D187*TAN($P187)+F187*TAN($N187))/(TAN($O187)+TAN($P187)+TAN($N187))</f>
+        <v>-6.4314872871840113E-16</v>
+      </c>
+      <c r="AX187" s="8">
+        <f>(C187*TAN($O187)+E187*TAN($P187)+G187*TAN($N187))/(TAN($O187)+TAN($P187)+TAN($N187))</f>
+        <v>-6.4314872871840113E-16</v>
+      </c>
+      <c r="AY187" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ187" s="27">
+        <f>(B187+D187+F187)/3</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="BA187" s="28">
+        <f>(C187+E187+G187)/3</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="BB187" t="str">
+        <f>A187</f>
+        <v>Right Isosceles</v>
+      </c>
+    </row>
+    <row r="188" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>142</v>
+      </c>
+      <c r="B188" s="5">
+        <v>0</v>
+      </c>
+      <c r="C188" s="5">
+        <v>0</v>
+      </c>
+      <c r="D188" s="5">
+        <v>4</v>
+      </c>
+      <c r="E188" s="5">
+        <v>0</v>
+      </c>
+      <c r="F188" s="5">
+        <v>4</v>
+      </c>
+      <c r="G188" s="5">
+        <v>6</v>
+      </c>
+      <c r="H188" s="59">
+        <f>SQRT((B188-D188)^2+(C188-E188)^2)</f>
+        <v>4</v>
+      </c>
+      <c r="I188" s="11">
+        <f>SQRT((F188-D188)^2+(G188-E188)^2)</f>
+        <v>6</v>
+      </c>
+      <c r="J188" s="66">
+        <f>SQRT((F188-B188)^2+(G188-C188)^2)</f>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="K188" s="70">
+        <f>DEGREES(ACOS((I188^2+J188^2-H188^2)/(2*I188*J188)))</f>
+        <v>33.690067525979778</v>
+      </c>
+      <c r="L188" s="71">
+        <f>DEGREES(ACOS((J188^2+H188^2-I188^2)/(2*J188*H188)))</f>
+        <v>56.309932474020215</v>
+      </c>
+      <c r="M188" s="71">
+        <f>DEGREES(ACOS((I188^2+H188^2-J188^2)/(2*I188*H188)))</f>
+        <v>89.999999999999986</v>
+      </c>
+      <c r="N188" s="72">
+        <f>RADIANS(K188)</f>
+        <v>0.58800260354756739</v>
+      </c>
+      <c r="O188" s="71">
+        <f>RADIANS(L188)</f>
+        <v>0.98279372324732905</v>
+      </c>
+      <c r="P188" s="73">
+        <f>RADIANS(M188)</f>
+        <v>1.5707963267948963</v>
+      </c>
+      <c r="Q188" s="74">
+        <f>2*$AL188/H188</f>
+        <v>6.0000000000000027</v>
+      </c>
+      <c r="R188" s="69">
+        <f>2*$AL188/I188</f>
+        <v>4.0000000000000018</v>
+      </c>
+      <c r="S188" s="75">
+        <f>2*$AL188/J188</f>
+        <v>3.3282011773513762</v>
+      </c>
+      <c r="T188" s="123">
+        <f>H188*I188/J188</f>
+        <v>3.3282011773513749</v>
+      </c>
+      <c r="U188" s="76">
+        <f>0.5*SQRT(2*J188^2+2*I188^2-H188^2)</f>
+        <v>6.324555320336759</v>
+      </c>
+      <c r="V188" s="77">
+        <f>0.5*SQRT(2*J188^2+2*H188^2-I188^2)</f>
+        <v>5</v>
+      </c>
+      <c r="W188" s="78">
+        <f>0.5*SQRT(2*I188^2+2*H188^2-J188^2)</f>
+        <v>3.6055512754639896</v>
+      </c>
+      <c r="X188" s="76">
+        <f>SQRT(J188*I188*(1-H188^2/(J188+I188)^2))</f>
+        <v>6.2689896414768924</v>
+      </c>
+      <c r="Y188" s="69">
+        <f>SQRT(J188*H188*(1-I188^2/(J188+H188)^2))</f>
+        <v>4.5368211873060869</v>
+      </c>
+      <c r="Z188" s="78">
+        <f>SQRT(I188*H188*(1-J188^2/(I188+H188)^2))</f>
+        <v>3.3941125496954285</v>
+      </c>
+      <c r="AA188" s="74">
+        <f>MAX(H188:J188)</f>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="AB188" s="11">
+        <f>IF(RANK(I188,$H188:$J188)+COUNTIF($H188:I188,I188)-1=2,I188,IF(RANK(J188,$H188:$J188)+COUNTIF($H188:J188,J188)-1=2,J188,H188))</f>
+        <v>6</v>
+      </c>
+      <c r="AC188" s="69">
+        <f>MIN(H188:J188)</f>
+        <v>4</v>
+      </c>
+      <c r="AD188" s="54">
+        <f>2*AA188*$AL188/($AA188^2+$AB188^2-$AC188^2)</f>
+        <v>2.4037008503093271</v>
+      </c>
+      <c r="AE188" s="11">
+        <f>2*AB188*$AL188/($AA188^2+$AB188^2-$AC188^2)</f>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="AF188" s="79">
+        <f>2*AC188*$AL188/($AA188^2-$AB188^2+$AC188^2)</f>
+        <v>3.0000000000000018</v>
+      </c>
+      <c r="AG188" s="11">
+        <f>INDEX($AD188:$AF188,1,MATCH(H188,$AA188:$AC188,0))</f>
+        <v>3.0000000000000018</v>
+      </c>
+      <c r="AH188" s="11">
+        <f>INDEX($AD188:$AF188,1,MATCH(I188,$AA188:$AC188,0))</f>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="AI188" s="66">
+        <f>INDEX($AD188:$AF188,1,MATCH(J188,$AA188:$AC188,0))</f>
+        <v>2.4037008503093271</v>
+      </c>
+      <c r="AJ188" s="26">
+        <f>I188+J188+H188</f>
+        <v>17.211102550927979</v>
+      </c>
+      <c r="AK188" s="26">
+        <f>AJ188/2</f>
+        <v>8.6055512754639896</v>
+      </c>
+      <c r="AL188" s="26">
+        <f>SQRT(AK188*(AK188-I188)*(AK188-J188)*(AK188-H188))</f>
+        <v>12.000000000000005</v>
+      </c>
+      <c r="AM188" s="13">
+        <f>0.5*I188*H188</f>
+        <v>12</v>
+      </c>
+      <c r="AN188" s="80">
+        <f>AL188/AK188</f>
+        <v>1.3944487245360113</v>
+      </c>
+      <c r="AO188" s="13">
+        <f>H188*I188/AJ188</f>
+        <v>1.3944487245360107</v>
+      </c>
+      <c r="AP188" s="11">
+        <f>($I188*B188+$J188*D188+$H188*F188)/$AJ188</f>
+        <v>2.6055512754639891</v>
+      </c>
+      <c r="AQ188" s="11">
+        <f>($I188*C188+$J188*E188+$H188*G188)/$AJ188</f>
+        <v>1.3944487245360107</v>
+      </c>
+      <c r="AR188" s="80">
+        <f>I188*J188*H188/(4*AL188)</f>
+        <v>3.6055512754639873</v>
+      </c>
+      <c r="AS188" s="13">
+        <f>0.5*J188</f>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="AT188" s="11">
+        <f>2*(B188*(E188-G188)+D188*(G188-C188)+F188*(C188-E188))</f>
+        <v>48</v>
+      </c>
+      <c r="AU188" s="11">
+        <f>((B188^2+C188^2)*(E188-G188)+(D188^2+E188^2)*(G188-C188)+(F188^2+G188^2)*(C188-E188))/AT188</f>
+        <v>2</v>
+      </c>
+      <c r="AV188" s="66">
+        <f>-((B188^2+C188^2)*(D188-F188)+(D188^2+E188^2)*(F188-B188)+(F188^2+G188^2)*(B188-D188))/AT188</f>
+        <v>3</v>
+      </c>
+      <c r="AW188" s="59">
+        <f>(B188*TAN($O188)+D188*TAN($P188)+F188*TAN($N188))/(TAN($O188)+TAN($P188)+TAN($N188))</f>
+        <v>3.9999999999999982</v>
+      </c>
+      <c r="AX188" s="11">
+        <f>(C188*TAN($O188)+E188*TAN($P188)+G188*TAN($N188))/(TAN($O188)+TAN($P188)+TAN($N188))</f>
+        <v>1.1332081106818481E-15</v>
+      </c>
+      <c r="AZ188" s="59">
+        <f>(B188+D188+F188)/3</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="BA188" s="66">
+        <f>(C188+E188+G188)/3</f>
+        <v>2</v>
+      </c>
+      <c r="BB188" t="str">
+        <f>A188</f>
+        <v>Right Triangle</v>
+      </c>
+      <c r="BC188">
+        <f>H188^2/J188</f>
+        <v>2.2188007849009166</v>
+      </c>
+      <c r="BD188">
+        <f>I188^2/J188</f>
+        <v>4.9923017660270625</v>
+      </c>
+      <c r="BE188">
+        <f>BC188+BD188</f>
+        <v>7.2111025509279791</v>
+      </c>
+    </row>
+    <row r="189" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>143</v>
+      </c>
+      <c r="B189" s="5">
+        <v>0</v>
+      </c>
+      <c r="C189" s="5">
+        <v>0</v>
+      </c>
+      <c r="D189" s="5">
+        <v>3</v>
+      </c>
+      <c r="E189" s="5">
+        <v>0</v>
+      </c>
+      <c r="F189" s="5">
+        <v>3</v>
+      </c>
+      <c r="G189" s="5">
+        <v>4</v>
+      </c>
+      <c r="H189" s="59">
+        <f>SQRT((B189-D189)^2+(C189-E189)^2)</f>
+        <v>3</v>
+      </c>
+      <c r="I189" s="11">
+        <f>SQRT((F189-D189)^2+(G189-E189)^2)</f>
+        <v>4</v>
+      </c>
+      <c r="J189" s="66">
+        <f>SQRT((F189-B189)^2+(G189-C189)^2)</f>
+        <v>5</v>
+      </c>
+      <c r="K189" s="70">
+        <f>DEGREES(ACOS((I189^2+J189^2-H189^2)/(2*I189*J189)))</f>
+        <v>36.869897645844013</v>
+      </c>
+      <c r="L189" s="71">
+        <f>DEGREES(ACOS((J189^2+H189^2-I189^2)/(2*J189*H189)))</f>
+        <v>53.13010235415598</v>
+      </c>
+      <c r="M189" s="71">
+        <f>DEGREES(ACOS((I189^2+H189^2-J189^2)/(2*I189*H189)))</f>
+        <v>90</v>
+      </c>
+      <c r="N189" s="72">
+        <f>RADIANS(K189)</f>
+        <v>0.64350110879328426</v>
+      </c>
+      <c r="O189" s="71">
+        <f>RADIANS(L189)</f>
+        <v>0.92729521800161219</v>
+      </c>
+      <c r="P189" s="73">
+        <f>RADIANS(M189)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="Q189" s="74">
+        <f>2*$AL189/H189</f>
+        <v>4</v>
+      </c>
+      <c r="R189" s="69">
+        <f>2*$AL189/I189</f>
+        <v>3</v>
+      </c>
+      <c r="S189" s="75">
+        <f>2*$AL189/J189</f>
+        <v>2.4</v>
+      </c>
+      <c r="T189" s="82">
+        <f>H189*I189/J189</f>
+        <v>2.4</v>
+      </c>
+      <c r="U189" s="76">
+        <f>0.5*SQRT(2*J189^2+2*I189^2-H189^2)</f>
+        <v>4.2720018726587652</v>
+      </c>
+      <c r="V189" s="77">
+        <f>0.5*SQRT(2*J189^2+2*H189^2-I189^2)</f>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="W189" s="78">
+        <f>0.5*SQRT(2*I189^2+2*H189^2-J189^2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="X189" s="76">
+        <f>SQRT(J189*I189*(1-H189^2/(J189+I189)^2))</f>
+        <v>4.2163702135578394</v>
+      </c>
+      <c r="Y189" s="69">
+        <f>SQRT(J189*H189*(1-I189^2/(J189+H189)^2))</f>
+        <v>3.3541019662496847</v>
+      </c>
+      <c r="Z189" s="78">
+        <f>SQRT(I189*H189*(1-J189^2/(I189+H189)^2))</f>
+        <v>2.4243661069253055</v>
+      </c>
+      <c r="AA189" s="74">
+        <f>MAX(H189:J189)</f>
+        <v>5</v>
+      </c>
+      <c r="AB189" s="11">
+        <f>IF(RANK(I189,$H189:$J189)+COUNTIF($H189:I189,I189)-1=2,I189,IF(RANK(J189,$H189:$J189)+COUNTIF($H189:J189,J189)-1=2,J189,H189))</f>
+        <v>4</v>
+      </c>
+      <c r="AC189" s="69">
+        <f>MIN(H189:J189)</f>
+        <v>3</v>
+      </c>
+      <c r="AD189" s="54">
+        <f>2*AA189*$AL189/($AA189^2+$AB189^2-$AC189^2)</f>
+        <v>1.875</v>
+      </c>
+      <c r="AE189" s="11">
+        <f>2*AB189*$AL189/($AA189^2+$AB189^2-$AC189^2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AF189" s="79">
+        <f>2*AC189*$AL189/($AA189^2-$AB189^2+$AC189^2)</f>
+        <v>2</v>
+      </c>
+      <c r="AG189" s="11">
+        <f>INDEX($AD189:$AF189,1,MATCH(H189,$AA189:$AC189,0))</f>
+        <v>2</v>
+      </c>
+      <c r="AH189" s="11">
+        <f>INDEX($AD189:$AF189,1,MATCH(I189,$AA189:$AC189,0))</f>
+        <v>1.5</v>
+      </c>
+      <c r="AI189" s="66">
+        <f>INDEX($AD189:$AF189,1,MATCH(J189,$AA189:$AC189,0))</f>
+        <v>1.875</v>
+      </c>
+      <c r="AJ189" s="26">
+        <f>I189+J189+H189</f>
+        <v>12</v>
+      </c>
+      <c r="AK189" s="26">
+        <f>AJ189/2</f>
+        <v>6</v>
+      </c>
+      <c r="AL189" s="26">
+        <f>SQRT(AK189*(AK189-I189)*(AK189-J189)*(AK189-H189))</f>
+        <v>6</v>
+      </c>
+      <c r="AM189" s="83">
+        <f>6*(H189/3)</f>
+        <v>6</v>
+      </c>
+      <c r="AN189" s="80">
+        <f>AL189/AK189</f>
+        <v>1</v>
+      </c>
+      <c r="AO189" s="83">
+        <f>1*(H189/3)</f>
+        <v>1</v>
+      </c>
+      <c r="AP189" s="11">
+        <f>($I189*B189+$J189*D189+$H189*F189)/$AJ189</f>
+        <v>2</v>
+      </c>
+      <c r="AQ189" s="11">
+        <f>($I189*C189+$J189*E189+$H189*G189)/$AJ189</f>
+        <v>1</v>
+      </c>
+      <c r="AR189" s="80">
+        <f>I189*J189*H189/(4*AL189)</f>
+        <v>2.5</v>
+      </c>
+      <c r="AS189" s="83">
+        <f>5/2*(H189/3)</f>
+        <v>2.5</v>
+      </c>
+      <c r="AT189" s="11">
+        <f>2*(B189*(E189-G189)+D189*(G189-C189)+F189*(C189-E189))</f>
+        <v>24</v>
+      </c>
+      <c r="AU189" s="11">
+        <f>((B189^2+C189^2)*(E189-G189)+(D189^2+E189^2)*(G189-C189)+(F189^2+G189^2)*(C189-E189))/AT189</f>
+        <v>1.5</v>
+      </c>
+      <c r="AV189" s="66">
+        <f>-((B189^2+C189^2)*(D189-F189)+(D189^2+E189^2)*(F189-B189)+(F189^2+G189^2)*(B189-D189))/AT189</f>
+        <v>2</v>
+      </c>
+      <c r="AW189" s="59">
+        <f>(B189*TAN($O189)+D189*TAN($P189)+F189*TAN($N189))/(TAN($O189)+TAN($P189)+TAN($N189))</f>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="AX189" s="11">
+        <f>(C189*TAN($O189)+E189*TAN($P189)+G189*TAN($N189))/(TAN($O189)+TAN($P189)+TAN($N189))</f>
+        <v>1.8377226823629293E-16</v>
+      </c>
+      <c r="AZ189" s="59">
+        <f>(B189+D189+F189)/3</f>
+        <v>2</v>
+      </c>
+      <c r="BA189" s="66">
+        <f>(C189+E189+G189)/3</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="BB189" t="str">
+        <f>A189</f>
+        <v>Triangle 345</v>
+      </c>
+      <c r="BC189" s="26">
+        <f>H189^2/J189</f>
+        <v>1.8</v>
+      </c>
+      <c r="BD189" s="26">
+        <f>I189^2/J189</f>
+        <v>3.2</v>
+      </c>
+      <c r="BE189">
+        <f>BC189+BD189</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:57" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="84" t="s">
+        <v>143</v>
+      </c>
+      <c r="B190" s="85">
+        <f>B189*3.5</f>
+        <v>0</v>
+      </c>
+      <c r="C190" s="85">
+        <f>C189*3.5</f>
+        <v>0</v>
+      </c>
+      <c r="D190" s="85">
+        <v>10.5</v>
+      </c>
+      <c r="E190" s="85">
+        <f>E189*3.5</f>
+        <v>0</v>
+      </c>
+      <c r="F190" s="85">
+        <v>10.5</v>
+      </c>
+      <c r="G190" s="85">
+        <v>14</v>
+      </c>
+      <c r="H190" s="86">
+        <f>SQRT((B190-D190)^2+(C190-E190)^2)</f>
+        <v>10.5</v>
+      </c>
+      <c r="I190" s="87">
+        <f>SQRT((F190-D190)^2+(G190-E190)^2)</f>
+        <v>14</v>
+      </c>
+      <c r="J190" s="88">
+        <f>SQRT((F190-B190)^2+(G190-C190)^2)</f>
+        <v>17.5</v>
+      </c>
+      <c r="K190" s="89">
+        <f>DEGREES(ACOS((I190^2+J190^2-H190^2)/(2*I190*J190)))</f>
+        <v>36.869897645844013</v>
+      </c>
+      <c r="L190" s="90">
+        <f>DEGREES(ACOS((J190^2+H190^2-I190^2)/(2*J190*H190)))</f>
+        <v>53.13010235415598</v>
+      </c>
+      <c r="M190" s="90">
+        <f>DEGREES(ACOS((I190^2+H190^2-J190^2)/(2*I190*H190)))</f>
+        <v>90</v>
+      </c>
+      <c r="N190" s="91">
+        <f>RADIANS(K190)</f>
+        <v>0.64350110879328426</v>
+      </c>
+      <c r="O190" s="90">
+        <f>RADIANS(L190)</f>
+        <v>0.92729521800161219</v>
+      </c>
+      <c r="P190" s="92">
+        <f>RADIANS(M190)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="Q190" s="93">
+        <f>2*$AL190/H190</f>
+        <v>14</v>
+      </c>
+      <c r="R190" s="94">
+        <f>2*$AL190/I190</f>
+        <v>10.5</v>
+      </c>
+      <c r="S190" s="95">
+        <f>2*$AL190/J190</f>
+        <v>8.4</v>
+      </c>
+      <c r="T190" s="82">
+        <f>(H190*I190/J190)</f>
+        <v>8.4</v>
+      </c>
+      <c r="U190" s="96">
+        <f>0.5*SQRT(2*J190^2+2*I190^2-H190^2)</f>
+        <v>14.952006554305679</v>
+      </c>
+      <c r="V190" s="97">
+        <f>0.5*SQRT(2*J190^2+2*H190^2-I190^2)</f>
+        <v>12.619429464123963</v>
+      </c>
+      <c r="W190" s="98">
+        <f>0.5*SQRT(2*I190^2+2*H190^2-J190^2)</f>
+        <v>8.75</v>
+      </c>
+      <c r="X190" s="96">
+        <f>SQRT(J190*I190*(1-H190^2/(J190+I190)^2))</f>
+        <v>14.757295747452437</v>
+      </c>
+      <c r="Y190" s="94">
+        <f>SQRT(J190*H190*(1-I190^2/(J190+H190)^2))</f>
+        <v>11.739356881873896</v>
+      </c>
+      <c r="Z190" s="98">
+        <f>SQRT(I190*H190*(1-J190^2/(I190+H190)^2))</f>
+        <v>8.4852813742385695</v>
+      </c>
+      <c r="AA190" s="93">
+        <f>MAX(H190:J190)</f>
+        <v>17.5</v>
+      </c>
+      <c r="AB190" s="87">
+        <f>IF(RANK(I190,$H190:$J190)+COUNTIF($H190:I190,I190)-1=2,I190,IF(RANK(J190,$H190:$J190)+COUNTIF($H190:J190,J190)-1=2,J190,H190))</f>
+        <v>14</v>
+      </c>
+      <c r="AC190" s="94">
+        <f>MIN(H190:J190)</f>
+        <v>10.5</v>
+      </c>
+      <c r="AD190" s="99">
+        <f>2*AA190*$AL190/($AA190^2+$AB190^2-$AC190^2)</f>
+        <v>6.5625</v>
+      </c>
+      <c r="AE190" s="87">
+        <f>2*AB190*$AL190/($AA190^2+$AB190^2-$AC190^2)</f>
+        <v>5.25</v>
+      </c>
+      <c r="AF190" s="100">
+        <f>2*AC190*$AL190/($AA190^2-$AB190^2+$AC190^2)</f>
+        <v>7</v>
+      </c>
+      <c r="AG190" s="87">
+        <f>INDEX($AD190:$AF190,1,MATCH(H190,$AA190:$AC190,0))</f>
+        <v>7</v>
+      </c>
+      <c r="AH190" s="87">
+        <f>INDEX($AD190:$AF190,1,MATCH(I190,$AA190:$AC190,0))</f>
+        <v>5.25</v>
+      </c>
+      <c r="AI190" s="88">
+        <f>INDEX($AD190:$AF190,1,MATCH(J190,$AA190:$AC190,0))</f>
+        <v>6.5625</v>
+      </c>
+      <c r="AJ190" s="101">
+        <f>I190+J190+H190</f>
+        <v>42</v>
+      </c>
+      <c r="AK190" s="101">
+        <f>AJ190/2</f>
+        <v>21</v>
+      </c>
+      <c r="AL190" s="101">
+        <f>SQRT(AK190*(AK190-I190)*(AK190-J190)*(AK190-H190))</f>
+        <v>73.5</v>
+      </c>
+      <c r="AM190" s="83">
+        <f>6*(H190/3)^2</f>
+        <v>73.5</v>
+      </c>
+      <c r="AN190" s="102">
+        <f>AL190/AK190</f>
+        <v>3.5</v>
+      </c>
+      <c r="AO190" s="83">
+        <f>1*(H190/3)</f>
+        <v>3.5</v>
+      </c>
+      <c r="AP190" s="87">
+        <f>($I190*B190+$J190*D190+$H190*F190)/$AJ190</f>
+        <v>7</v>
+      </c>
+      <c r="AQ190" s="87">
+        <f>($I190*C190+$J190*E190+$H190*G190)/$AJ190</f>
+        <v>3.5</v>
+      </c>
+      <c r="AR190" s="102">
+        <f>I190*J190*H190/(4*AL190)</f>
+        <v>8.75</v>
+      </c>
+      <c r="AS190" s="83">
+        <f>5/2*(H190/3)</f>
+        <v>8.75</v>
+      </c>
+      <c r="AT190" s="87">
+        <f>2*(B190*(E190-G190)+D190*(G190-C190)+F190*(C190-E190))</f>
+        <v>294</v>
+      </c>
+      <c r="AU190" s="87">
+        <f>((B190^2+C190^2)*(E190-G190)+(D190^2+E190^2)*(G190-C190)+(F190^2+G190^2)*(C190-E190))/AT190</f>
+        <v>5.25</v>
+      </c>
+      <c r="AV190" s="88">
+        <f>-((B190^2+C190^2)*(D190-F190)+(D190^2+E190^2)*(F190-B190)+(F190^2+G190^2)*(B190-D190))/AT190</f>
+        <v>7</v>
+      </c>
+      <c r="AW190" s="86">
+        <f>(B190*TAN($O190)+D190*TAN($P190)+F190*TAN($N190))/(TAN($O190)+TAN($P190)+TAN($N190))</f>
+        <v>10.499999999999998</v>
+      </c>
+      <c r="AX190" s="87">
+        <f>(C190*TAN($O190)+E190*TAN($P190)+G190*TAN($N190))/(TAN($O190)+TAN($P190)+TAN($N190))</f>
+        <v>6.4320293882702521E-16</v>
+      </c>
+      <c r="AZ190" s="86">
+        <f>(B190+D190+F190)/3</f>
+        <v>7</v>
+      </c>
+      <c r="BA190" s="88">
+        <f>(C190+E190+G190)/3</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="BB190" s="84" t="str">
+        <f>A190</f>
+        <v>Triangle 345</v>
+      </c>
+      <c r="BC190" s="26">
+        <f>H190^2/J190</f>
+        <v>6.3</v>
+      </c>
+      <c r="BD190" s="26">
+        <f>I190^2/J190</f>
+        <v>11.2</v>
+      </c>
+      <c r="BE190">
+        <f>BC190+BD190</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>144</v>
+      </c>
+      <c r="B191" s="5">
+        <v>0</v>
+      </c>
+      <c r="C191" s="5">
+        <v>0</v>
+      </c>
+      <c r="D191" s="5">
+        <v>4</v>
+      </c>
+      <c r="E191" s="5">
+        <v>0</v>
+      </c>
+      <c r="F191" s="5">
+        <v>4</v>
+      </c>
+      <c r="G191" s="81">
+        <f>F191/TAN(RADIANS(30))</f>
+        <v>6.9282032302755097</v>
+      </c>
+      <c r="H191" s="59">
+        <f>SQRT((B191-D191)^2+(C191-E191)^2)</f>
+        <v>4</v>
+      </c>
+      <c r="I191" s="11">
+        <f>SQRT((F191-D191)^2+(G191-E191)^2)</f>
+        <v>6.9282032302755097</v>
+      </c>
+      <c r="J191" s="66">
+        <f>SQRT((F191-B191)^2+(G191-C191)^2)</f>
+        <v>8</v>
+      </c>
+      <c r="K191" s="70">
+        <f>DEGREES(ACOS((I191^2+J191^2-H191^2)/(2*I191*J191)))</f>
+        <v>30.000000000000004</v>
+      </c>
+      <c r="L191" s="71">
+        <f>DEGREES(ACOS((J191^2+H191^2-I191^2)/(2*J191*H191)))</f>
+        <v>60.000000000000007</v>
+      </c>
+      <c r="M191" s="71">
+        <f>DEGREES(ACOS((I191^2+H191^2-J191^2)/(2*I191*H191)))</f>
+        <v>90</v>
+      </c>
+      <c r="N191" s="72">
+        <f>RADIANS(K191)</f>
+        <v>0.52359877559829893</v>
+      </c>
+      <c r="O191" s="71">
+        <f>RADIANS(L191)</f>
+        <v>1.0471975511965979</v>
+      </c>
+      <c r="P191" s="73">
+        <f>RADIANS(M191)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="Q191" s="74">
+        <f>2*$AL191/H191</f>
+        <v>6.9282032302755114</v>
+      </c>
+      <c r="R191" s="69">
+        <f>2*$AL191/I191</f>
+        <v>4.0000000000000009</v>
+      </c>
+      <c r="S191" s="75">
+        <f>2*$AL191/J191</f>
+        <v>3.4641016151377557</v>
+      </c>
+      <c r="T191" s="123">
+        <f>H191*I191/J191</f>
+        <v>3.4641016151377548</v>
+      </c>
+      <c r="U191" s="76">
+        <f>0.5*SQRT(2*J191^2+2*I191^2-H191^2)</f>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="V191" s="77">
+        <f>0.5*SQRT(2*J191^2+2*H191^2-I191^2)</f>
+        <v>5.2915026221291814</v>
+      </c>
+      <c r="W191" s="78">
+        <f>0.5*SQRT(2*I191^2+2*H191^2-J191^2)</f>
+        <v>4</v>
+      </c>
+      <c r="X191" s="76">
+        <f>SQRT(J191*I191*(1-H191^2/(J191+I191)^2))</f>
+        <v>7.1726037773444284</v>
+      </c>
+      <c r="Y191" s="69">
+        <f>SQRT(J191*H191*(1-I191^2/(J191+H191)^2))</f>
+        <v>4.6188021535170058</v>
+      </c>
+      <c r="Z191" s="78">
+        <f>SQRT(I191*H191*(1-J191^2/(I191+H191)^2))</f>
+        <v>3.5863018886722147</v>
+      </c>
+      <c r="AA191" s="74">
+        <f>MAX(H191:J191)</f>
+        <v>8</v>
+      </c>
+      <c r="AB191" s="11">
+        <f>IF(RANK(I191,$H191:$J191)+COUNTIF($H191:I191,I191)-1=2,I191,IF(RANK(J191,$H191:$J191)+COUNTIF($H191:J191,J191)-1=2,J191,H191))</f>
+        <v>6.9282032302755097</v>
+      </c>
+      <c r="AC191" s="69">
+        <f>MIN(H191:J191)</f>
+        <v>4</v>
+      </c>
+      <c r="AD191" s="54">
+        <f>2*AA191*$AL191/($AA191^2+$AB191^2-$AC191^2)</f>
+        <v>2.3094010767585038</v>
+      </c>
+      <c r="AE191" s="11">
+        <f>2*AB191*$AL191/($AA191^2+$AB191^2-$AC191^2)</f>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="AF191" s="79">
+        <f>2*AC191*$AL191/($AA191^2-$AB191^2+$AC191^2)</f>
+        <v>3.4641016151377566</v>
+      </c>
+      <c r="AG191" s="11">
+        <f>INDEX($AD191:$AF191,1,MATCH(H191,$AA191:$AC191,0))</f>
+        <v>3.4641016151377566</v>
+      </c>
+      <c r="AH191" s="11">
+        <f>INDEX($AD191:$AF191,1,MATCH(I191,$AA191:$AC191,0))</f>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="AI191" s="66">
+        <f>INDEX($AD191:$AF191,1,MATCH(J191,$AA191:$AC191,0))</f>
+        <v>2.3094010767585038</v>
+      </c>
+      <c r="AJ191" s="21">
+        <f>I191+J191+H191</f>
+        <v>18.928203230275511</v>
+      </c>
+      <c r="AK191" s="32">
+        <f>AJ191/2</f>
+        <v>9.4641016151377553</v>
+      </c>
+      <c r="AL191" s="26">
+        <f>SQRT(AK191*(AK191-I191)*(AK191-J191)*(AK191-H191))</f>
+        <v>13.856406460551023</v>
+      </c>
+      <c r="AM191" s="123">
+        <f>(1/8)*J191^2*SQRT(3)</f>
+        <v>13.856406460551018</v>
+      </c>
+      <c r="AN191" s="80">
+        <f>AL191/AK191</f>
+        <v>1.4641016151377551</v>
+      </c>
+      <c r="AO191" s="13">
+        <f>0.25*J191*(SQRT(3)-1)</f>
+        <v>1.4641016151377544</v>
+      </c>
+      <c r="AP191" s="11">
+        <f>($I191*B191+$J191*D191+$H191*F191)/$AJ191</f>
+        <v>2.5358983848622452</v>
+      </c>
+      <c r="AQ191" s="11">
+        <f>($I191*C191+$J191*E191+$H191*G191)/$AJ191</f>
+        <v>1.4641016151377546</v>
+      </c>
+      <c r="AR191" s="80">
+        <f>I191*J191*H191/(4*AL191)</f>
+        <v>3.9999999999999991</v>
+      </c>
+      <c r="AS191" s="13">
+        <f>0.5*J191</f>
+        <v>4</v>
+      </c>
+      <c r="AT191" s="11">
+        <f>2*(B191*(E191-G191)+D191*(G191-C191)+F191*(C191-E191))</f>
+        <v>55.425625842204077</v>
+      </c>
+      <c r="AU191" s="11">
+        <f>((B191^2+C191^2)*(E191-G191)+(D191^2+E191^2)*(G191-C191)+(F191^2+G191^2)*(C191-E191))/AT191</f>
+        <v>2</v>
+      </c>
+      <c r="AV191" s="66">
+        <f>-((B191^2+C191^2)*(D191-F191)+(D191^2+E191^2)*(F191-B191)+(F191^2+G191^2)*(B191-D191))/AT191</f>
+        <v>3.4641016151377544</v>
+      </c>
+      <c r="AW191" s="59">
+        <f>(B191*TAN($O191)+D191*TAN($P191)+F191*TAN($N191))/(TAN($O191)+TAN($P191)+TAN($N191))</f>
+        <v>3.9999999999999996</v>
+      </c>
+      <c r="AX191" s="11">
+        <f>(C191*TAN($O191)+E191*TAN($P191)+G191*TAN($N191))/(TAN($O191)+TAN($P191)+TAN($N191))</f>
+        <v>2.4502969098172405E-16</v>
+      </c>
+      <c r="AZ191" s="59">
+        <f>(B191+D191+F191)/3</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="BA191" s="66">
+        <f>(C191+E191+G191)/3</f>
+        <v>2.3094010767585034</v>
+      </c>
+      <c r="BB191" t="str">
+        <f>A191</f>
+        <v>Triangle 306090</v>
+      </c>
+      <c r="BC191" s="26">
+        <f>H191^2/J191</f>
+        <v>2</v>
+      </c>
+      <c r="BD191" s="26">
+        <f>I191^2/J191</f>
+        <v>6.0000000000000009</v>
+      </c>
+      <c r="BE191">
+        <f>BC191+BD191</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>145</v>
+      </c>
+      <c r="B192" s="5">
+        <v>4</v>
+      </c>
+      <c r="C192" s="103">
+        <f>(F192/2)*SQRT(3)</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="D192" s="5">
+        <v>0</v>
+      </c>
+      <c r="E192" s="5">
+        <v>0</v>
+      </c>
+      <c r="F192" s="5">
+        <v>8</v>
+      </c>
+      <c r="G192" s="5">
+        <v>0</v>
+      </c>
+      <c r="H192" s="59">
+        <f>SQRT((B192-D192)^2+(C192-E192)^2)</f>
+        <v>8</v>
+      </c>
+      <c r="I192" s="11">
+        <f>SQRT((F192-D192)^2+(G192-E192)^2)</f>
+        <v>8</v>
+      </c>
+      <c r="J192" s="66">
+        <f>SQRT((F192-B192)^2+(G192-C192)^2)</f>
+        <v>8</v>
+      </c>
+      <c r="K192" s="70">
+        <f>DEGREES(ACOS((I192^2+J192^2-H192^2)/(2*I192*J192)))</f>
+        <v>59.999999999999993</v>
+      </c>
+      <c r="L192" s="71">
+        <f>DEGREES(ACOS((J192^2+H192^2-I192^2)/(2*J192*H192)))</f>
+        <v>59.999999999999993</v>
+      </c>
+      <c r="M192" s="71">
+        <f>DEGREES(ACOS((I192^2+H192^2-J192^2)/(2*I192*H192)))</f>
+        <v>59.999999999999993</v>
+      </c>
+      <c r="N192" s="72">
+        <f>RADIANS(K192)</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="O192" s="71">
+        <f>RADIANS(L192)</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="P192" s="73">
+        <f>RADIANS(M192)</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="Q192" s="74">
+        <f>2*$AL192/H192</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="R192" s="69">
+        <f>2*$AL192/I192</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="S192" s="75">
+        <f>2*$AL192/J192</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="T192" s="123">
+        <f>I192*SQRT(3)/2</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="U192" s="76">
+        <f>0.5*SQRT(2*J192^2+2*I192^2-H192^2)</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="V192" s="77">
+        <f>0.5*SQRT(2*J192^2+2*H192^2-I192^2)</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="W192" s="78">
+        <f>0.5*SQRT(2*I192^2+2*H192^2-J192^2)</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="X192" s="76">
+        <f>SQRT(J192*I192*(1-H192^2/(J192+I192)^2))</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="Y192" s="69">
+        <f>SQRT(J192*H192*(1-I192^2/(J192+H192)^2))</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="Z192" s="78">
+        <f>SQRT(I192*H192*(1-J192^2/(I192+H192)^2))</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="AA192" s="74">
+        <f>MAX(H192:J192)</f>
+        <v>8</v>
+      </c>
+      <c r="AB192" s="11">
+        <f>IF(RANK(I192,$H192:$J192)+COUNTIF($H192:I192,I192)-1=2,I192,IF(RANK(J192,$H192:$J192)+COUNTIF($H192:J192,J192)-1=2,J192,H192))</f>
+        <v>8</v>
+      </c>
+      <c r="AC192" s="69">
+        <f>MIN(H192:J192)</f>
+        <v>8</v>
+      </c>
+      <c r="AD192" s="54">
+        <f>2*AA192*$AL192/($AA192^2+$AB192^2-$AC192^2)</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="AE192" s="11">
+        <f>2*AB192*$AL192/($AA192^2+$AB192^2-$AC192^2)</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="AF192" s="79">
+        <f>2*AC192*$AL192/($AA192^2-$AB192^2+$AC192^2)</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="AG192" s="11">
+        <f>INDEX($AD192:$AF192,1,MATCH(H192,$AA192:$AC192,0))</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="AH192" s="11">
+        <f>INDEX($AD192:$AF192,1,MATCH(I192,$AA192:$AC192,0))</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="AI192" s="66">
+        <f>INDEX($AD192:$AF192,1,MATCH(J192,$AA192:$AC192,0))</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="AJ192" s="26">
+        <f>I192+J192+H192</f>
+        <v>24</v>
+      </c>
+      <c r="AK192" s="26">
+        <f>AJ192/2</f>
+        <v>12</v>
+      </c>
+      <c r="AL192" s="26">
+        <f>SQRT(AK192*(AK192-I192)*(AK192-J192)*(AK192-H192))</f>
+        <v>27.712812921102035</v>
+      </c>
+      <c r="AM192" s="13">
+        <f>0.25*I192^2*SQRT(3)</f>
+        <v>27.712812921102035</v>
+      </c>
+      <c r="AN192" s="80">
+        <f>AL192/AK192</f>
+        <v>2.3094010767585029</v>
+      </c>
+      <c r="AO192" s="13">
+        <f>I192*SQRT(3)/6</f>
+        <v>2.3094010767585029</v>
+      </c>
+      <c r="AP192" s="11">
+        <f>($I192*B192+$J192*D192+$H192*F192)/$AJ192</f>
+        <v>4</v>
+      </c>
+      <c r="AQ192" s="11">
+        <f>($I192*C192+$J192*E192+$H192*G192)/$AJ192</f>
+        <v>2.3094010767585029</v>
+      </c>
+      <c r="AR192" s="80">
+        <f>I192*J192*H192/(4*AL192)</f>
+        <v>4.6188021535170067</v>
+      </c>
+      <c r="AS192" s="13">
+        <f>I192/SQRT(3)</f>
+        <v>4.6188021535170067</v>
+      </c>
+      <c r="AT192" s="11">
+        <f>2*(B192*(E192-G192)+D192*(G192-C192)+F192*(C192-E192))</f>
+        <v>110.85125168440814</v>
+      </c>
+      <c r="AU192" s="11">
+        <f>((B192^2+C192^2)*(E192-G192)+(D192^2+E192^2)*(G192-C192)+(F192^2+G192^2)*(C192-E192))/AT192</f>
+        <v>4</v>
+      </c>
+      <c r="AV192" s="66">
+        <f>-((B192^2+C192^2)*(D192-F192)+(D192^2+E192^2)*(F192-B192)+(F192^2+G192^2)*(B192-D192))/AT192</f>
+        <v>2.3094010767585025</v>
+      </c>
+      <c r="AW192" s="59">
+        <f>(B192*TAN($O192)+D192*TAN($P192)+F192*TAN($N192))/(TAN($O192)+TAN($P192)+TAN($N192))</f>
+        <v>4</v>
+      </c>
+      <c r="AX192" s="11">
+        <f>(C192*TAN($O192)+E192*TAN($P192)+G192*TAN($N192))/(TAN($O192)+TAN($P192)+TAN($N192))</f>
+        <v>2.3094010767585029</v>
+      </c>
+      <c r="AZ192" s="59">
+        <f>(B192+D192+F192)/3</f>
+        <v>4</v>
+      </c>
+      <c r="BA192" s="66">
+        <f>(C192+E192+G192)/3</f>
+        <v>2.3094010767585029</v>
+      </c>
+      <c r="BB192" t="str">
+        <f>A192</f>
+        <v>Equilateral Triangle</v>
+      </c>
+    </row>
+    <row r="195" spans="19:19" x14ac:dyDescent="0.3">
+      <c r="S195" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="16">
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="D180:E180"/>
+    <mergeCell ref="F180:G180"/>
+    <mergeCell ref="H180:J180"/>
+    <mergeCell ref="AP180:AQ180"/>
+    <mergeCell ref="AT180:AV180"/>
+    <mergeCell ref="AW180:AX180"/>
+    <mergeCell ref="AZ180:BA180"/>
+    <mergeCell ref="K180:P180"/>
+    <mergeCell ref="Q180:S180"/>
+    <mergeCell ref="U180:W180"/>
+    <mergeCell ref="X180:Z180"/>
+    <mergeCell ref="AA180:AI180"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed testing of Translation, Rotation, Scale transformations for polyline & shape
</commit_message>
<xml_diff>
--- a/docs/Geometry Tests.xlsx
+++ b/docs/Geometry Tests.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\personal\MPT.Net\MPT\Geometry\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F5EF01-BC44-44D7-859E-1DCA878EE2BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03024868-18D8-45A6-BC79-54D894FAF2A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4644" yWindow="1608" windowWidth="16656" windowHeight="10752" tabRatio="824" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extents" sheetId="4" r:id="rId1"/>
     <sheet name="LineSegment" sheetId="12" r:id="rId2"/>
     <sheet name="Shapes" sheetId="13" r:id="rId3"/>
+    <sheet name="Transformations" sheetId="14" r:id="rId4"/>
+    <sheet name="Fillets &amp; Chamfers" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="214">
   <si>
     <t>X</t>
   </si>
@@ -471,6 +473,205 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>Sig Figs</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Value/scale</t>
+  </si>
+  <si>
+    <t>Result w/ round</t>
+  </si>
+  <si>
+    <t>Result w/o round</t>
+  </si>
+  <si>
+    <t>Result w/ round total</t>
+  </si>
+  <si>
+    <t>Value/scale w round</t>
+  </si>
+  <si>
+    <t>Skew</t>
+  </si>
+  <si>
+    <t>Pt 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x </t>
+  </si>
+  <si>
+    <t>Pt 2</t>
+  </si>
+  <si>
+    <t>Pt 3</t>
+  </si>
+  <si>
+    <t>Pt 4</t>
+  </si>
+  <si>
+    <t>Skew X</t>
+  </si>
+  <si>
+    <t>Skew Y</t>
+  </si>
+  <si>
+    <t>lambdaX</t>
+  </si>
+  <si>
+    <t>lambdaY</t>
+  </si>
+  <si>
+    <t>Translate</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Pt 1.5</t>
+  </si>
+  <si>
+    <t>Mirror</t>
+  </si>
+  <si>
+    <t>Delta x</t>
+  </si>
+  <si>
+    <t>Delta y</t>
+  </si>
+  <si>
+    <t>Test Label</t>
+  </si>
+  <si>
+    <t>Negative x</t>
+  </si>
+  <si>
+    <t>Negative y</t>
+  </si>
+  <si>
+    <t>Default in Quadrant II</t>
+  </si>
+  <si>
+    <t>Default in Quadrant III</t>
+  </si>
+  <si>
+    <t>Default in Quadrant IV</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Smaller</t>
+  </si>
+  <si>
+    <t>Default - +x, y, Quadrant I</t>
+  </si>
+  <si>
+    <t>Shear -x</t>
+  </si>
+  <si>
+    <t>Shear +x</t>
+  </si>
+  <si>
+    <t>Shear +y</t>
+  </si>
+  <si>
+    <t>Shear -y</t>
+  </si>
+  <si>
+    <t>Shear +x, +y, Quadrant I</t>
+  </si>
+  <si>
+    <t>Shear +x, +y, Quadrant II</t>
+  </si>
+  <si>
+    <t>Shear +x, +y, Quadrant III</t>
+  </si>
+  <si>
+    <t>Shear +x, +y, Quadrant IV</t>
+  </si>
+  <si>
+    <t>Rotation 
+(degrees)</t>
+  </si>
+  <si>
+    <t>Mirror Pt 1</t>
+  </si>
+  <si>
+    <t>Mirror Pt 2</t>
+  </si>
+  <si>
+    <t>Mirror about y-axis to Quadrant II</t>
+  </si>
+  <si>
+    <t>Mirror about y-axis to Quadrant II, reversed line</t>
+  </si>
+  <si>
+    <t>Mirror about x-axis to Quadrant IV</t>
+  </si>
+  <si>
+    <t>Mirror about x-axis to Quadrant IV, reversed line</t>
+  </si>
+  <si>
+    <t>Mirror about 45 deg sloped line about shape center</t>
+  </si>
+  <si>
+    <t>Mirror about 45 deg sloped line to quadrant III</t>
+  </si>
+  <si>
+    <t>Mirror about 45 deg sloped line about shape center, reversed line</t>
+  </si>
+  <si>
+    <t>Mirror about 45 deg sloped line to quadrant III, reversed line</t>
+  </si>
+  <si>
+    <t>Rotate + to quadrant II</t>
+  </si>
+  <si>
+    <t>Rotate + to quadrant III</t>
+  </si>
+  <si>
+    <t>Rotate + to quadrant IV</t>
+  </si>
+  <si>
+    <t>Rotate + full circle</t>
+  </si>
+  <si>
+    <t>Rotate - to quadrant II</t>
+  </si>
+  <si>
+    <t>Rotate - to quadrant III</t>
+  </si>
+  <si>
+    <t>Rotate - to quadrant IV</t>
+  </si>
+  <si>
+    <t>Rotate - full circle</t>
+  </si>
+  <si>
+    <t>* All transformation tests are about an origin. To do it about an arbitrary point, merely translate origin to arbitrary point, do transformation, then move origin back by original translation</t>
+  </si>
+  <si>
+    <t>Validate these, blue lambdas are suspicious</t>
+  </si>
+  <si>
+    <t>Line Segment</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>Default - larger, Quadrant I</t>
+  </si>
+  <si>
+    <t>PolyLine</t>
   </si>
 </sst>
 </file>
@@ -543,7 +744,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +766,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,7 +944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -857,6 +1064,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -869,7 +1079,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -878,12 +1091,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6159,10 +6388,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E420A0-5044-4817-9532-D9946D0E8FC8}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView topLeftCell="F67" workbookViewId="0">
-      <selection activeCell="K80" sqref="K80"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6500,24 +6730,24 @@
       </c>
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="119" t="s">
+      <c r="A13" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="119"/>
-      <c r="C13" s="119"/>
-      <c r="D13" s="119"/>
-      <c r="E13" s="119"/>
-      <c r="F13" s="119"/>
-      <c r="G13" s="119"/>
-      <c r="H13" s="116" t="s">
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="117"/>
-      <c r="J13" s="117"/>
-      <c r="K13" s="117"/>
-      <c r="L13" s="117"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="118"/>
+      <c r="I13" s="118"/>
+      <c r="J13" s="118"/>
+      <c r="K13" s="118"/>
+      <c r="L13" s="118"/>
+      <c r="M13" s="118"/>
+      <c r="N13" s="119"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -7346,14 +7576,14 @@
       </c>
     </row>
     <row r="37" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O37" s="119" t="s">
+      <c r="O37" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="P37" s="119"/>
-      <c r="Q37" s="119" t="s">
+      <c r="P37" s="115"/>
+      <c r="Q37" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="R37" s="119"/>
+      <c r="R37" s="115"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
@@ -8071,22 +8301,22 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="115" t="s">
+      <c r="A51" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="115"/>
-      <c r="C51" s="115" t="s">
+      <c r="B51" s="116"/>
+      <c r="C51" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="D51" s="115"/>
-      <c r="F51" s="115" t="s">
+      <c r="D51" s="116"/>
+      <c r="F51" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="G51" s="115"/>
-      <c r="H51" s="115" t="s">
+      <c r="G51" s="116"/>
+      <c r="H51" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="I51" s="115"/>
+      <c r="I51" s="116"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
@@ -8146,7 +8376,7 @@
         <v>8</v>
       </c>
       <c r="I53">
-        <f t="shared" ref="I53:I61" si="30">ROUND(B53+((C53-A53)*SIN(E53)+(D53-B53)*COS(E53)),6)</f>
+        <f>ROUND(B53+((C53-A53)*SIN(E53)+(D53-B53)*COS(E53)),6)</f>
         <v>4</v>
       </c>
     </row>
@@ -8180,7 +8410,7 @@
         <v>4.1213199999999999</v>
       </c>
       <c r="I54">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="I53:I61" si="30">ROUND(B54+((C54-A54)*SIN(E54)+(D54-B54)*COS(E54)),6)</f>
         <v>7.3639609999999998</v>
       </c>
     </row>
@@ -8428,22 +8658,22 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="115" t="s">
+      <c r="A64" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="B64" s="115"/>
-      <c r="C64" s="115" t="s">
+      <c r="B64" s="116"/>
+      <c r="C64" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="D64" s="115"/>
-      <c r="F64" s="115" t="s">
+      <c r="D64" s="116"/>
+      <c r="F64" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="G64" s="115"/>
-      <c r="H64" s="115" t="s">
+      <c r="G64" s="116"/>
+      <c r="H64" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="I64" s="115"/>
+      <c r="I64" s="116"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
@@ -8785,26 +9015,26 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="115" t="s">
+      <c r="A77" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="B77" s="115"/>
-      <c r="C77" s="115" t="s">
+      <c r="B77" s="116"/>
+      <c r="C77" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="D77" s="115"/>
-      <c r="E77" s="115" t="s">
+      <c r="D77" s="116"/>
+      <c r="E77" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="F77" s="115"/>
-      <c r="H77" s="115" t="s">
+      <c r="F77" s="116"/>
+      <c r="H77" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="I77" s="115"/>
-      <c r="J77" s="115" t="s">
+      <c r="I77" s="116"/>
+      <c r="J77" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="K77" s="115"/>
+      <c r="K77" s="116"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
@@ -9202,11 +9432,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
     <mergeCell ref="J77:K77"/>
     <mergeCell ref="E77:F77"/>
     <mergeCell ref="H13:N13"/>
@@ -9219,6 +9444,11 @@
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="H77:I77"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -9227,10 +9457,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AE85C4-CC88-430A-A443-610E34209E7B}">
-  <dimension ref="A2:BE195"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A2:BE205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J167" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK159" sqref="AK159"/>
+    <sheetView topLeftCell="A162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U202" sqref="U202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9259,24 +9490,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="E2" s="123" t="s">
+      <c r="E2" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123" t="s">
+      <c r="F2" s="120"/>
+      <c r="G2" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="123"/>
+      <c r="H2" s="120"/>
       <c r="I2" t="s">
         <v>58</v>
       </c>
       <c r="L2" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="123" t="s">
+      <c r="Q2" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="R2" s="123"/>
+      <c r="R2" s="120"/>
       <c r="S2" t="s">
         <v>59</v>
       </c>
@@ -12257,77 +12488,77 @@
       </c>
     </row>
     <row r="180" spans="1:57" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="115" t="s">
+      <c r="B180" s="116" t="s">
         <v>107</v>
       </c>
-      <c r="C180" s="115"/>
-      <c r="D180" s="115" t="s">
+      <c r="C180" s="116"/>
+      <c r="D180" s="116" t="s">
         <v>108</v>
       </c>
-      <c r="E180" s="115"/>
-      <c r="F180" s="115" t="s">
+      <c r="E180" s="116"/>
+      <c r="F180" s="116" t="s">
         <v>109</v>
       </c>
-      <c r="G180" s="115"/>
-      <c r="H180" s="122" t="s">
+      <c r="G180" s="116"/>
+      <c r="H180" s="121" t="s">
         <v>111</v>
       </c>
-      <c r="I180" s="120"/>
-      <c r="J180" s="121"/>
-      <c r="K180" s="122" t="s">
+      <c r="I180" s="122"/>
+      <c r="J180" s="123"/>
+      <c r="K180" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="L180" s="120"/>
-      <c r="M180" s="120"/>
-      <c r="N180" s="120"/>
-      <c r="O180" s="120"/>
-      <c r="P180" s="121"/>
-      <c r="Q180" s="122" t="s">
+      <c r="L180" s="122"/>
+      <c r="M180" s="122"/>
+      <c r="N180" s="122"/>
+      <c r="O180" s="122"/>
+      <c r="P180" s="123"/>
+      <c r="Q180" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="R180" s="120"/>
-      <c r="S180" s="121"/>
-      <c r="U180" s="122" t="s">
+      <c r="R180" s="122"/>
+      <c r="S180" s="123"/>
+      <c r="U180" s="121" t="s">
         <v>116</v>
       </c>
-      <c r="V180" s="120"/>
-      <c r="W180" s="121"/>
-      <c r="X180" s="122" t="s">
+      <c r="V180" s="122"/>
+      <c r="W180" s="123"/>
+      <c r="X180" s="121" t="s">
         <v>117</v>
       </c>
-      <c r="Y180" s="120"/>
-      <c r="Z180" s="121"/>
-      <c r="AA180" s="122" t="s">
+      <c r="Y180" s="122"/>
+      <c r="Z180" s="123"/>
+      <c r="AA180" s="121" t="s">
         <v>121</v>
       </c>
-      <c r="AB180" s="120"/>
-      <c r="AC180" s="120"/>
-      <c r="AD180" s="120"/>
-      <c r="AE180" s="120"/>
-      <c r="AF180" s="120"/>
-      <c r="AG180" s="120"/>
-      <c r="AH180" s="120"/>
-      <c r="AI180" s="121"/>
+      <c r="AB180" s="122"/>
+      <c r="AC180" s="122"/>
+      <c r="AD180" s="122"/>
+      <c r="AE180" s="122"/>
+      <c r="AF180" s="122"/>
+      <c r="AG180" s="122"/>
+      <c r="AH180" s="122"/>
+      <c r="AI180" s="123"/>
       <c r="AN180" s="105"/>
-      <c r="AP180" s="120" t="s">
+      <c r="AP180" s="122" t="s">
         <v>128</v>
       </c>
-      <c r="AQ180" s="120"/>
+      <c r="AQ180" s="122"/>
       <c r="AR180" s="105"/>
-      <c r="AT180" s="120" t="s">
+      <c r="AT180" s="122" t="s">
         <v>129</v>
       </c>
-      <c r="AU180" s="120"/>
-      <c r="AV180" s="121"/>
-      <c r="AW180" s="122" t="s">
+      <c r="AU180" s="122"/>
+      <c r="AV180" s="123"/>
+      <c r="AW180" s="121" t="s">
         <v>130</v>
       </c>
-      <c r="AX180" s="120"/>
+      <c r="AX180" s="122"/>
       <c r="AY180" s="106"/>
-      <c r="AZ180" s="122" t="s">
+      <c r="AZ180" s="121" t="s">
         <v>131</v>
       </c>
-      <c r="BA180" s="121"/>
+      <c r="BA180" s="123"/>
     </row>
     <row r="181" spans="1:57" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B181" s="4" t="s">
@@ -14819,18 +15050,243 @@
         <v>Equilateral Triangle</v>
       </c>
     </row>
-    <row r="195" spans="19:19" x14ac:dyDescent="0.3">
+    <row r="195" spans="19:38" x14ac:dyDescent="0.3">
       <c r="S195" s="24"/>
+    </row>
+    <row r="198" spans="19:38" x14ac:dyDescent="0.3">
+      <c r="Z198" t="s">
+        <v>150</v>
+      </c>
+      <c r="AG198">
+        <v>1.2345E-2</v>
+      </c>
+      <c r="AH198">
+        <v>1.2355E-2</v>
+      </c>
+      <c r="AI198">
+        <v>12.345000000000001</v>
+      </c>
+      <c r="AJ198">
+        <v>1234.5</v>
+      </c>
+      <c r="AK198">
+        <v>1.2345E-6</v>
+      </c>
+      <c r="AL198">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="199" spans="19:38" x14ac:dyDescent="0.3">
+      <c r="X199">
+        <f>0.012355/(0.00001)</f>
+        <v>1235.4999999999998</v>
+      </c>
+      <c r="Z199" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG199">
+        <v>4</v>
+      </c>
+      <c r="AH199">
+        <v>4</v>
+      </c>
+      <c r="AI199">
+        <v>4</v>
+      </c>
+      <c r="AJ199">
+        <v>4</v>
+      </c>
+      <c r="AK199">
+        <v>4</v>
+      </c>
+      <c r="AL199">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="19:38" x14ac:dyDescent="0.3">
+      <c r="X200">
+        <f>0.00001 * ROUND(X199,4)</f>
+        <v>1.2355000000000001E-2</v>
+      </c>
+      <c r="Z200" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG200">
+        <f t="shared" ref="AG200:AL200" si="74">10^(_xlfn.FLOOR.MATH(LOG10(ABS(AG198)))+1-AG199)</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AH200">
+        <f t="shared" si="74"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AI200">
+        <f t="shared" si="74"/>
+        <v>0.01</v>
+      </c>
+      <c r="AJ200">
+        <f t="shared" si="74"/>
+        <v>1</v>
+      </c>
+      <c r="AK200">
+        <f t="shared" si="74"/>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="AL200">
+        <f t="shared" si="74"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="201" spans="19:38" x14ac:dyDescent="0.3">
+      <c r="X201" s="21">
+        <f>0.00001 * ROUND(X199,0)</f>
+        <v>1.2360000000000001E-2</v>
+      </c>
+      <c r="Z201" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG201">
+        <f t="shared" ref="AG201:AL201" si="75">AG198/AG200</f>
+        <v>1234.5</v>
+      </c>
+      <c r="AH201">
+        <f t="shared" si="75"/>
+        <v>1235.4999999999998</v>
+      </c>
+      <c r="AI201">
+        <f t="shared" si="75"/>
+        <v>1234.5</v>
+      </c>
+      <c r="AJ201">
+        <f t="shared" si="75"/>
+        <v>1234.5</v>
+      </c>
+      <c r="AK201">
+        <f t="shared" si="75"/>
+        <v>1234.5</v>
+      </c>
+      <c r="AL201">
+        <f t="shared" si="75"/>
+        <v>1234.5</v>
+      </c>
+    </row>
+    <row r="202" spans="19:38" x14ac:dyDescent="0.3">
+      <c r="Z202" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG202">
+        <f t="shared" ref="AG202:AL202" si="76">AG200*AG201</f>
+        <v>1.2345000000000002E-2</v>
+      </c>
+      <c r="AH202">
+        <f t="shared" si="76"/>
+        <v>1.2354999999999998E-2</v>
+      </c>
+      <c r="AI202">
+        <f t="shared" si="76"/>
+        <v>12.345000000000001</v>
+      </c>
+      <c r="AJ202">
+        <f t="shared" si="76"/>
+        <v>1234.5</v>
+      </c>
+      <c r="AK202">
+        <f t="shared" si="76"/>
+        <v>1.2345E-6</v>
+      </c>
+      <c r="AL202">
+        <f t="shared" si="76"/>
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="203" spans="19:38" x14ac:dyDescent="0.3">
+      <c r="Z203" t="s">
+        <v>155</v>
+      </c>
+      <c r="AG203">
+        <f t="shared" ref="AG203:AL203" si="77">ROUND(AG201,0)</f>
+        <v>1235</v>
+      </c>
+      <c r="AH203">
+        <f t="shared" si="77"/>
+        <v>1236</v>
+      </c>
+      <c r="AI203">
+        <f t="shared" si="77"/>
+        <v>1235</v>
+      </c>
+      <c r="AJ203">
+        <f t="shared" si="77"/>
+        <v>1235</v>
+      </c>
+      <c r="AK203">
+        <f t="shared" si="77"/>
+        <v>1235</v>
+      </c>
+      <c r="AL203">
+        <f t="shared" si="77"/>
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="204" spans="19:38" x14ac:dyDescent="0.3">
+      <c r="Z204" t="s">
+        <v>152</v>
+      </c>
+      <c r="AG204">
+        <f t="shared" ref="AG204:AL204" si="78">AG200*AG203</f>
+        <v>1.2350000000000002E-2</v>
+      </c>
+      <c r="AH204">
+        <f t="shared" si="78"/>
+        <v>1.2360000000000001E-2</v>
+      </c>
+      <c r="AI204">
+        <f t="shared" si="78"/>
+        <v>12.35</v>
+      </c>
+      <c r="AJ204">
+        <f t="shared" si="78"/>
+        <v>1235</v>
+      </c>
+      <c r="AK204">
+        <f t="shared" si="78"/>
+        <v>1.235E-6</v>
+      </c>
+      <c r="AL204">
+        <f t="shared" si="78"/>
+        <v>12350</v>
+      </c>
+    </row>
+    <row r="205" spans="19:38" x14ac:dyDescent="0.3">
+      <c r="Z205" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG205">
+        <f t="shared" ref="AG205:AL205" si="79">ROUND(AG200*AG201,AG199)</f>
+        <v>1.23E-2</v>
+      </c>
+      <c r="AH205">
+        <f t="shared" si="79"/>
+        <v>1.24E-2</v>
+      </c>
+      <c r="AI205">
+        <f t="shared" si="79"/>
+        <v>12.345000000000001</v>
+      </c>
+      <c r="AJ205">
+        <f t="shared" si="79"/>
+        <v>1234.5</v>
+      </c>
+      <c r="AK205">
+        <f t="shared" si="79"/>
+        <v>0</v>
+      </c>
+      <c r="AL205">
+        <f t="shared" si="79"/>
+        <v>12345</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="D180:E180"/>
-    <mergeCell ref="F180:G180"/>
-    <mergeCell ref="H180:J180"/>
     <mergeCell ref="AP180:AQ180"/>
     <mergeCell ref="AT180:AV180"/>
     <mergeCell ref="AW180:AX180"/>
@@ -14840,9 +15296,3701 @@
     <mergeCell ref="U180:W180"/>
     <mergeCell ref="X180:Z180"/>
     <mergeCell ref="AA180:AI180"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="D180:E180"/>
+    <mergeCell ref="F180:G180"/>
+    <mergeCell ref="H180:J180"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2FDBBF9-E775-4B43-A689-615DB15B5682}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:AA57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J25" workbookViewId="0">
+      <selection activeCell="AA39" sqref="AA39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:27" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="125"/>
+      <c r="C3" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="125"/>
+      <c r="E3" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="125"/>
+      <c r="G3" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" s="125"/>
+      <c r="I3" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="K3" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="L3" s="125"/>
+      <c r="M3" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="N3" s="125"/>
+      <c r="O3" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="P3" s="125"/>
+      <c r="Q3" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="R3" s="125"/>
+      <c r="S3" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA3" s="137" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="126">
+        <v>2</v>
+      </c>
+      <c r="C5" s="15">
+        <v>5</v>
+      </c>
+      <c r="D5" s="126">
+        <v>3</v>
+      </c>
+      <c r="E5" s="15">
+        <v>3</v>
+      </c>
+      <c r="F5" s="126">
+        <v>5</v>
+      </c>
+      <c r="G5" s="15">
+        <v>2</v>
+      </c>
+      <c r="H5" s="126">
+        <v>3</v>
+      </c>
+      <c r="I5" s="5">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="128">
+        <f>A5+$I5</f>
+        <v>6</v>
+      </c>
+      <c r="L5" s="129">
+        <f>B5+$J5</f>
+        <v>3</v>
+      </c>
+      <c r="M5" s="128">
+        <f>C5+$I5</f>
+        <v>8</v>
+      </c>
+      <c r="N5" s="129">
+        <f>D5+$J5</f>
+        <v>4</v>
+      </c>
+      <c r="O5" s="128">
+        <f>E5+$I5</f>
+        <v>6</v>
+      </c>
+      <c r="P5" s="129">
+        <f>F5+$J5</f>
+        <v>6</v>
+      </c>
+      <c r="Q5" s="128">
+        <f>G5+$I5</f>
+        <v>5</v>
+      </c>
+      <c r="R5" s="129">
+        <f>H5+$J5</f>
+        <v>4</v>
+      </c>
+      <c r="S5" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z5" t="str">
+        <f>"[TestCase("&amp;A5&amp;", "&amp;B5&amp;", "&amp;C5&amp;", "&amp;D5&amp;", "&amp;E5&amp;", "&amp;F5&amp;", "&amp;I5&amp;", "&amp;J5&amp;", "&amp;K5&amp;", "&amp;L5&amp;", "&amp;M5&amp;", "&amp;N5&amp;", "&amp;O5&amp;", "&amp;P5&amp;")]    // "&amp;S5</f>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 3, 1, 6, 3, 8, 4, 6, 6)]    // Default - +x, y, Quadrant I</v>
+      </c>
+      <c r="AA5" t="str">
+        <f>"[TestCase("&amp;A5&amp;", "&amp;B5&amp;", "&amp;C5&amp;", "&amp;D5&amp;", "&amp;E5&amp;", "&amp;F5&amp;", "&amp;G5&amp;", "&amp;H5&amp;", "&amp;I5&amp;", "&amp;J5&amp;", "&amp;K5&amp;", "&amp;L5&amp;", "&amp;M5&amp;", "&amp;N5&amp;", "&amp;O5&amp;", "&amp;P5&amp;", "&amp;Q5&amp;", "&amp;R5&amp;")]    // "&amp;S5</f>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 2, 3, 3, 1, 6, 3, 8, 4, 6, 6, 5, 4)]    // Default - +x, y, Quadrant I</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="127">
+        <f>A$5</f>
+        <v>3</v>
+      </c>
+      <c r="B6" s="10">
+        <f t="shared" ref="B6:H10" si="0">B$5</f>
+        <v>2</v>
+      </c>
+      <c r="C6" s="127">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E6" s="127">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G6" s="127">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I6" s="5">
+        <v>-3</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+      <c r="K6" s="127">
+        <f t="shared" ref="K6:K10" si="1">A6+$I6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="10">
+        <f t="shared" ref="L6:L10" si="2">B6+$J6</f>
+        <v>3</v>
+      </c>
+      <c r="M6" s="127">
+        <f t="shared" ref="M6:M10" si="3">C6+$I6</f>
+        <v>2</v>
+      </c>
+      <c r="N6" s="10">
+        <f t="shared" ref="N6:N10" si="4">D6+$J6</f>
+        <v>4</v>
+      </c>
+      <c r="O6" s="127">
+        <f t="shared" ref="O6:O10" si="5">E6+$I6</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="10">
+        <f t="shared" ref="P6:P10" si="6">F6+$J6</f>
+        <v>6</v>
+      </c>
+      <c r="Q6" s="127">
+        <f t="shared" ref="Q6:Q10" si="7">G6+$I6</f>
+        <v>-1</v>
+      </c>
+      <c r="R6" s="10">
+        <f t="shared" ref="R6:R10" si="8">H6+$J6</f>
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z6" t="str">
+        <f t="shared" ref="Z6:Z10" si="9">"[TestCase("&amp;A6&amp;", "&amp;B6&amp;", "&amp;C6&amp;", "&amp;D6&amp;", "&amp;E6&amp;", "&amp;F6&amp;", "&amp;I6&amp;", "&amp;J6&amp;", "&amp;K6&amp;", "&amp;L6&amp;", "&amp;M6&amp;", "&amp;N6&amp;", "&amp;O6&amp;", "&amp;P6&amp;")]    // "&amp;S6</f>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, -3, 1, 0, 3, 2, 4, 0, 6)]    // Negative x</v>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" ref="AA6:AA10" si="10">"[TestCase("&amp;A6&amp;", "&amp;B6&amp;", "&amp;C6&amp;", "&amp;D6&amp;", "&amp;E6&amp;", "&amp;F6&amp;", "&amp;G6&amp;", "&amp;H6&amp;", "&amp;I6&amp;", "&amp;J6&amp;", "&amp;K6&amp;", "&amp;L6&amp;", "&amp;M6&amp;", "&amp;N6&amp;", "&amp;O6&amp;", "&amp;P6&amp;", "&amp;Q6&amp;", "&amp;R6&amp;")]    // "&amp;S6</f>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 2, 3, -3, 1, 0, 3, 2, 4, 0, 6, -1, 4)]    // Negative x</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" s="127">
+        <f t="shared" ref="A7:A10" si="11">A$5</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C7" s="127">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E7" s="127">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G7" s="127">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I7" s="5">
+        <v>3</v>
+      </c>
+      <c r="J7" s="5">
+        <v>-1</v>
+      </c>
+      <c r="K7" s="127">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L7" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M7" s="127">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="N7" s="10">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="O7" s="127">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P7" s="10">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="Q7" s="127">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="R7" s="10">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="S7" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z7" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 3, -1, 6, 1, 8, 2, 6, 4)]    // Negative y</v>
+      </c>
+      <c r="AA7" t="str">
+        <f t="shared" si="10"/>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 2, 3, 3, -1, 6, 1, 8, 2, 6, 4, 5, 2)]    // Negative y</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A8" s="127">
+        <f>-A$5</f>
+        <v>-3</v>
+      </c>
+      <c r="B8" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C8" s="127">
+        <f>-C$5</f>
+        <v>-5</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8" s="127">
+        <f>-E$5</f>
+        <v>-3</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="127">
+        <f>-G$5</f>
+        <v>-2</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1</v>
+      </c>
+      <c r="K8" s="127">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M8" s="127">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="N8" s="10">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="O8" s="127">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="10">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="Q8" s="127">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R8" s="10">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="S8" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z8" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(-3, 2, -5, 3, -3, 5, 3, 1, 0, 3, -2, 4, 0, 6)]    // Default in Quadrant II</v>
+      </c>
+      <c r="AA8" t="str">
+        <f t="shared" si="10"/>
+        <v>[TestCase(-3, 2, -5, 3, -3, 5, -2, 3, 3, 1, 0, 3, -2, 4, 0, 6, 1, 4)]    // Default in Quadrant II</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A9" s="127">
+        <f>-A$5</f>
+        <v>-3</v>
+      </c>
+      <c r="B9" s="10">
+        <f>-B$5</f>
+        <v>-2</v>
+      </c>
+      <c r="C9" s="127">
+        <f>-C$5</f>
+        <v>-5</v>
+      </c>
+      <c r="D9" s="10">
+        <f>-D$5</f>
+        <v>-3</v>
+      </c>
+      <c r="E9" s="127">
+        <f>-E$5</f>
+        <v>-3</v>
+      </c>
+      <c r="F9" s="10">
+        <f>-F$5</f>
+        <v>-5</v>
+      </c>
+      <c r="G9" s="127">
+        <f>-G$5</f>
+        <v>-2</v>
+      </c>
+      <c r="H9" s="10">
+        <f>-H$5</f>
+        <v>-3</v>
+      </c>
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
+      <c r="K9" s="127">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="10">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="M9" s="127">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="N9" s="10">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="O9" s="127">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="10">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="Q9" s="127">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R9" s="10">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="S9" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z9" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(-3, -2, -5, -3, -3, -5, 3, 1, 0, -1, -2, -2, 0, -4)]    // Default in Quadrant III</v>
+      </c>
+      <c r="AA9" t="str">
+        <f t="shared" si="10"/>
+        <v>[TestCase(-3, -2, -5, -3, -3, -5, -2, -3, 3, 1, 0, -1, -2, -2, 0, -4, 1, -2)]    // Default in Quadrant III</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A10" s="127">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="B10" s="10">
+        <f>-B$5</f>
+        <v>-2</v>
+      </c>
+      <c r="C10" s="127">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="10">
+        <f>-D$5</f>
+        <v>-3</v>
+      </c>
+      <c r="E10" s="127">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F10" s="10">
+        <f>-F$5</f>
+        <v>-5</v>
+      </c>
+      <c r="G10" s="127">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H10" s="10">
+        <f>-H$5</f>
+        <v>-3</v>
+      </c>
+      <c r="I10" s="5">
+        <v>3</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
+      <c r="K10" s="127">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L10" s="10">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="M10" s="127">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="N10" s="10">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="O10" s="127">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P10" s="10">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="Q10" s="127">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="R10" s="10">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="S10" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z10" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(3, -2, 5, -3, 3, -5, 3, 1, 6, -1, 8, -2, 6, -4)]    // Default in Quadrant IV</v>
+      </c>
+      <c r="AA10" t="str">
+        <f t="shared" si="10"/>
+        <v>[TestCase(3, -2, 5, -3, 3, -5, 2, -3, 3, 1, 6, -1, 8, -2, 6, -4, 5, -2)]    // Default in Quadrant IV</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="125"/>
+      <c r="C13" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="125"/>
+      <c r="E13" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" s="125"/>
+      <c r="G13" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="H13" s="125"/>
+      <c r="I13" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J13" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="K13" s="125"/>
+      <c r="L13" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="M13" s="125"/>
+      <c r="N13" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="O13" s="125"/>
+      <c r="P13" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q13" s="125"/>
+      <c r="R13" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA13" s="137" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="126">
+        <v>2</v>
+      </c>
+      <c r="C15" s="15">
+        <v>5</v>
+      </c>
+      <c r="D15" s="126">
+        <v>3</v>
+      </c>
+      <c r="E15" s="15">
+        <v>3</v>
+      </c>
+      <c r="F15" s="126">
+        <v>5</v>
+      </c>
+      <c r="G15" s="15">
+        <v>2</v>
+      </c>
+      <c r="H15" s="126">
+        <v>3</v>
+      </c>
+      <c r="I15" s="5">
+        <v>2</v>
+      </c>
+      <c r="J15" s="128">
+        <f>A15*$I15</f>
+        <v>6</v>
+      </c>
+      <c r="K15" s="129">
+        <f t="shared" ref="K15:Q15" si="12">B15*$I15</f>
+        <v>4</v>
+      </c>
+      <c r="L15" s="128">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="M15" s="129">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="N15" s="128">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="O15" s="129">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="P15" s="128">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="Q15" s="129">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="R15" t="s">
+        <v>212</v>
+      </c>
+      <c r="Z15" t="str">
+        <f>"[TestCase("&amp;A15&amp;", "&amp;B15&amp;", "&amp;C15&amp;", "&amp;D15&amp;", "&amp;E15&amp;", "&amp;F15&amp;", "&amp;I15&amp;", "&amp;J15&amp;", "&amp;K15&amp;", "&amp;L15&amp;", "&amp;M15&amp;", "&amp;N15&amp;", "&amp;O15&amp;")]    // "&amp;R15</f>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 2, 6, 4, 10, 6, 6, 10)]    // Default - larger, Quadrant I</v>
+      </c>
+      <c r="AA15" t="str">
+        <f>"[TestCase("&amp;A15&amp;", "&amp;B15&amp;", "&amp;C15&amp;", "&amp;D15&amp;", "&amp;E15&amp;", "&amp;F15&amp;", "&amp;G15&amp;", "&amp;H15&amp;", "&amp;I15&amp;", "&amp;J15&amp;", "&amp;K15&amp;", "&amp;L15&amp;", "&amp;M15&amp;", "&amp;N15&amp;", "&amp;O15&amp;", "&amp;P15&amp;", "&amp;Q15&amp;")]    // "&amp;R15</f>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 2, 3, 2, 6, 4, 10, 6, 6, 10, 4, 6)]    // Default - larger, Quadrant I</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A16" s="127">
+        <f>A$15</f>
+        <v>3</v>
+      </c>
+      <c r="B16" s="10">
+        <f t="shared" ref="B16:H18" si="13">B$15</f>
+        <v>2</v>
+      </c>
+      <c r="C16" s="127">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="D16" s="10">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="E16" s="127">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="G16" s="127">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="128">
+        <f t="shared" ref="J16:J18" si="14">A16*$I16</f>
+        <v>1.5</v>
+      </c>
+      <c r="K16" s="129">
+        <f t="shared" ref="K16:K18" si="15">B16*$I16</f>
+        <v>1</v>
+      </c>
+      <c r="L16" s="128">
+        <f t="shared" ref="L16:L18" si="16">C16*$I16</f>
+        <v>2.5</v>
+      </c>
+      <c r="M16" s="129">
+        <f t="shared" ref="M16:M18" si="17">D16*$I16</f>
+        <v>1.5</v>
+      </c>
+      <c r="N16" s="128">
+        <f t="shared" ref="N16:N18" si="18">E16*$I16</f>
+        <v>1.5</v>
+      </c>
+      <c r="O16" s="129">
+        <f t="shared" ref="O16:O18" si="19">F16*$I16</f>
+        <v>2.5</v>
+      </c>
+      <c r="P16" s="128">
+        <f t="shared" ref="P16:P18" si="20">G16*$I16</f>
+        <v>1</v>
+      </c>
+      <c r="Q16" s="129">
+        <f t="shared" ref="Q16:Q18" si="21">H16*$I16</f>
+        <v>1.5</v>
+      </c>
+      <c r="R16" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z16" t="str">
+        <f t="shared" ref="Z16:Z21" si="22">"[TestCase("&amp;A16&amp;", "&amp;B16&amp;", "&amp;C16&amp;", "&amp;D16&amp;", "&amp;E16&amp;", "&amp;F16&amp;", "&amp;I16&amp;", "&amp;J16&amp;", "&amp;K16&amp;", "&amp;L16&amp;", "&amp;M16&amp;", "&amp;N16&amp;", "&amp;O16&amp;")]    // "&amp;R16</f>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 0.5, 1.5, 1, 2.5, 1.5, 1.5, 2.5)]    // Smaller</v>
+      </c>
+      <c r="AA16" t="str">
+        <f t="shared" ref="AA16:AA21" si="23">"[TestCase("&amp;A16&amp;", "&amp;B16&amp;", "&amp;C16&amp;", "&amp;D16&amp;", "&amp;E16&amp;", "&amp;F16&amp;", "&amp;G16&amp;", "&amp;H16&amp;", "&amp;I16&amp;", "&amp;J16&amp;", "&amp;K16&amp;", "&amp;L16&amp;", "&amp;M16&amp;", "&amp;N16&amp;", "&amp;O16&amp;", "&amp;P16&amp;", "&amp;Q16&amp;")]    // "&amp;R16</f>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 2, 3, 0.5, 1.5, 1, 2.5, 1.5, 1.5, 2.5, 1, 1.5)]    // Smaller</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A17" s="127">
+        <f t="shared" ref="A17:A18" si="24">A$15</f>
+        <v>3</v>
+      </c>
+      <c r="B17" s="10">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="C17" s="127">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="D17" s="10">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="E17" s="127">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="G17" s="127">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="I17" s="5">
+        <v>-2</v>
+      </c>
+      <c r="J17" s="128">
+        <f t="shared" si="14"/>
+        <v>-6</v>
+      </c>
+      <c r="K17" s="129">
+        <f t="shared" si="15"/>
+        <v>-4</v>
+      </c>
+      <c r="L17" s="128">
+        <f t="shared" si="16"/>
+        <v>-10</v>
+      </c>
+      <c r="M17" s="129">
+        <f t="shared" si="17"/>
+        <v>-6</v>
+      </c>
+      <c r="N17" s="128">
+        <f t="shared" si="18"/>
+        <v>-6</v>
+      </c>
+      <c r="O17" s="129">
+        <f t="shared" si="19"/>
+        <v>-10</v>
+      </c>
+      <c r="P17" s="128">
+        <f t="shared" si="20"/>
+        <v>-4</v>
+      </c>
+      <c r="Q17" s="129">
+        <f t="shared" si="21"/>
+        <v>-6</v>
+      </c>
+      <c r="R17" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z17" t="str">
+        <f t="shared" si="22"/>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, -2, -6, -4, -10, -6, -6, -10)]    // Negative</v>
+      </c>
+      <c r="AA17" t="str">
+        <f t="shared" si="23"/>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 2, 3, -2, -6, -4, -10, -6, -6, -10, -4, -6)]    // Negative</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A18" s="127">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+      <c r="B18" s="10">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="C18" s="127">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="E18" s="127">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="G18" s="127">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="128">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="128">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="129">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="128">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="129">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="128">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="129">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="str">
+        <f t="shared" si="22"/>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 0, 0, 0, 0, 0, 0, 0)]    // 0</v>
+      </c>
+      <c r="AA18" t="str">
+        <f t="shared" si="23"/>
+        <v>[TestCase(3, 2, 5, 3, 3, 5, 2, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0)]    // 0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A19" s="127">
+        <f>-A$5</f>
+        <v>-3</v>
+      </c>
+      <c r="B19" s="10">
+        <f t="shared" ref="B19:H21" si="25">B$5</f>
+        <v>2</v>
+      </c>
+      <c r="C19" s="127">
+        <f>-C$5</f>
+        <v>-5</v>
+      </c>
+      <c r="D19" s="10">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="E19" s="127">
+        <f>-E$5</f>
+        <v>-3</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="25"/>
+        <v>5</v>
+      </c>
+      <c r="G19" s="127">
+        <f>-G$5</f>
+        <v>-2</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="I19" s="5">
+        <v>2</v>
+      </c>
+      <c r="J19" s="128">
+        <f t="shared" ref="J19:J21" si="26">A19*$I19</f>
+        <v>-6</v>
+      </c>
+      <c r="K19" s="129">
+        <f t="shared" ref="K19:K21" si="27">B19*$I19</f>
+        <v>4</v>
+      </c>
+      <c r="L19" s="128">
+        <f t="shared" ref="L19:L21" si="28">C19*$I19</f>
+        <v>-10</v>
+      </c>
+      <c r="M19" s="129">
+        <f t="shared" ref="M19:M21" si="29">D19*$I19</f>
+        <v>6</v>
+      </c>
+      <c r="N19" s="128">
+        <f t="shared" ref="N19:N21" si="30">E19*$I19</f>
+        <v>-6</v>
+      </c>
+      <c r="O19" s="129">
+        <f t="shared" ref="O19:O21" si="31">F19*$I19</f>
+        <v>10</v>
+      </c>
+      <c r="P19" s="128">
+        <f t="shared" ref="P19:P21" si="32">G19*$I19</f>
+        <v>-4</v>
+      </c>
+      <c r="Q19" s="129">
+        <f t="shared" ref="Q19:Q21" si="33">H19*$I19</f>
+        <v>6</v>
+      </c>
+      <c r="R19" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z19" t="str">
+        <f t="shared" si="22"/>
+        <v>[TestCase(-3, 2, -5, 3, -3, 5, 2, -6, 4, -10, 6, -6, 10)]    // Default in Quadrant II</v>
+      </c>
+      <c r="AA19" t="str">
+        <f t="shared" si="23"/>
+        <v>[TestCase(-3, 2, -5, 3, -3, 5, -2, 3, 2, -6, 4, -10, 6, -6, 10, -4, 6)]    // Default in Quadrant II</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A20" s="127">
+        <f>-A$5</f>
+        <v>-3</v>
+      </c>
+      <c r="B20" s="10">
+        <f>-B$5</f>
+        <v>-2</v>
+      </c>
+      <c r="C20" s="127">
+        <f>-C$5</f>
+        <v>-5</v>
+      </c>
+      <c r="D20" s="10">
+        <f>-D$5</f>
+        <v>-3</v>
+      </c>
+      <c r="E20" s="127">
+        <f>-E$5</f>
+        <v>-3</v>
+      </c>
+      <c r="F20" s="10">
+        <f>-F$5</f>
+        <v>-5</v>
+      </c>
+      <c r="G20" s="127">
+        <f>-G$5</f>
+        <v>-2</v>
+      </c>
+      <c r="H20" s="10">
+        <f>-H$5</f>
+        <v>-3</v>
+      </c>
+      <c r="I20" s="5">
+        <v>2</v>
+      </c>
+      <c r="J20" s="128">
+        <f t="shared" si="26"/>
+        <v>-6</v>
+      </c>
+      <c r="K20" s="129">
+        <f t="shared" si="27"/>
+        <v>-4</v>
+      </c>
+      <c r="L20" s="128">
+        <f t="shared" si="28"/>
+        <v>-10</v>
+      </c>
+      <c r="M20" s="129">
+        <f t="shared" si="29"/>
+        <v>-6</v>
+      </c>
+      <c r="N20" s="128">
+        <f t="shared" si="30"/>
+        <v>-6</v>
+      </c>
+      <c r="O20" s="129">
+        <f t="shared" si="31"/>
+        <v>-10</v>
+      </c>
+      <c r="P20" s="128">
+        <f t="shared" si="32"/>
+        <v>-4</v>
+      </c>
+      <c r="Q20" s="129">
+        <f t="shared" si="33"/>
+        <v>-6</v>
+      </c>
+      <c r="R20" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z20" t="str">
+        <f t="shared" si="22"/>
+        <v>[TestCase(-3, -2, -5, -3, -3, -5, 2, -6, -4, -10, -6, -6, -10)]    // Default in Quadrant III</v>
+      </c>
+      <c r="AA20" t="str">
+        <f t="shared" si="23"/>
+        <v>[TestCase(-3, -2, -5, -3, -3, -5, -2, -3, 2, -6, -4, -10, -6, -6, -10, -4, -6)]    // Default in Quadrant III</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A21" s="127">
+        <f t="shared" ref="A21" si="34">A$5</f>
+        <v>3</v>
+      </c>
+      <c r="B21" s="10">
+        <f>-B$5</f>
+        <v>-2</v>
+      </c>
+      <c r="C21" s="127">
+        <f t="shared" si="25"/>
+        <v>5</v>
+      </c>
+      <c r="D21" s="10">
+        <f>-D$5</f>
+        <v>-3</v>
+      </c>
+      <c r="E21" s="127">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="F21" s="10">
+        <f>-F$5</f>
+        <v>-5</v>
+      </c>
+      <c r="G21" s="127">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="H21" s="10">
+        <f>-H$5</f>
+        <v>-3</v>
+      </c>
+      <c r="I21" s="5">
+        <v>2</v>
+      </c>
+      <c r="J21" s="128">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="K21" s="129">
+        <f t="shared" si="27"/>
+        <v>-4</v>
+      </c>
+      <c r="L21" s="128">
+        <f t="shared" si="28"/>
+        <v>10</v>
+      </c>
+      <c r="M21" s="129">
+        <f t="shared" si="29"/>
+        <v>-6</v>
+      </c>
+      <c r="N21" s="128">
+        <f t="shared" si="30"/>
+        <v>6</v>
+      </c>
+      <c r="O21" s="129">
+        <f t="shared" si="31"/>
+        <v>-10</v>
+      </c>
+      <c r="P21" s="128">
+        <f t="shared" si="32"/>
+        <v>4</v>
+      </c>
+      <c r="Q21" s="129">
+        <f t="shared" si="33"/>
+        <v>-6</v>
+      </c>
+      <c r="R21" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z21" t="str">
+        <f t="shared" si="22"/>
+        <v>[TestCase(3, -2, 5, -3, 3, -5, 2, 6, -4, 10, -6, 6, -10)]    // Default in Quadrant IV</v>
+      </c>
+      <c r="AA21" t="str">
+        <f t="shared" si="23"/>
+        <v>[TestCase(3, -2, 5, -3, 3, -5, 2, -3, 2, 6, -4, 10, -6, 6, -10, 4, -6)]    // Default in Quadrant IV</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="125"/>
+      <c r="C24" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="125"/>
+      <c r="E24" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="F24" s="125"/>
+      <c r="G24" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="H24" s="125"/>
+      <c r="I24" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M24" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="N24" s="125"/>
+      <c r="O24" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="P24" s="125"/>
+      <c r="Q24" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="R24" s="125"/>
+      <c r="S24" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="T24" s="125"/>
+      <c r="U24" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z24" s="136" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA24" s="136" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="T25" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A26" s="15">
+        <v>3</v>
+      </c>
+      <c r="B26" s="126">
+        <v>2</v>
+      </c>
+      <c r="C26" s="15">
+        <v>5</v>
+      </c>
+      <c r="D26" s="126">
+        <v>3</v>
+      </c>
+      <c r="E26" s="15">
+        <v>3</v>
+      </c>
+      <c r="F26" s="126">
+        <v>5</v>
+      </c>
+      <c r="G26" s="15">
+        <v>2</v>
+      </c>
+      <c r="H26" s="126">
+        <v>3</v>
+      </c>
+      <c r="I26" s="5">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <f>I26/MAX(B26,D26,F26,H26)</f>
+        <v>0.4</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>K26/MAX(A26,C26,E26,G26)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="128">
+        <f>A26+$J26*B26</f>
+        <v>3.8</v>
+      </c>
+      <c r="N26" s="129">
+        <f>B26+$L26*A26</f>
+        <v>2</v>
+      </c>
+      <c r="O26" s="128">
+        <f>C26+$J26*D26</f>
+        <v>6.2</v>
+      </c>
+      <c r="P26" s="129">
+        <f>D26+$L26*C26</f>
+        <v>3</v>
+      </c>
+      <c r="Q26" s="128">
+        <f>E26+$J26*F26</f>
+        <v>5</v>
+      </c>
+      <c r="R26" s="129">
+        <f>F26+$L26*E26</f>
+        <v>5</v>
+      </c>
+      <c r="S26" s="128">
+        <f>G26+$J26*H26</f>
+        <v>3.2</v>
+      </c>
+      <c r="T26" s="129">
+        <f>H26+$L26*G26</f>
+        <v>3</v>
+      </c>
+      <c r="U26" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z26" t="str">
+        <f>"[TestCase("&amp;A26&amp;", "&amp;B26&amp;", "&amp;C26&amp;", "&amp;D26&amp;", "&amp;I26&amp;", "&amp;K26&amp;", "&amp;M26&amp;", "&amp;N26&amp;", "&amp;O26&amp;", "&amp;P26&amp;")]    // "&amp;U26</f>
+        <v>[TestCase(3, 2, 5, 3, 2, 0, 3.8, 2, 6.2, 3)]    // Shear +x</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A27" s="127">
+        <f>A$26</f>
+        <v>3</v>
+      </c>
+      <c r="B27" s="10">
+        <f>B$26</f>
+        <v>2</v>
+      </c>
+      <c r="C27" s="127">
+        <f>C$26</f>
+        <v>5</v>
+      </c>
+      <c r="D27" s="10">
+        <f>D$26</f>
+        <v>3</v>
+      </c>
+      <c r="E27" s="127">
+        <f>E$26</f>
+        <v>3</v>
+      </c>
+      <c r="F27" s="10">
+        <f>F$26</f>
+        <v>5</v>
+      </c>
+      <c r="G27" s="127">
+        <f>G$26</f>
+        <v>2</v>
+      </c>
+      <c r="H27" s="10">
+        <f>H$26</f>
+        <v>3</v>
+      </c>
+      <c r="I27" s="5">
+        <v>-2</v>
+      </c>
+      <c r="J27">
+        <f>I27/MAX(B27,D27,F27,H27)</f>
+        <v>-0.4</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>K27/MAX(A27,C27,E27,G27)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="127">
+        <f>A27+$J27*B27</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N27" s="10">
+        <f>B27+$L27*A27</f>
+        <v>2</v>
+      </c>
+      <c r="O27" s="127">
+        <f>C27+$J27*D27</f>
+        <v>3.8</v>
+      </c>
+      <c r="P27" s="10">
+        <f>D27+$L27*C27</f>
+        <v>3</v>
+      </c>
+      <c r="Q27" s="127">
+        <f>E27+$J27*F27</f>
+        <v>1</v>
+      </c>
+      <c r="R27" s="10">
+        <f>F27+$L27*E27</f>
+        <v>5</v>
+      </c>
+      <c r="S27" s="127">
+        <f>G27+$J27*H27</f>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="T27" s="10">
+        <f>H27+$L27*G27</f>
+        <v>3</v>
+      </c>
+      <c r="U27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A28" s="127">
+        <f>A$26</f>
+        <v>3</v>
+      </c>
+      <c r="B28" s="10">
+        <f>B$26</f>
+        <v>2</v>
+      </c>
+      <c r="C28" s="127">
+        <f>C$26</f>
+        <v>5</v>
+      </c>
+      <c r="D28" s="10">
+        <f>D$26</f>
+        <v>3</v>
+      </c>
+      <c r="E28" s="127">
+        <f>E$26</f>
+        <v>3</v>
+      </c>
+      <c r="F28" s="10">
+        <f>F$26</f>
+        <v>5</v>
+      </c>
+      <c r="G28" s="127">
+        <f>G$26</f>
+        <v>2</v>
+      </c>
+      <c r="H28" s="10">
+        <f>H$26</f>
+        <v>3</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f>I28/MAX(B28,D28,F28,H28)</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="5">
+        <v>2</v>
+      </c>
+      <c r="L28">
+        <f>K28/MAX(A28,C28,E28,G28)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M28" s="127">
+        <f>A28+$J28*B28</f>
+        <v>3</v>
+      </c>
+      <c r="N28" s="10">
+        <f>B28+$L28*A28</f>
+        <v>3.2</v>
+      </c>
+      <c r="O28" s="127">
+        <f>C28+$J28*D28</f>
+        <v>5</v>
+      </c>
+      <c r="P28" s="10">
+        <f>D28+$L28*C28</f>
+        <v>5</v>
+      </c>
+      <c r="Q28" s="127">
+        <f>E28+$J28*F28</f>
+        <v>3</v>
+      </c>
+      <c r="R28" s="10">
+        <f>F28+$L28*E28</f>
+        <v>6.2</v>
+      </c>
+      <c r="S28" s="127">
+        <f>G28+$J28*H28</f>
+        <v>2</v>
+      </c>
+      <c r="T28" s="10">
+        <f>H28+$L28*G28</f>
+        <v>3.8</v>
+      </c>
+      <c r="U28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A29" s="127">
+        <f>A$26</f>
+        <v>3</v>
+      </c>
+      <c r="B29" s="10">
+        <f>B$26</f>
+        <v>2</v>
+      </c>
+      <c r="C29" s="127">
+        <f>C$26</f>
+        <v>5</v>
+      </c>
+      <c r="D29" s="10">
+        <f>D$26</f>
+        <v>3</v>
+      </c>
+      <c r="E29" s="127">
+        <f>E$26</f>
+        <v>3</v>
+      </c>
+      <c r="F29" s="10">
+        <f>F$26</f>
+        <v>5</v>
+      </c>
+      <c r="G29" s="127">
+        <f>G$26</f>
+        <v>2</v>
+      </c>
+      <c r="H29" s="10">
+        <f>H$26</f>
+        <v>3</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f>I29/MAX(B29,D29,F29,H29)</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="5">
+        <v>-2</v>
+      </c>
+      <c r="L29">
+        <f>K29/MAX(A29,C29,E29,G29)</f>
+        <v>-0.4</v>
+      </c>
+      <c r="M29" s="127">
+        <f>A29+$J29*B29</f>
+        <v>3</v>
+      </c>
+      <c r="N29" s="10">
+        <f>B29+$L29*A29</f>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="O29" s="127">
+        <f>C29+$J29*D29</f>
+        <v>5</v>
+      </c>
+      <c r="P29" s="10">
+        <f>D29+$L29*C29</f>
+        <v>1</v>
+      </c>
+      <c r="Q29" s="127">
+        <f>E29+$J29*F29</f>
+        <v>3</v>
+      </c>
+      <c r="R29" s="10">
+        <f>F29+$L29*E29</f>
+        <v>3.8</v>
+      </c>
+      <c r="S29" s="127">
+        <f>G29+$J29*H29</f>
+        <v>2</v>
+      </c>
+      <c r="T29" s="10">
+        <f>H29+$L29*G29</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A30" s="127">
+        <f>A$26</f>
+        <v>3</v>
+      </c>
+      <c r="B30" s="10">
+        <f>B$26</f>
+        <v>2</v>
+      </c>
+      <c r="C30" s="127">
+        <f>C$26</f>
+        <v>5</v>
+      </c>
+      <c r="D30" s="10">
+        <f>D$26</f>
+        <v>3</v>
+      </c>
+      <c r="E30" s="127">
+        <f>E$26</f>
+        <v>3</v>
+      </c>
+      <c r="F30" s="10">
+        <f>F$26</f>
+        <v>5</v>
+      </c>
+      <c r="G30" s="127">
+        <f>G$26</f>
+        <v>2</v>
+      </c>
+      <c r="H30" s="10">
+        <f>H$26</f>
+        <v>3</v>
+      </c>
+      <c r="I30" s="5">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <f>I30/MAX(B30,D30,F30,H30)</f>
+        <v>0.4</v>
+      </c>
+      <c r="K30" s="5">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <f>K30/MAX(A30,C30,E30,G30)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M30" s="127">
+        <f>A30+$J30*B30</f>
+        <v>3.8</v>
+      </c>
+      <c r="N30" s="10">
+        <f>B30+$L30*A30</f>
+        <v>3.8</v>
+      </c>
+      <c r="O30" s="127">
+        <f>C30+$J30*D30</f>
+        <v>6.2</v>
+      </c>
+      <c r="P30" s="10">
+        <f>D30+$L30*C30</f>
+        <v>6</v>
+      </c>
+      <c r="Q30" s="127">
+        <f>E30+$J30*F30</f>
+        <v>5</v>
+      </c>
+      <c r="R30" s="10">
+        <f>F30+$L30*E30</f>
+        <v>6.8</v>
+      </c>
+      <c r="S30" s="127">
+        <f>G30+$J30*H30</f>
+        <v>3.2</v>
+      </c>
+      <c r="T30" s="10">
+        <f>H30+$L30*G30</f>
+        <v>4.2</v>
+      </c>
+      <c r="U30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A31" s="127">
+        <f>-A$5</f>
+        <v>-3</v>
+      </c>
+      <c r="B31" s="10">
+        <f t="shared" ref="B31:H33" si="35">B$5</f>
+        <v>2</v>
+      </c>
+      <c r="C31" s="127">
+        <f>-C$5</f>
+        <v>-5</v>
+      </c>
+      <c r="D31" s="10">
+        <f t="shared" si="35"/>
+        <v>3</v>
+      </c>
+      <c r="E31" s="127">
+        <f>-E$5</f>
+        <v>-3</v>
+      </c>
+      <c r="F31" s="10">
+        <f t="shared" si="35"/>
+        <v>5</v>
+      </c>
+      <c r="G31" s="127">
+        <f>-G$5</f>
+        <v>-2</v>
+      </c>
+      <c r="H31" s="10">
+        <f t="shared" si="35"/>
+        <v>3</v>
+      </c>
+      <c r="I31" s="5">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <f>I31/MAX(B31,D31,F31,H31)</f>
+        <v>0.4</v>
+      </c>
+      <c r="K31" s="5">
+        <v>3</v>
+      </c>
+      <c r="L31" s="131">
+        <f>K31/MAX(A31,C31,E31,G31)</f>
+        <v>-1.5</v>
+      </c>
+      <c r="M31" s="127">
+        <f>A31+$J31*B31</f>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="N31" s="10">
+        <f>B31+$L31*A31</f>
+        <v>6.5</v>
+      </c>
+      <c r="O31" s="127">
+        <f>C31+$J31*D31</f>
+        <v>-3.8</v>
+      </c>
+      <c r="P31" s="10">
+        <f>D31+$L31*C31</f>
+        <v>10.5</v>
+      </c>
+      <c r="Q31" s="127">
+        <f>E31+$J31*F31</f>
+        <v>-1</v>
+      </c>
+      <c r="R31" s="10">
+        <f>F31+$L31*E31</f>
+        <v>9.5</v>
+      </c>
+      <c r="S31" s="127">
+        <f>G31+$J31*H31</f>
+        <v>-0.79999999999999982</v>
+      </c>
+      <c r="T31" s="10">
+        <f>H31+$L31*G31</f>
+        <v>6</v>
+      </c>
+      <c r="U31" t="s">
+        <v>186</v>
+      </c>
+      <c r="W31" s="131" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A32" s="127">
+        <f>-A$5</f>
+        <v>-3</v>
+      </c>
+      <c r="B32" s="10">
+        <f>-B$5</f>
+        <v>-2</v>
+      </c>
+      <c r="C32" s="127">
+        <f>-C$5</f>
+        <v>-5</v>
+      </c>
+      <c r="D32" s="10">
+        <f>-D$5</f>
+        <v>-3</v>
+      </c>
+      <c r="E32" s="127">
+        <f>-E$5</f>
+        <v>-3</v>
+      </c>
+      <c r="F32" s="10">
+        <f>-F$5</f>
+        <v>-5</v>
+      </c>
+      <c r="G32" s="127">
+        <f>-G$5</f>
+        <v>-2</v>
+      </c>
+      <c r="H32" s="10">
+        <f>-H$5</f>
+        <v>-3</v>
+      </c>
+      <c r="I32" s="5">
+        <v>2</v>
+      </c>
+      <c r="J32" s="131">
+        <f>I32/MAX(B32,D32,F32,H32)</f>
+        <v>-1</v>
+      </c>
+      <c r="K32" s="5">
+        <v>3</v>
+      </c>
+      <c r="L32" s="131">
+        <f>K32/MAX(A32,C32,E32,G32)</f>
+        <v>-1.5</v>
+      </c>
+      <c r="M32" s="127">
+        <f>A32+$J32*B32</f>
+        <v>-1</v>
+      </c>
+      <c r="N32" s="10">
+        <f>B32+$L32*A32</f>
+        <v>2.5</v>
+      </c>
+      <c r="O32" s="127">
+        <f>C32+$J32*D32</f>
+        <v>-2</v>
+      </c>
+      <c r="P32" s="10">
+        <f>D32+$L32*C32</f>
+        <v>4.5</v>
+      </c>
+      <c r="Q32" s="127">
+        <f>E32+$J32*F32</f>
+        <v>2</v>
+      </c>
+      <c r="R32" s="10">
+        <f>F32+$L32*E32</f>
+        <v>-0.5</v>
+      </c>
+      <c r="S32" s="127">
+        <f>G32+$J32*H32</f>
+        <v>1</v>
+      </c>
+      <c r="T32" s="10">
+        <f>H32+$L32*G32</f>
+        <v>0</v>
+      </c>
+      <c r="U32" t="s">
+        <v>187</v>
+      </c>
+      <c r="W32" s="131" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A33" s="127">
+        <f t="shared" ref="A33" si="36">A$5</f>
+        <v>3</v>
+      </c>
+      <c r="B33" s="10">
+        <f>-B$5</f>
+        <v>-2</v>
+      </c>
+      <c r="C33" s="127">
+        <f t="shared" si="35"/>
+        <v>5</v>
+      </c>
+      <c r="D33" s="10">
+        <f>-D$5</f>
+        <v>-3</v>
+      </c>
+      <c r="E33" s="127">
+        <f t="shared" si="35"/>
+        <v>3</v>
+      </c>
+      <c r="F33" s="10">
+        <f>-F$5</f>
+        <v>-5</v>
+      </c>
+      <c r="G33" s="127">
+        <f t="shared" si="35"/>
+        <v>2</v>
+      </c>
+      <c r="H33" s="10">
+        <f>-H$5</f>
+        <v>-3</v>
+      </c>
+      <c r="I33" s="5">
+        <v>2</v>
+      </c>
+      <c r="J33" s="131">
+        <f>I33/MAX(B33,D33,F33,H33)</f>
+        <v>-1</v>
+      </c>
+      <c r="K33" s="5">
+        <v>3</v>
+      </c>
+      <c r="L33" s="131">
+        <f>K33/MAX(A33,C33,E33,G33)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M33" s="127">
+        <f>A33+$J33*B33</f>
+        <v>5</v>
+      </c>
+      <c r="N33" s="10">
+        <f>B33+$L33*A33</f>
+        <v>-0.20000000000000018</v>
+      </c>
+      <c r="O33" s="127">
+        <f>C33+$J33*D33</f>
+        <v>8</v>
+      </c>
+      <c r="P33" s="10">
+        <f>D33+$L33*C33</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="127">
+        <f>E33+$J33*F33</f>
+        <v>8</v>
+      </c>
+      <c r="R33" s="10">
+        <f>F33+$L33*E33</f>
+        <v>-3.2</v>
+      </c>
+      <c r="S33" s="127">
+        <f>G33+$J33*H33</f>
+        <v>5</v>
+      </c>
+      <c r="T33" s="10">
+        <f>H33+$L33*G33</f>
+        <v>-1.8</v>
+      </c>
+      <c r="U33" t="s">
+        <v>188</v>
+      </c>
+      <c r="W33" s="131" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36" s="125"/>
+      <c r="C36" s="124" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36" s="125"/>
+      <c r="E36" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="F36" s="125"/>
+      <c r="G36" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="125"/>
+      <c r="I36" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="J36" s="125"/>
+      <c r="K36" s="130" t="s">
+        <v>189</v>
+      </c>
+      <c r="L36" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="M36" s="125"/>
+      <c r="N36" s="124" t="s">
+        <v>168</v>
+      </c>
+      <c r="O36" s="125"/>
+      <c r="P36" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q36" s="125"/>
+      <c r="R36" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="S36" s="125"/>
+      <c r="T36" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="U36" s="125"/>
+      <c r="V36" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z36" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA36" s="137" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="M37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="O37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="R37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="S37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="T37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="U37" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A38" s="15">
+        <v>3</v>
+      </c>
+      <c r="B38" s="126">
+        <v>2</v>
+      </c>
+      <c r="C38" s="15">
+        <v>4</v>
+      </c>
+      <c r="D38" s="126">
+        <v>3</v>
+      </c>
+      <c r="E38" s="15">
+        <v>5</v>
+      </c>
+      <c r="F38" s="126">
+        <v>3</v>
+      </c>
+      <c r="G38" s="15">
+        <v>3</v>
+      </c>
+      <c r="H38" s="126">
+        <v>5</v>
+      </c>
+      <c r="I38" s="15">
+        <v>2</v>
+      </c>
+      <c r="J38" s="126">
+        <v>3</v>
+      </c>
+      <c r="K38" s="5">
+        <v>90</v>
+      </c>
+      <c r="L38" s="127">
+        <f>ROUND(A38*COS(RADIANS($K38))-B38*SIN(RADIANS($K38)), 6)</f>
+        <v>-2</v>
+      </c>
+      <c r="M38">
+        <f>ROUND(A38*SIN(RADIANS($K38))+B38*COS(RADIANS($K38)),6)</f>
+        <v>3</v>
+      </c>
+      <c r="N38" s="127">
+        <f>ROUND(C38*COS(RADIANS($K38))-D38*SIN(RADIANS($K38)), 6)</f>
+        <v>-3</v>
+      </c>
+      <c r="O38">
+        <f>ROUND(C38*SIN(RADIANS($K38))+D38*COS(RADIANS($K38)),6)</f>
+        <v>4</v>
+      </c>
+      <c r="P38" s="127">
+        <f>ROUND(E38*COS(RADIANS($K38))-F38*SIN(RADIANS($K38)), 6)</f>
+        <v>-3</v>
+      </c>
+      <c r="Q38">
+        <f>ROUND(E38*SIN(RADIANS($K38))+F38*COS(RADIANS($K38)),6)</f>
+        <v>5</v>
+      </c>
+      <c r="R38" s="127">
+        <f>ROUND(G38*COS(RADIANS($K38))-H38*SIN(RADIANS($K38)), 6)</f>
+        <v>-5</v>
+      </c>
+      <c r="S38">
+        <f>ROUND(G38*SIN(RADIANS($K38))+H38*COS(RADIANS($K38)),6)</f>
+        <v>3</v>
+      </c>
+      <c r="T38" s="127">
+        <f>ROUND(I38*COS(RADIANS($K38))-J38*SIN(RADIANS($K38)), 6)</f>
+        <v>-3</v>
+      </c>
+      <c r="U38" s="10">
+        <f>ROUND(I38*SIN(RADIANS($K38))+J38*COS(RADIANS($K38)),6)</f>
+        <v>2</v>
+      </c>
+      <c r="V38" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z38" t="str">
+        <f>"[TestCase("&amp;A38&amp;", "&amp;B38&amp;", "&amp;C38&amp;", "&amp;D38&amp;", "&amp;E38&amp;", "&amp;F38&amp;", "&amp;K38&amp;", "&amp;L38&amp;", "&amp;M38&amp;", "&amp;N38&amp;", "&amp;O38&amp;", "&amp;P38&amp;", "&amp;Q38&amp;")]    // "&amp;V38</f>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 90, -2, 3, -3, 4, -3, 5)]    // Rotate + to quadrant II</v>
+      </c>
+      <c r="AA38" t="str">
+        <f>"[TestCase("&amp;A38&amp;", "&amp;B38&amp;", "&amp;C38&amp;", "&amp;D38&amp;", "&amp;E38&amp;", "&amp;F38&amp;", "&amp;G38&amp;", "&amp;H38&amp;", "&amp;I38&amp;", "&amp;J38&amp;", "&amp;K38&amp;", "&amp;L38&amp;", "&amp;M38&amp;", "&amp;N38&amp;", "&amp;O38&amp;", "&amp;P38&amp;", "&amp;Q38&amp;", "&amp;R38&amp;", "&amp;S38&amp;", "&amp;T38&amp;", "&amp;U38&amp;")]    // "&amp;V38</f>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 3, 5, 2, 3, 90, -2, 3, -3, 4, -3, 5, -5, 3, -3, 2)]    // Rotate + to quadrant II</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A39" s="127">
+        <f>A$38</f>
+        <v>3</v>
+      </c>
+      <c r="B39" s="10">
+        <f>B$38</f>
+        <v>2</v>
+      </c>
+      <c r="C39" s="127">
+        <f>C$38</f>
+        <v>4</v>
+      </c>
+      <c r="D39" s="10">
+        <f>D$38</f>
+        <v>3</v>
+      </c>
+      <c r="E39" s="127">
+        <f>E$38</f>
+        <v>5</v>
+      </c>
+      <c r="F39" s="10">
+        <f>F$38</f>
+        <v>3</v>
+      </c>
+      <c r="G39" s="127">
+        <f>G$38</f>
+        <v>3</v>
+      </c>
+      <c r="H39" s="10">
+        <f>H$38</f>
+        <v>5</v>
+      </c>
+      <c r="I39" s="127">
+        <f>I$38</f>
+        <v>2</v>
+      </c>
+      <c r="J39" s="10">
+        <f>J$38</f>
+        <v>3</v>
+      </c>
+      <c r="K39" s="5">
+        <v>180</v>
+      </c>
+      <c r="L39" s="127">
+        <f t="shared" ref="L39:L45" si="37">ROUND(A39*COS(RADIANS($K39))-B39*SIN(RADIANS($K39)), 6)</f>
+        <v>-3</v>
+      </c>
+      <c r="M39">
+        <f t="shared" ref="M39:M45" si="38">ROUND(A39*SIN(RADIANS($K39))+B39*COS(RADIANS($K39)),6)</f>
+        <v>-2</v>
+      </c>
+      <c r="N39" s="127">
+        <f t="shared" ref="N39:N45" si="39">ROUND(C39*COS(RADIANS($K39))-D39*SIN(RADIANS($K39)), 6)</f>
+        <v>-4</v>
+      </c>
+      <c r="O39">
+        <f t="shared" ref="O39:O45" si="40">ROUND(C39*SIN(RADIANS($K39))+D39*COS(RADIANS($K39)),6)</f>
+        <v>-3</v>
+      </c>
+      <c r="P39" s="127">
+        <f t="shared" ref="P39:P45" si="41">ROUND(E39*COS(RADIANS($K39))-F39*SIN(RADIANS($K39)), 6)</f>
+        <v>-5</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" ref="Q39:Q45" si="42">ROUND(E39*SIN(RADIANS($K39))+F39*COS(RADIANS($K39)),6)</f>
+        <v>-3</v>
+      </c>
+      <c r="R39" s="127">
+        <f t="shared" ref="R39:R45" si="43">ROUND(G39*COS(RADIANS($K39))-H39*SIN(RADIANS($K39)), 6)</f>
+        <v>-3</v>
+      </c>
+      <c r="S39">
+        <f t="shared" ref="S39:S45" si="44">ROUND(G39*SIN(RADIANS($K39))+H39*COS(RADIANS($K39)),6)</f>
+        <v>-5</v>
+      </c>
+      <c r="T39" s="127">
+        <f t="shared" ref="T39:T45" si="45">ROUND(I39*COS(RADIANS($K39))-J39*SIN(RADIANS($K39)), 6)</f>
+        <v>-2</v>
+      </c>
+      <c r="U39" s="10">
+        <f t="shared" ref="U39:U45" si="46">ROUND(I39*SIN(RADIANS($K39))+J39*COS(RADIANS($K39)),6)</f>
+        <v>-3</v>
+      </c>
+      <c r="V39" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z39" t="str">
+        <f t="shared" ref="Z39:Z45" si="47">"[TestCase("&amp;A39&amp;", "&amp;B39&amp;", "&amp;C39&amp;", "&amp;D39&amp;", "&amp;E39&amp;", "&amp;F39&amp;", "&amp;K39&amp;", "&amp;L39&amp;", "&amp;M39&amp;", "&amp;N39&amp;", "&amp;O39&amp;", "&amp;P39&amp;", "&amp;Q39&amp;")]    // "&amp;V39</f>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 180, -3, -2, -4, -3, -5, -3)]    // Rotate + to quadrant III</v>
+      </c>
+      <c r="AA39" t="str">
+        <f t="shared" ref="AA39:AA45" si="48">"[TestCase("&amp;A39&amp;", "&amp;B39&amp;", "&amp;C39&amp;", "&amp;D39&amp;", "&amp;E39&amp;", "&amp;F39&amp;", "&amp;G39&amp;", "&amp;H39&amp;", "&amp;I39&amp;", "&amp;J39&amp;", "&amp;K39&amp;", "&amp;L39&amp;", "&amp;M39&amp;", "&amp;N39&amp;", "&amp;O39&amp;", "&amp;P39&amp;", "&amp;Q39&amp;", "&amp;R39&amp;", "&amp;S39&amp;", "&amp;T39&amp;", "&amp;U39&amp;")]    // "&amp;V39</f>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 3, 5, 2, 3, 180, -3, -2, -4, -3, -5, -3, -3, -5, -2, -3)]    // Rotate + to quadrant III</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A40" s="127">
+        <f>A$38</f>
+        <v>3</v>
+      </c>
+      <c r="B40" s="10">
+        <f>B$38</f>
+        <v>2</v>
+      </c>
+      <c r="C40" s="127">
+        <f>C$38</f>
+        <v>4</v>
+      </c>
+      <c r="D40" s="10">
+        <f>D$38</f>
+        <v>3</v>
+      </c>
+      <c r="E40" s="127">
+        <f>E$38</f>
+        <v>5</v>
+      </c>
+      <c r="F40" s="10">
+        <f>F$38</f>
+        <v>3</v>
+      </c>
+      <c r="G40" s="127">
+        <f>G$38</f>
+        <v>3</v>
+      </c>
+      <c r="H40" s="10">
+        <f>H$38</f>
+        <v>5</v>
+      </c>
+      <c r="I40" s="127">
+        <f>I$38</f>
+        <v>2</v>
+      </c>
+      <c r="J40" s="10">
+        <f>J$38</f>
+        <v>3</v>
+      </c>
+      <c r="K40" s="5">
+        <v>270</v>
+      </c>
+      <c r="L40" s="127">
+        <f t="shared" si="37"/>
+        <v>2</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="38"/>
+        <v>-3</v>
+      </c>
+      <c r="N40" s="127">
+        <f t="shared" si="39"/>
+        <v>3</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="40"/>
+        <v>-4</v>
+      </c>
+      <c r="P40" s="127">
+        <f t="shared" si="41"/>
+        <v>3</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="42"/>
+        <v>-5</v>
+      </c>
+      <c r="R40" s="127">
+        <f t="shared" si="43"/>
+        <v>5</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="44"/>
+        <v>-3</v>
+      </c>
+      <c r="T40" s="127">
+        <f t="shared" si="45"/>
+        <v>3</v>
+      </c>
+      <c r="U40" s="10">
+        <f t="shared" si="46"/>
+        <v>-2</v>
+      </c>
+      <c r="V40" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z40" t="str">
+        <f t="shared" si="47"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 270, 2, -3, 3, -4, 3, -5)]    // Rotate + to quadrant IV</v>
+      </c>
+      <c r="AA40" t="str">
+        <f t="shared" si="48"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 3, 5, 2, 3, 270, 2, -3, 3, -4, 3, -5, 5, -3, 3, -2)]    // Rotate + to quadrant IV</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A41" s="127">
+        <f>A$38</f>
+        <v>3</v>
+      </c>
+      <c r="B41" s="10">
+        <f>B$38</f>
+        <v>2</v>
+      </c>
+      <c r="C41" s="127">
+        <f>C$38</f>
+        <v>4</v>
+      </c>
+      <c r="D41" s="10">
+        <f>D$38</f>
+        <v>3</v>
+      </c>
+      <c r="E41" s="127">
+        <f>E$38</f>
+        <v>5</v>
+      </c>
+      <c r="F41" s="10">
+        <f>F$38</f>
+        <v>3</v>
+      </c>
+      <c r="G41" s="127">
+        <f>G$38</f>
+        <v>3</v>
+      </c>
+      <c r="H41" s="10">
+        <f>H$38</f>
+        <v>5</v>
+      </c>
+      <c r="I41" s="127">
+        <f>I$38</f>
+        <v>2</v>
+      </c>
+      <c r="J41" s="10">
+        <f>J$38</f>
+        <v>3</v>
+      </c>
+      <c r="K41" s="5">
+        <v>360</v>
+      </c>
+      <c r="L41" s="127">
+        <f t="shared" si="37"/>
+        <v>3</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="38"/>
+        <v>2</v>
+      </c>
+      <c r="N41" s="127">
+        <f t="shared" si="39"/>
+        <v>4</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="40"/>
+        <v>3</v>
+      </c>
+      <c r="P41" s="127">
+        <f t="shared" si="41"/>
+        <v>5</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="42"/>
+        <v>3</v>
+      </c>
+      <c r="R41" s="127">
+        <f t="shared" si="43"/>
+        <v>3</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="44"/>
+        <v>5</v>
+      </c>
+      <c r="T41" s="127">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="U41" s="10">
+        <f t="shared" si="46"/>
+        <v>3</v>
+      </c>
+      <c r="V41" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z41" t="str">
+        <f t="shared" si="47"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 360, 3, 2, 4, 3, 5, 3)]    // Rotate + full circle</v>
+      </c>
+      <c r="AA41" t="str">
+        <f t="shared" si="48"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 3, 5, 2, 3, 360, 3, 2, 4, 3, 5, 3, 3, 5, 2, 3)]    // Rotate + full circle</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A42" s="127">
+        <f>A$38</f>
+        <v>3</v>
+      </c>
+      <c r="B42" s="10">
+        <f>B$38</f>
+        <v>2</v>
+      </c>
+      <c r="C42" s="127">
+        <f>C$38</f>
+        <v>4</v>
+      </c>
+      <c r="D42" s="10">
+        <f>D$38</f>
+        <v>3</v>
+      </c>
+      <c r="E42" s="127">
+        <f>E$38</f>
+        <v>5</v>
+      </c>
+      <c r="F42" s="10">
+        <f>F$38</f>
+        <v>3</v>
+      </c>
+      <c r="G42" s="127">
+        <f>G$38</f>
+        <v>3</v>
+      </c>
+      <c r="H42" s="10">
+        <f>H$38</f>
+        <v>5</v>
+      </c>
+      <c r="I42" s="127">
+        <f>I$38</f>
+        <v>2</v>
+      </c>
+      <c r="J42" s="10">
+        <f>J$38</f>
+        <v>3</v>
+      </c>
+      <c r="K42" s="5">
+        <v>-90</v>
+      </c>
+      <c r="L42" s="127">
+        <f t="shared" si="37"/>
+        <v>2</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="38"/>
+        <v>-3</v>
+      </c>
+      <c r="N42" s="127">
+        <f t="shared" si="39"/>
+        <v>3</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="40"/>
+        <v>-4</v>
+      </c>
+      <c r="P42" s="127">
+        <f t="shared" si="41"/>
+        <v>3</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="42"/>
+        <v>-5</v>
+      </c>
+      <c r="R42" s="127">
+        <f t="shared" si="43"/>
+        <v>5</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="44"/>
+        <v>-3</v>
+      </c>
+      <c r="T42" s="127">
+        <f t="shared" si="45"/>
+        <v>3</v>
+      </c>
+      <c r="U42" s="10">
+        <f t="shared" si="46"/>
+        <v>-2</v>
+      </c>
+      <c r="V42" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z42" t="str">
+        <f t="shared" si="47"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, -90, 2, -3, 3, -4, 3, -5)]    // Rotate - to quadrant II</v>
+      </c>
+      <c r="AA42" t="str">
+        <f t="shared" si="48"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 3, 5, 2, 3, -90, 2, -3, 3, -4, 3, -5, 5, -3, 3, -2)]    // Rotate - to quadrant II</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A43" s="127">
+        <f>A$38</f>
+        <v>3</v>
+      </c>
+      <c r="B43" s="10">
+        <f>B$38</f>
+        <v>2</v>
+      </c>
+      <c r="C43" s="127">
+        <f>C$38</f>
+        <v>4</v>
+      </c>
+      <c r="D43" s="10">
+        <f>D$38</f>
+        <v>3</v>
+      </c>
+      <c r="E43" s="127">
+        <f>E$38</f>
+        <v>5</v>
+      </c>
+      <c r="F43" s="10">
+        <f>F$38</f>
+        <v>3</v>
+      </c>
+      <c r="G43" s="127">
+        <f>G$38</f>
+        <v>3</v>
+      </c>
+      <c r="H43" s="10">
+        <f>H$38</f>
+        <v>5</v>
+      </c>
+      <c r="I43" s="127">
+        <f>I$38</f>
+        <v>2</v>
+      </c>
+      <c r="J43" s="10">
+        <f>J$38</f>
+        <v>3</v>
+      </c>
+      <c r="K43" s="5">
+        <v>-180</v>
+      </c>
+      <c r="L43" s="127">
+        <f t="shared" si="37"/>
+        <v>-3</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="38"/>
+        <v>-2</v>
+      </c>
+      <c r="N43" s="127">
+        <f t="shared" si="39"/>
+        <v>-4</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="40"/>
+        <v>-3</v>
+      </c>
+      <c r="P43" s="127">
+        <f t="shared" si="41"/>
+        <v>-5</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="42"/>
+        <v>-3</v>
+      </c>
+      <c r="R43" s="127">
+        <f t="shared" si="43"/>
+        <v>-3</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="44"/>
+        <v>-5</v>
+      </c>
+      <c r="T43" s="127">
+        <f t="shared" si="45"/>
+        <v>-2</v>
+      </c>
+      <c r="U43" s="10">
+        <f t="shared" si="46"/>
+        <v>-3</v>
+      </c>
+      <c r="V43" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z43" t="str">
+        <f t="shared" si="47"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, -180, -3, -2, -4, -3, -5, -3)]    // Rotate - to quadrant III</v>
+      </c>
+      <c r="AA43" t="str">
+        <f t="shared" si="48"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 3, 5, 2, 3, -180, -3, -2, -4, -3, -5, -3, -3, -5, -2, -3)]    // Rotate - to quadrant III</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A44" s="127">
+        <f>A$38</f>
+        <v>3</v>
+      </c>
+      <c r="B44" s="10">
+        <f>B$38</f>
+        <v>2</v>
+      </c>
+      <c r="C44" s="127">
+        <f>C$38</f>
+        <v>4</v>
+      </c>
+      <c r="D44" s="10">
+        <f>D$38</f>
+        <v>3</v>
+      </c>
+      <c r="E44" s="127">
+        <f>E$38</f>
+        <v>5</v>
+      </c>
+      <c r="F44" s="10">
+        <f>F$38</f>
+        <v>3</v>
+      </c>
+      <c r="G44" s="127">
+        <f>G$38</f>
+        <v>3</v>
+      </c>
+      <c r="H44" s="10">
+        <f>H$38</f>
+        <v>5</v>
+      </c>
+      <c r="I44" s="127">
+        <f>I$38</f>
+        <v>2</v>
+      </c>
+      <c r="J44" s="10">
+        <f>J$38</f>
+        <v>3</v>
+      </c>
+      <c r="K44" s="5">
+        <v>-270</v>
+      </c>
+      <c r="L44" s="127">
+        <f t="shared" si="37"/>
+        <v>-2</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="38"/>
+        <v>3</v>
+      </c>
+      <c r="N44" s="127">
+        <f t="shared" si="39"/>
+        <v>-3</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="40"/>
+        <v>4</v>
+      </c>
+      <c r="P44" s="127">
+        <f t="shared" si="41"/>
+        <v>-3</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="42"/>
+        <v>5</v>
+      </c>
+      <c r="R44" s="127">
+        <f t="shared" si="43"/>
+        <v>-5</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="44"/>
+        <v>3</v>
+      </c>
+      <c r="T44" s="127">
+        <f t="shared" si="45"/>
+        <v>-3</v>
+      </c>
+      <c r="U44" s="10">
+        <f t="shared" si="46"/>
+        <v>2</v>
+      </c>
+      <c r="V44" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z44" t="str">
+        <f t="shared" si="47"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, -270, -2, 3, -3, 4, -3, 5)]    // Rotate - to quadrant IV</v>
+      </c>
+      <c r="AA44" t="str">
+        <f t="shared" si="48"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 3, 5, 2, 3, -270, -2, 3, -3, 4, -3, 5, -5, 3, -3, 2)]    // Rotate - to quadrant IV</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A45" s="127">
+        <f>A$38</f>
+        <v>3</v>
+      </c>
+      <c r="B45" s="10">
+        <f>B$38</f>
+        <v>2</v>
+      </c>
+      <c r="C45" s="127">
+        <f>C$38</f>
+        <v>4</v>
+      </c>
+      <c r="D45" s="10">
+        <f>D$38</f>
+        <v>3</v>
+      </c>
+      <c r="E45" s="127">
+        <f>E$38</f>
+        <v>5</v>
+      </c>
+      <c r="F45" s="10">
+        <f>F$38</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="127">
+        <f>G$38</f>
+        <v>3</v>
+      </c>
+      <c r="H45" s="10">
+        <f>H$38</f>
+        <v>5</v>
+      </c>
+      <c r="I45" s="127">
+        <f>I$38</f>
+        <v>2</v>
+      </c>
+      <c r="J45" s="10">
+        <f>J$38</f>
+        <v>3</v>
+      </c>
+      <c r="K45" s="5">
+        <v>-360</v>
+      </c>
+      <c r="L45" s="127">
+        <f t="shared" si="37"/>
+        <v>3</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="38"/>
+        <v>2</v>
+      </c>
+      <c r="N45" s="127">
+        <f t="shared" si="39"/>
+        <v>4</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="40"/>
+        <v>3</v>
+      </c>
+      <c r="P45" s="127">
+        <f t="shared" si="41"/>
+        <v>5</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="42"/>
+        <v>3</v>
+      </c>
+      <c r="R45" s="127">
+        <f t="shared" si="43"/>
+        <v>3</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="44"/>
+        <v>5</v>
+      </c>
+      <c r="T45" s="127">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="U45" s="10">
+        <f t="shared" si="46"/>
+        <v>3</v>
+      </c>
+      <c r="V45" t="s">
+        <v>207</v>
+      </c>
+      <c r="Z45" t="str">
+        <f t="shared" si="47"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, -360, 3, 2, 4, 3, 5, 3)]    // Rotate - full circle</v>
+      </c>
+      <c r="AA45" t="str">
+        <f t="shared" si="48"/>
+        <v>[TestCase(3, 2, 4, 3, 5, 3, 3, 5, 2, 3, -360, 3, 2, 4, 3, 5, 3, 3, 5, 2, 3)]    // Rotate - full circle</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" s="125"/>
+      <c r="C48" s="124" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="125"/>
+      <c r="E48" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="F48" s="125"/>
+      <c r="G48" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="H48" s="125"/>
+      <c r="I48" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="J48" s="125"/>
+      <c r="K48" s="124" t="s">
+        <v>190</v>
+      </c>
+      <c r="L48" s="132"/>
+      <c r="M48" s="122" t="s">
+        <v>191</v>
+      </c>
+      <c r="N48" s="116"/>
+      <c r="O48" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="P48" s="125"/>
+      <c r="Q48" s="124" t="s">
+        <v>168</v>
+      </c>
+      <c r="R48" s="125"/>
+      <c r="S48" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="T48" s="125"/>
+      <c r="U48" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="V48" s="125"/>
+      <c r="W48" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="X48" s="125"/>
+      <c r="Y48" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z48" s="136" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA48" s="136" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L49" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="P49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="R49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="S49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="T49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="U49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="V49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="W49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="X49" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A50" s="15">
+        <v>3</v>
+      </c>
+      <c r="B50" s="126">
+        <v>2</v>
+      </c>
+      <c r="C50" s="15">
+        <v>4</v>
+      </c>
+      <c r="D50" s="126">
+        <v>3</v>
+      </c>
+      <c r="E50" s="15">
+        <v>5</v>
+      </c>
+      <c r="F50" s="126">
+        <v>3</v>
+      </c>
+      <c r="G50" s="15">
+        <v>3</v>
+      </c>
+      <c r="H50" s="126">
+        <v>5</v>
+      </c>
+      <c r="I50" s="15">
+        <v>2</v>
+      </c>
+      <c r="J50" s="126">
+        <v>3</v>
+      </c>
+      <c r="K50" s="15">
+        <v>0</v>
+      </c>
+      <c r="L50" s="133">
+        <v>1</v>
+      </c>
+      <c r="M50" s="5">
+        <v>0</v>
+      </c>
+      <c r="N50" s="5">
+        <v>-1</v>
+      </c>
+      <c r="O50" s="134"/>
+      <c r="P50" s="135"/>
+      <c r="Q50" s="134"/>
+      <c r="R50" s="135"/>
+      <c r="S50" s="134"/>
+      <c r="T50" s="135"/>
+      <c r="U50" s="134"/>
+      <c r="V50" s="135"/>
+      <c r="W50" s="134"/>
+      <c r="X50" s="135"/>
+      <c r="Y50" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z50" t="str">
+        <f>"[TestCase("&amp;A50&amp;", "&amp;B50&amp;", "&amp;C50&amp;", "&amp;D50&amp;", "&amp;K50&amp;", "&amp;L50&amp;", "&amp;M50&amp;", "&amp;N50&amp;", "&amp;O50&amp;", "&amp;P50&amp;", "&amp;Q50&amp;", "&amp;R5050&amp;")]    // "&amp;Y50</f>
+        <v>[TestCase(3, 2, 4, 3, 0, 1, 0, -1, , , , )]    // Mirror about y-axis to Quadrant II</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A51" s="127">
+        <f>A$50</f>
+        <v>3</v>
+      </c>
+      <c r="B51" s="10">
+        <f t="shared" ref="B51:J51" si="49">B$50</f>
+        <v>2</v>
+      </c>
+      <c r="C51" s="127">
+        <f t="shared" si="49"/>
+        <v>4</v>
+      </c>
+      <c r="D51" s="10">
+        <f t="shared" si="49"/>
+        <v>3</v>
+      </c>
+      <c r="E51" s="127">
+        <f t="shared" si="49"/>
+        <v>5</v>
+      </c>
+      <c r="F51" s="10">
+        <f t="shared" si="49"/>
+        <v>3</v>
+      </c>
+      <c r="G51" s="127">
+        <f t="shared" si="49"/>
+        <v>3</v>
+      </c>
+      <c r="H51" s="10">
+        <f t="shared" si="49"/>
+        <v>5</v>
+      </c>
+      <c r="I51" s="127">
+        <f t="shared" si="49"/>
+        <v>2</v>
+      </c>
+      <c r="J51" s="10">
+        <f t="shared" si="49"/>
+        <v>3</v>
+      </c>
+      <c r="K51" s="15">
+        <v>0</v>
+      </c>
+      <c r="L51" s="133">
+        <v>-1</v>
+      </c>
+      <c r="M51" s="5">
+        <v>0</v>
+      </c>
+      <c r="N51" s="5">
+        <v>1</v>
+      </c>
+      <c r="O51" s="134"/>
+      <c r="P51" s="135"/>
+      <c r="Q51" s="134"/>
+      <c r="R51" s="135"/>
+      <c r="S51" s="134"/>
+      <c r="T51" s="135"/>
+      <c r="U51" s="134"/>
+      <c r="V51" s="135"/>
+      <c r="W51" s="134"/>
+      <c r="X51" s="135"/>
+      <c r="Y51" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z51" t="str">
+        <f t="shared" ref="Z51:Z57" si="50">"[TestCase("&amp;A51&amp;", "&amp;B51&amp;", "&amp;C51&amp;", "&amp;D51&amp;", "&amp;K51&amp;", "&amp;L51&amp;", "&amp;M51&amp;", "&amp;N51&amp;", "&amp;O51&amp;", "&amp;P51&amp;", "&amp;Q51&amp;", "&amp;R5051&amp;")]    // "&amp;Y51</f>
+        <v>[TestCase(3, 2, 4, 3, 0, -1, 0, 1, , , , )]    // Mirror about y-axis to Quadrant II, reversed line</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A52" s="127">
+        <f t="shared" ref="A52:J57" si="51">A$50</f>
+        <v>3</v>
+      </c>
+      <c r="B52" s="10">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="C52" s="127">
+        <f t="shared" si="51"/>
+        <v>4</v>
+      </c>
+      <c r="D52" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="E52" s="127">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="F52" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="G52" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="H52" s="10">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="I52" s="127">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="J52" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="K52" s="15">
+        <v>1</v>
+      </c>
+      <c r="L52" s="133">
+        <v>0</v>
+      </c>
+      <c r="M52" s="5">
+        <v>-1</v>
+      </c>
+      <c r="N52" s="5">
+        <v>0</v>
+      </c>
+      <c r="O52" s="134"/>
+      <c r="P52" s="135"/>
+      <c r="Q52" s="134"/>
+      <c r="R52" s="135"/>
+      <c r="S52" s="134"/>
+      <c r="T52" s="135"/>
+      <c r="U52" s="134"/>
+      <c r="V52" s="135"/>
+      <c r="W52" s="134"/>
+      <c r="X52" s="135"/>
+      <c r="Y52" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z52" t="str">
+        <f t="shared" si="50"/>
+        <v>[TestCase(3, 2, 4, 3, 1, 0, -1, 0, , , , )]    // Mirror about x-axis to Quadrant IV</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A53" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="B53" s="10">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="C53" s="127">
+        <f t="shared" si="51"/>
+        <v>4</v>
+      </c>
+      <c r="D53" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="E53" s="127">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="F53" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="G53" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="H53" s="10">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="I53" s="127">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="J53" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="K53" s="15">
+        <v>-1</v>
+      </c>
+      <c r="L53" s="133">
+        <v>0</v>
+      </c>
+      <c r="M53" s="5">
+        <v>1</v>
+      </c>
+      <c r="N53" s="5">
+        <v>0</v>
+      </c>
+      <c r="O53" s="134"/>
+      <c r="P53" s="135"/>
+      <c r="Q53" s="134"/>
+      <c r="R53" s="135"/>
+      <c r="S53" s="134"/>
+      <c r="T53" s="135"/>
+      <c r="U53" s="134"/>
+      <c r="V53" s="135"/>
+      <c r="W53" s="134"/>
+      <c r="X53" s="135"/>
+      <c r="Y53" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z53" t="str">
+        <f t="shared" si="50"/>
+        <v>[TestCase(3, 2, 4, 3, -1, 0, 1, 0, , , , )]    // Mirror about x-axis to Quadrant IV, reversed line</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A54" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="B54" s="10">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="C54" s="127">
+        <f t="shared" si="51"/>
+        <v>4</v>
+      </c>
+      <c r="D54" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="E54" s="127">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="F54" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="H54" s="10">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="I54" s="127">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="J54" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="K54" s="15">
+        <v>0</v>
+      </c>
+      <c r="L54" s="133">
+        <v>0</v>
+      </c>
+      <c r="M54" s="5">
+        <v>1</v>
+      </c>
+      <c r="N54" s="5">
+        <v>1</v>
+      </c>
+      <c r="O54" s="134"/>
+      <c r="P54" s="135"/>
+      <c r="Q54" s="134"/>
+      <c r="R54" s="135"/>
+      <c r="S54" s="134"/>
+      <c r="T54" s="135"/>
+      <c r="U54" s="134"/>
+      <c r="V54" s="135"/>
+      <c r="W54" s="134"/>
+      <c r="X54" s="135"/>
+      <c r="Y54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z54" t="str">
+        <f t="shared" si="50"/>
+        <v>[TestCase(3, 2, 4, 3, 0, 0, 1, 1, , , , )]    // Mirror about 45 deg sloped line about shape center</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A55" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="B55" s="10">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="C55" s="127">
+        <f t="shared" si="51"/>
+        <v>4</v>
+      </c>
+      <c r="D55" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="E55" s="127">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="F55" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="G55" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="H55" s="10">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="I55" s="127">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="J55" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="K55" s="15">
+        <v>0</v>
+      </c>
+      <c r="L55" s="133">
+        <v>0</v>
+      </c>
+      <c r="M55" s="5">
+        <v>-1</v>
+      </c>
+      <c r="N55" s="5">
+        <v>-1</v>
+      </c>
+      <c r="O55" s="134"/>
+      <c r="P55" s="135"/>
+      <c r="Q55" s="134"/>
+      <c r="R55" s="135"/>
+      <c r="S55" s="134"/>
+      <c r="T55" s="135"/>
+      <c r="U55" s="134"/>
+      <c r="V55" s="135"/>
+      <c r="W55" s="134"/>
+      <c r="X55" s="135"/>
+      <c r="Y55" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z55" t="str">
+        <f t="shared" si="50"/>
+        <v>[TestCase(3, 2, 4, 3, 0, 0, -1, -1, , , , )]    // Mirror about 45 deg sloped line about shape center, reversed line</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A56" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="B56" s="10">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="C56" s="127">
+        <f t="shared" si="51"/>
+        <v>4</v>
+      </c>
+      <c r="D56" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="E56" s="127">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="F56" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="G56" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="H56" s="10">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="I56" s="127">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="J56" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="K56" s="15">
+        <v>0</v>
+      </c>
+      <c r="L56" s="133">
+        <v>0</v>
+      </c>
+      <c r="M56" s="5">
+        <v>-1</v>
+      </c>
+      <c r="N56" s="5">
+        <v>1</v>
+      </c>
+      <c r="O56" s="134"/>
+      <c r="P56" s="135"/>
+      <c r="Q56" s="134"/>
+      <c r="R56" s="135"/>
+      <c r="S56" s="134"/>
+      <c r="T56" s="135"/>
+      <c r="U56" s="134"/>
+      <c r="V56" s="135"/>
+      <c r="W56" s="134"/>
+      <c r="X56" s="135"/>
+      <c r="Y56" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z56" t="str">
+        <f t="shared" si="50"/>
+        <v>[TestCase(3, 2, 4, 3, 0, 0, -1, 1, , , , )]    // Mirror about 45 deg sloped line to quadrant III</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A57" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="B57" s="10">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="C57" s="127">
+        <f t="shared" si="51"/>
+        <v>4</v>
+      </c>
+      <c r="D57" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="E57" s="127">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="F57" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="G57" s="127">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="H57" s="10">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="I57" s="127">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="J57" s="10">
+        <f t="shared" si="51"/>
+        <v>3</v>
+      </c>
+      <c r="K57" s="15">
+        <v>0</v>
+      </c>
+      <c r="L57" s="133">
+        <v>0</v>
+      </c>
+      <c r="M57" s="5">
+        <v>1</v>
+      </c>
+      <c r="N57" s="5">
+        <v>-1</v>
+      </c>
+      <c r="O57" s="134"/>
+      <c r="P57" s="135"/>
+      <c r="Q57" s="134"/>
+      <c r="R57" s="135"/>
+      <c r="S57" s="134"/>
+      <c r="T57" s="135"/>
+      <c r="U57" s="134"/>
+      <c r="V57" s="135"/>
+      <c r="W57" s="134"/>
+      <c r="X57" s="135"/>
+      <c r="Y57" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z57" t="str">
+        <f t="shared" si="50"/>
+        <v>[TestCase(3, 2, 4, 3, 0, 0, 1, -1, , , , )]    // Mirror about 45 deg sloped line to quadrant III, reversed line</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="46">
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="U48:V48"/>
+    <mergeCell ref="W48:X48"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBF033D-0D4B-47C9-BEC2-54C9B12F8A53}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>